<commit_message>
Final fixes to run through Staging
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742CCF0A-7CB5-45E5-84A8-552F59FA1260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F9C12C-3F6B-453F-BF9B-A48CC540A415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26850" yWindow="16050" windowWidth="13095" windowHeight="15465" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
+    <workbookView xWindow="-26850" yWindow="16050" windowWidth="18240" windowHeight="15465" activeTab="1" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
   <sheets>
-    <sheet name="Performance" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance_SNOW" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance_CHPC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>readindividuals</t>
   </si>
@@ -49,16 +50,49 @@
   </si>
   <si>
     <t>readhouseholdmemberships</t>
+  </si>
+  <si>
+    <t>Agincourt</t>
+  </si>
+  <si>
+    <t>DIMAMO</t>
+  </si>
+  <si>
+    <t>AHRI</t>
+  </si>
+  <si>
+    <t>readindividualmemberships</t>
+  </si>
+  <si>
+    <t>readeducationstatuses</t>
+  </si>
+  <si>
+    <t>readhouseholdsocioeconomic</t>
+  </si>
+  <si>
+    <t>readmaritalstatuses</t>
+  </si>
+  <si>
+    <t>readlabourstatuses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -84,15 +118,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -419,7 +456,7 @@
     <col min="7" max="7" width="8.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -433,8 +470,12 @@
         <f>C2-B2</f>
         <v>2.0254629635019228E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="2">
+        <f>SUM(F2:H2)</f>
+        <v>2.0254629635019228E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -448,8 +489,12 @@
         <f>C3-B3</f>
         <v>4.6296292566694319E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I11" si="0">SUM(F3:H3)</f>
+        <v>4.6296292566694319E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -477,8 +522,12 @@
         <f>E4-D4</f>
         <v>9.2592592409346253E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8599537035916001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -492,8 +541,12 @@
         <f>C5-B5</f>
         <v>1.7361111531499773E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7361111531499773E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -506,6 +559,360 @@
       <c r="F6" s="2">
         <f>C6-B6</f>
         <v>2.546296309446916E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.546296309446916E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44207.520138888889</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44207.540219907409</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44207.544895833336</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44207.572766203702</v>
+      </c>
+      <c r="F7" s="2">
+        <f>C7-B7</f>
+        <v>2.008101851970423E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" ref="G7:H7" si="1">D7-C7</f>
+        <v>4.6759259275859222E-3</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7870370366144925E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2627314813435078E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44207.602777777778</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44207.603495370371</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44207.603541666664</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44207.603877314818</v>
+      </c>
+      <c r="F8" s="2">
+        <f>C8-B8</f>
+        <v>7.1759259299142286E-4</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8" si="2">D8-C8</f>
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8" si="3">E8-D8</f>
+        <v>3.3564815385034308E-4</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0995370394084603E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44207.603877314818</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44207.604085648149</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44207.604097222225</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44207.604143518518</v>
+      </c>
+      <c r="F9" s="2">
+        <f>C9-B9</f>
+        <v>2.0833333110203966E-4</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" ref="G9" si="4">D9-C9</f>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9" si="5">E9-D9</f>
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6620370044838637E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44207.604143518518</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44207.604259259257</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44207.604270833333</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44207.604444444441</v>
+      </c>
+      <c r="F10" s="2">
+        <f>C10-B10</f>
+        <v>1.1574073869269341E-4</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" ref="G10:G11" si="6">D10-C10</f>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" ref="H10:H11" si="7">E10-D10</f>
+        <v>1.7361110803904012E-4</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>3.0092592351138592E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44207.604444444441</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44207.604618055557</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44207.604675925926</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44207.605150462965</v>
+      </c>
+      <c r="F11" s="2">
+        <f>C11-B11</f>
+        <v>1.7361111531499773E-4</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="6"/>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="7"/>
+        <v>4.7453703882638365E-4</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>7.0601852348772809E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="2">
+        <f>SUM(I2:I11)</f>
+        <v>8.6099537038535345E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751965E-4A3A-442F-9C21-79FCCBFBF505}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" customWidth="1"/>
+    <col min="5" max="6" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44207.434687499997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44207.435486111113</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="G2" s="2">
+        <f>C2-B2</f>
+        <v>7.9861111589707434E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44207.435486111113</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44207.435543981483</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="G3" s="2">
+        <f>C3-B3</f>
+        <v>5.7870369346346706E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44207.435543981483</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44207.453425925924</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44207.466666666667</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44207.471053240741</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44207.471215277779</v>
+      </c>
+      <c r="G4" s="2">
+        <f>C4-B4</f>
+        <v>1.788194444088731E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <f>D4-C4</f>
+        <v>1.3240740743640345E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <f>F4-E4</f>
+        <v>1.6203703853534535E-4</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44207.471215277779</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44207.471597222226</v>
+      </c>
+      <c r="G5" s="2">
+        <f>C5-B5</f>
+        <v>3.819444464170374E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44207.471597222226</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44207.472071759257</v>
+      </c>
+      <c r="G6" s="2">
+        <f>C6-B6</f>
+        <v>4.7453703155042604E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44207.472071759257</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44207.512962962966</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44207.52207175926</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44207.57366898148</v>
+      </c>
+      <c r="G7" s="2">
+        <f>C7-B7</f>
+        <v>4.0891203709179536E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:I7" si="0">D7-C7</f>
+        <v>9.1087962937308475E-3</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>5.1597222220152617E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developing consolidate preferred households
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A98EA5E-86B5-42E6-B79C-8C33E73722AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57C1415-F448-4906-9F20-D301F9159D1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4760" windowWidth="19700" windowHeight="11120" activeTab="2" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
+    <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_SNOW" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>readindividuals</t>
   </si>
@@ -172,19 +172,23 @@
   </si>
   <si>
     <t>Household membership day extraction</t>
+  </si>
+  <si>
+    <t>consolidatepreferredhousehold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss;@"/>
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="dd\ hh:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -224,7 +228,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -239,6 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -555,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -585,18 +590,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44207.333333333336</v>
+        <v>44213.747048611112</v>
       </c>
       <c r="C2" s="1">
-        <v>44207.335358796299</v>
+        <v>44213.747488425928</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" ref="F2:F11" si="0">C2-B2</f>
-        <v>2.0254629635019228E-3</v>
+        <v>4.398148157633841E-4</v>
       </c>
       <c r="I2" s="2">
         <f>SUM(F2:H2)</f>
-        <v>2.0254629635019228E-3</v>
+        <v>4.398148157633841E-4</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -604,18 +609,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>44207.335358796299</v>
+        <v>44213.747488425928</v>
       </c>
       <c r="C3" s="1">
-        <v>44207.335405092592</v>
+        <v>44213.747523148151</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" si="0"/>
-        <v>4.6296292566694319E-5</v>
+        <v>3.4722223062999547E-5</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ref="I3:I11" si="1">SUM(F3:H3)</f>
-        <v>4.6296292566694319E-5</v>
+        <v>3.4722223062999547E-5</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -623,32 +628,32 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>44207.335405092592</v>
+        <v>44213.747523148151</v>
       </c>
       <c r="C4" s="1">
-        <v>44207.361539351848</v>
+        <v>44213.752395833333</v>
       </c>
       <c r="D4" s="1">
-        <v>44207.363912037035</v>
+        <v>44213.753182870372</v>
       </c>
       <c r="E4" s="1">
-        <v>44207.364004629628</v>
+        <v>44213.753449074073</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>2.6134259256650694E-2</v>
+        <v>4.8726851819083095E-3</v>
       </c>
       <c r="G4" s="2">
         <f>D4-C4</f>
-        <v>2.3726851868559606E-3</v>
+        <v>7.8703703911742195E-4</v>
       </c>
       <c r="H4" s="2">
         <f>E4-D4</f>
-        <v>9.2592592409346253E-5</v>
+        <v>2.6620370044838637E-4</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="1"/>
-        <v>2.8599537035916001E-2</v>
+        <v>5.9259259214741178E-3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -656,18 +661,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>44207.364004629628</v>
+        <v>44213.753449074073</v>
       </c>
       <c r="C5" s="1">
-        <v>44207.364178240743</v>
+        <v>44213.753645833334</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>1.7361111531499773E-4</v>
+        <v>1.9675926159834489E-4</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="1"/>
-        <v>1.7361111531499773E-4</v>
+        <v>1.9675926159834489E-4</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -675,18 +680,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>44207.364178240743</v>
+        <v>44213.753645833334</v>
       </c>
       <c r="C6" s="1">
-        <v>44207.364432870374</v>
+        <v>44213.753912037035</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>2.546296309446916E-4</v>
+        <v>2.6620370044838637E-4</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>2.546296309446916E-4</v>
+        <v>2.6620370044838637E-4</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -694,32 +699,32 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>44207.520138888889</v>
+        <v>44213.753912037035</v>
       </c>
       <c r="C7" s="1">
-        <v>44207.540219907409</v>
+        <v>44213.775034722225</v>
       </c>
       <c r="D7" s="1">
-        <v>44207.544895833336</v>
+        <v>44213.780173611114</v>
       </c>
       <c r="E7" s="1">
-        <v>44207.572766203702</v>
+        <v>44213.803611111114</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>2.008101851970423E-2</v>
+        <v>2.1122685189766344E-2</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" ref="G7:H7" si="2">D7-C7</f>
-        <v>4.6759259275859222E-3</v>
+        <v>5.1388888896326534E-3</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>2.7870370366144925E-2</v>
+        <v>2.34375E-2</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="1"/>
-        <v>5.2627314813435078E-2</v>
+        <v>4.9699074079398997E-2</v>
       </c>
       <c r="K7">
         <v>411</v>
@@ -738,32 +743,32 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>44207.602777777778</v>
+        <v>44213.803611111114</v>
       </c>
       <c r="C8" s="1">
-        <v>44207.603495370371</v>
+        <v>44213.803738425922</v>
       </c>
       <c r="D8" s="1">
-        <v>44207.603541666664</v>
+        <v>44213.803773148145</v>
       </c>
       <c r="E8" s="1">
-        <v>44207.603877314818</v>
+        <v>44213.804085648146</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>7.1759259299142286E-4</v>
+        <v>1.2731480819638819E-4</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" ref="G8" si="3">D8-C8</f>
-        <v>4.6296292566694319E-5</v>
+        <v>3.4722223062999547E-5</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ref="H8" si="4">E8-D8</f>
-        <v>3.3564815385034308E-4</v>
+        <v>3.125000002910383E-4</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>1.0995370394084603E-3</v>
+        <v>4.7453703155042604E-4</v>
       </c>
       <c r="K8">
         <v>427</v>
@@ -782,32 +787,32 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>44207.603877314818</v>
+        <v>44213.804085648146</v>
       </c>
       <c r="C9" s="1">
-        <v>44207.604085648149</v>
+        <v>44213.804328703707</v>
       </c>
       <c r="D9" s="1">
-        <v>44207.604097222225</v>
+        <v>44213.804340277777</v>
       </c>
       <c r="E9" s="1">
-        <v>44207.604143518518</v>
+        <v>44213.804386574076</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>2.0833333110203966E-4</v>
+        <v>2.4305556144099683E-4</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" ref="G9" si="5">D9-C9</f>
-        <v>1.1574076779652387E-5</v>
+        <v>1.1574069503694773E-5</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ref="H9" si="6">E9-D9</f>
-        <v>4.6296292566694319E-5</v>
+        <v>4.6296299842651933E-5</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>2.6620370044838637E-4</v>
+        <v>3.0092593078734353E-4</v>
       </c>
       <c r="K9">
         <v>1781</v>
@@ -826,32 +831,32 @@
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>44207.604143518518</v>
+        <v>44213.804386574076</v>
       </c>
       <c r="C10" s="1">
-        <v>44207.604259259257</v>
+        <v>44213.804490740738</v>
       </c>
       <c r="D10" s="1">
-        <v>44207.604270833333</v>
+        <v>44213.804513888892</v>
       </c>
       <c r="E10" s="1">
-        <v>44207.604444444441</v>
+        <v>44213.804664351854</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>1.1574073869269341E-4</v>
+        <v>1.0416666191304103E-4</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" ref="G10:G11" si="7">D10-C10</f>
-        <v>1.1574076779652387E-5</v>
+        <v>2.3148153559304774E-5</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ref="H10:H11" si="8">E10-D10</f>
-        <v>1.7361110803904012E-4</v>
+        <v>1.5046296175569296E-4</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="1"/>
-        <v>3.0092592351138592E-4</v>
+        <v>2.7777777722803876E-4</v>
       </c>
       <c r="K10">
         <v>1810</v>
@@ -870,32 +875,36 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>44207.604444444441</v>
+        <v>44213.804664351854</v>
       </c>
       <c r="C11" s="1">
-        <v>44207.604618055557</v>
+        <v>44213.804837962962</v>
       </c>
       <c r="D11" s="1">
-        <v>44207.604675925926</v>
+        <v>44213.804884259262</v>
       </c>
       <c r="E11" s="1">
-        <v>44207.605150462965</v>
+        <v>44213.805347222224</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>1.7361111531499773E-4</v>
+        <v>1.7361110803904012E-4</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="7"/>
-        <v>5.7870369346346706E-5</v>
+        <v>4.6296299842651933E-5</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="8"/>
-        <v>4.7453703882638365E-4</v>
+        <v>4.6296296204673126E-4</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="1"/>
-        <v>7.0601852348772809E-4</v>
+        <v>6.8287036992842332E-4</v>
+      </c>
+      <c r="J11" s="2">
+        <f>SUM(I2:I11)</f>
+        <v>5.8298611111240461E-2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -903,32 +912,32 @@
         <v>40</v>
       </c>
       <c r="B12" s="1">
-        <v>44213.332650462966</v>
+        <v>44213.805347222224</v>
       </c>
       <c r="C12" s="1">
-        <v>44213.334609710648</v>
+        <v>44213.807071759256</v>
       </c>
       <c r="D12" s="1">
-        <v>44213.335057870368</v>
+        <v>44213.807557870372</v>
       </c>
       <c r="E12" s="1">
-        <v>44213.336493275463</v>
+        <v>44213.808831018519</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" ref="F12:F14" si="9">C12-B12</f>
-        <v>1.9592476819525473E-3</v>
+        <f t="shared" ref="F12:F15" si="9">C12-B12</f>
+        <v>1.7245370327145793E-3</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G12:G14" si="10">D12-C12</f>
-        <v>4.4815972069045529E-4</v>
+        <f t="shared" ref="G12:G15" si="10">D12-C12</f>
+        <v>4.8611111560603604E-4</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H12:H14" si="11">E12-D12</f>
-        <v>1.4354050945257768E-3</v>
+        <f t="shared" ref="H12:H15" si="11">E12-D12</f>
+        <v>1.2731481474475004E-3</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ref="I12:I14" si="12">SUM(F12:H12)</f>
-        <v>3.8428124971687794E-3</v>
+        <v>3.4837962957681157E-3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -936,32 +945,32 @@
         <v>41</v>
       </c>
       <c r="B13" s="1">
-        <v>44213.536539351851</v>
+        <v>44215.502141203702</v>
       </c>
       <c r="C13" s="1">
-        <v>44213.536921296298</v>
+        <v>44215.502766203703</v>
       </c>
       <c r="D13" s="1">
-        <v>44213.53702546296</v>
+        <v>44215.502881944441</v>
       </c>
       <c r="E13" s="1">
-        <v>44213.537301331016</v>
+        <v>44215.503263888888</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="9"/>
-        <v>3.819444464170374E-4</v>
+        <v>6.2500000058207661E-4</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="10"/>
-        <v>1.0416666191304103E-4</v>
+        <v>1.1574073869269341E-4</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="11"/>
-        <v>2.7586805663304403E-4</v>
+        <v>3.819444464170374E-4</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="12"/>
-        <v>7.6197916496312246E-4</v>
+        <v>1.1226851856918074E-3</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -969,32 +978,75 @@
         <v>42</v>
       </c>
       <c r="B14" s="1">
-        <v>44213.555555555555</v>
+        <v>44213.809675925928</v>
       </c>
       <c r="C14" s="1">
-        <v>44213.558495370373</v>
+        <v>44213.812106481484</v>
       </c>
       <c r="D14" s="1">
-        <v>44213.559004629627</v>
+        <v>44213.812604166669</v>
       </c>
       <c r="E14" s="1">
-        <v>44213.561160659723</v>
+        <v>44213.814786192132</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="9"/>
-        <v>2.9398148180916905E-3</v>
+        <v>2.4305555562023073E-3</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="10"/>
-        <v>5.0925925461342558E-4</v>
+        <v>4.9768518510973081E-4</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="11"/>
-        <v>2.1560300956480205E-3</v>
+        <v>2.1820254623889923E-3</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="12"/>
-        <v>5.6051041683531366E-3</v>
+        <v>5.1102662037010305E-3</v>
+      </c>
+      <c r="J14" s="2">
+        <f>SUM(I12:I14)</f>
+        <v>9.7167476851609536E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44215.540155358794</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44215.559965763889</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44215.686909722222</v>
+      </c>
+      <c r="E15" s="1">
+        <v>44215.696608796294</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="9"/>
+        <v>1.9810405094176531E-2</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="10"/>
+        <v>0.12694395833386807</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="11"/>
+        <v>9.6990740712499246E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
+        <f>C15-B15</f>
+        <v>1.9810405094176531E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <f>E15-D15</f>
+        <v>9.6990740712499246E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1005,15 +1057,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751965E-4A3A-442F-9C21-79FCCBFBF505}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.19921875" customWidth="1"/>
     <col min="5" max="6" width="16.19921875" bestFit="1" customWidth="1"/>
@@ -1036,19 +1088,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44207.434687499997</v>
+        <v>44213.818287037036</v>
       </c>
       <c r="C2" s="1">
-        <v>44207.435486111113</v>
+        <v>44213.818969907406</v>
       </c>
       <c r="D2" s="1"/>
       <c r="G2" s="2">
         <f t="shared" ref="G2:G11" si="0">C2-B2</f>
-        <v>7.9861111589707434E-4</v>
+        <v>6.8287036992842332E-4</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(G2:I2)</f>
-        <v>7.9861111589707434E-4</v>
+        <v>6.8287036992842332E-4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1056,10 +1108,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>44207.435486111113</v>
+        <v>44213.818969907406</v>
       </c>
       <c r="C3" s="1">
-        <v>44207.435543981483</v>
+        <v>44213.819027777776</v>
       </c>
       <c r="D3" s="1"/>
       <c r="G3" s="2">
@@ -1076,35 +1128,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>44207.435543981483</v>
+        <v>44213.819027777776</v>
       </c>
       <c r="C4" s="1">
-        <v>44207.453425925924</v>
+        <v>44213.825798611113</v>
       </c>
       <c r="D4" s="1">
-        <v>44207.466666666667</v>
+        <v>44213.827326388891</v>
       </c>
       <c r="E4" s="1">
-        <v>44207.471053240741</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44207.471215277779</v>
-      </c>
+        <v>44213.827488425923</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>1.788194444088731E-2</v>
+        <v>6.7708333372138441E-3</v>
       </c>
       <c r="H4" s="2">
         <f>D4-C4</f>
-        <v>1.3240740743640345E-2</v>
+        <v>1.527777778392192E-3</v>
       </c>
       <c r="I4" s="2">
-        <f>F4-E4</f>
-        <v>1.6203703853534535E-4</v>
+        <f>E4-D4</f>
+        <v>1.6203703125938773E-4</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="1"/>
-        <v>3.1284722223063E-2</v>
+        <v>8.4606481468654238E-3</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -1114,18 +1164,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>44207.471215277779</v>
+        <v>44213.827488425923</v>
       </c>
       <c r="C5" s="1">
-        <v>44207.471597222226</v>
+        <v>44213.827847222223</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>3.819444464170374E-4</v>
+        <v>3.5879630013369024E-4</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="1"/>
-        <v>3.819444464170374E-4</v>
+        <v>3.5879630013369024E-4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1133,18 +1183,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>44207.471597222226</v>
+        <v>44213.827847222223</v>
       </c>
       <c r="C6" s="1">
-        <v>44207.472071759257</v>
+        <v>44213.828321759262</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>4.7453703155042604E-4</v>
+        <v>4.7453703882638365E-4</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="1"/>
-        <v>4.7453703155042604E-4</v>
+        <v>4.7453703882638365E-4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1152,32 +1202,32 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>44207.472071759257</v>
+        <v>44213.828321759262</v>
       </c>
       <c r="C7" s="1">
-        <v>44207.512962962966</v>
+        <v>44213.88490740741</v>
       </c>
       <c r="D7" s="1">
-        <v>44207.52207175926</v>
+        <v>44213.899305555555</v>
       </c>
       <c r="E7" s="1">
-        <v>44207.57366898148</v>
+        <v>44213.959282407406</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>4.0891203709179536E-2</v>
+        <v>5.6585648148029577E-2</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ref="H7:I8" si="2">D7-C7</f>
-        <v>9.1087962937308475E-3</v>
+        <v>1.4398148145119194E-2</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="2"/>
-        <v>5.1597222220152617E-2</v>
+        <v>5.9976851851388346E-2</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="1"/>
-        <v>0.101597222223063</v>
+        <v>0.13096064814453712</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1185,32 +1235,32 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>44207.617361111108</v>
+        <v>44213.959282407406</v>
       </c>
       <c r="C8" s="1">
-        <v>44207.618275462963</v>
+        <v>44213.959444444445</v>
       </c>
       <c r="D8" s="1">
-        <v>44207.618321759262</v>
+        <v>44213.959490740737</v>
       </c>
       <c r="E8" s="1">
-        <v>44207.618761574071</v>
+        <v>44213.959918981483</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>9.1435185458976775E-4</v>
+        <v>1.6203703853534535E-4</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>4.6296299842651933E-5</v>
+        <v>4.6296292566694319E-5</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>4.3981480848742649E-4</v>
+        <v>4.2824074625968933E-4</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="1"/>
-        <v>1.4004629629198462E-3</v>
+        <v>6.36574077361729E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1218,20 +1268,20 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>44207.618761574071</v>
+        <v>44213.959918981483</v>
       </c>
       <c r="C9" s="1">
-        <v>44207.61922453704</v>
+        <v>44213.960277777776</v>
       </c>
       <c r="D9" s="1">
-        <v>44207.619247685187</v>
+        <v>44213.960300925923</v>
       </c>
       <c r="E9" s="1">
-        <v>44207.619317129633</v>
+        <v>44213.960370370369</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>4.6296296932268888E-4</v>
+        <v>3.5879629285773262E-4</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ref="H9" si="3">D9-C9</f>
@@ -1243,7 +1293,7 @@
       </c>
       <c r="J9" s="2">
         <f t="shared" si="1"/>
-        <v>5.5555556173203513E-4</v>
+        <v>4.5138888526707888E-4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1251,20 +1301,20 @@
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>44207.619317129633</v>
+        <v>44213.960370370369</v>
       </c>
       <c r="C10" s="1">
-        <v>44207.619479166664</v>
+        <v>44213.960532407407</v>
       </c>
       <c r="D10" s="1">
-        <v>44207.619490740741</v>
+        <v>44213.960543981484</v>
       </c>
       <c r="E10" s="1">
-        <v>44207.619745370372</v>
+        <v>44213.960787037038</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>1.6203703125938773E-4</v>
+        <v>1.6203703853534535E-4</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ref="H10:H11" si="5">D10-C10</f>
@@ -1272,11 +1322,11 @@
       </c>
       <c r="I10" s="2">
         <f t="shared" ref="I10:I11" si="6">E10-D10</f>
-        <v>2.546296309446916E-4</v>
+        <v>2.4305555416503921E-4</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="1"/>
-        <v>4.2824073898373172E-4</v>
+        <v>4.1666666948003694E-4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1284,16 +1334,16 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>44207.619745370372</v>
+        <v>44213.960787037038</v>
       </c>
       <c r="C11" s="1">
-        <v>44207.619976851849</v>
+        <v>44213.961018518516</v>
       </c>
       <c r="D11" s="1">
-        <v>44207.620046296295</v>
+        <v>44213.961087962962</v>
       </c>
       <c r="E11" s="1">
-        <v>44207.620671296296</v>
+        <v>44213.961736111109</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
@@ -1305,29 +1355,136 @@
       </c>
       <c r="I11" s="2">
         <f t="shared" si="6"/>
-        <v>6.2500000058207661E-4</v>
+        <v>6.4814814686542377E-4</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="1"/>
-        <v>9.2592592409346253E-4</v>
+        <v>9.4907407037680969E-4</v>
+      </c>
+      <c r="K11" s="2">
+        <f>SUM(J2:J11)</f>
+        <v>0.14344907407212304</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44213.961736111109</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44213.981145833335</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44213.985208333332</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44214.000081018516</v>
+      </c>
       <c r="G12" s="2">
-        <f>SUM(G2:G11)</f>
-        <v>6.2256944445834961E-2</v>
+        <f t="shared" ref="G12" si="7">C12-B12</f>
+        <v>1.9409722226555459E-2</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H12:I12" si="7">SUM(H2:H11)</f>
-        <v>2.2500000006402843E-2</v>
+        <f t="shared" ref="H12" si="8">D12-C12</f>
+        <v>4.0624999965075403E-3</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="7"/>
-        <v>5.3148148144828156E-2</v>
+        <f t="shared" ref="I12" si="9">E12-D12</f>
+        <v>1.4872685183945578E-2</v>
       </c>
       <c r="J12" s="2">
-        <f>SUM(G12:I12)</f>
-        <v>0.13790509259706596</v>
+        <f t="shared" ref="J12" si="10">SUM(G12:I12)</f>
+        <v>3.8344907407008577E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44214.000081018516</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44214.004120370373</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44214.004803240743</v>
+      </c>
+      <c r="E13" s="1">
+        <v>44214.007384259261</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" ref="G13:G14" si="11">C13-B13</f>
+        <v>4.0393518575001508E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" ref="H13:H14" si="12">D13-C13</f>
+        <v>6.8287036992842332E-4</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" ref="I13:I14" si="13">E13-D13</f>
+        <v>2.5810185179580003E-3</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" ref="J13:J14" si="14">SUM(G13:I13)</f>
+        <v>7.3032407453865744E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44214.007384259261</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44214.032986111109</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44214.037870370368</v>
+      </c>
+      <c r="E14" s="1">
+        <v>44214.060711805556</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="11"/>
+        <v>2.5601851848477963E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="12"/>
+        <v>4.8842592586879618E-3</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="13"/>
+        <v>2.2841435187729076E-2</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="14"/>
+        <v>5.3327546294895001E-2</v>
+      </c>
+      <c r="K14" s="2">
+        <f>SUM(J12:J14)</f>
+        <v>9.8975694447290152E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G15" s="2">
+        <f>SUM(G2:G14)</f>
+        <v>0.11489583334332565</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15:J15" si="15">SUM(H2:H14)</f>
+        <v>2.5706018510391004E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="15"/>
+        <v>0.10182291666569654</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="15"/>
+        <v>0.24242476851941319</v>
       </c>
     </row>
   </sheetData>
@@ -1338,24 +1495,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87CE502-9FA2-453D-9130-46B0AFC0874E}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.19921875" customWidth="1"/>
-    <col min="4" max="7" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
@@ -1378,7 +1536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1417,7 +1575,7 @@
         <v>1.1574073869269341E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1452,11 +1610,11 @@
         <v>0</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K15" si="2">SUM(H3:J3)</f>
+        <f t="shared" ref="K3:K14" si="2">SUM(H3:J3)</f>
         <v>1.1574076779652387E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1495,7 +1653,7 @@
         <v>1.5856481550144963E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1516,7 +1674,7 @@
         <v>3.4722215787041932E-5</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:J14" si="3">E5-D5</f>
+        <f t="shared" ref="I5:I14" si="3">E5-D5</f>
         <v>2.314814628334716E-5</v>
       </c>
       <c r="K5" s="4">
@@ -1524,7 +1682,7 @@
         <v>5.7870362070389092E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1563,7 +1721,7 @@
         <v>1.1574073869269341E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1592,7 +1750,7 @@
         <v>0.39409722222626442</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1631,7 +1789,7 @@
         <v>3.5949074073869269E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1670,7 +1828,7 @@
         <v>5.2083333139307797E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1709,7 +1867,7 @@
         <v>1.122685192967765E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1748,7 +1906,7 @@
         <v>4.7453703155042604E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1787,7 +1945,7 @@
         <v>7.8703703911742195E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1816,7 +1974,7 @@
         <v>6.454861110978527E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1844,8 +2002,12 @@
         <f t="shared" si="2"/>
         <v>1.3194444472901523E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="4">
+        <f>SUM(K2:K14)</f>
+        <v>0.50070601852348773</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1884,7 +2046,7 @@
         <v>5.2499999997962732E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1902,6 +2064,9 @@
       </c>
       <c r="F16" s="1">
         <v>44214.171851851854</v>
+      </c>
+      <c r="G16" s="1">
+        <v>44214.298935185187</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" ref="H16" si="6">C16-B16</f>
@@ -1911,12 +2076,16 @@
         <f t="shared" ref="I16" si="7">E16-D16</f>
         <v>0.12162037037342088</v>
       </c>
+      <c r="J16" s="4">
+        <f>G16-F16</f>
+        <v>0.12708333333284827</v>
+      </c>
       <c r="K16" s="4">
         <f t="shared" ref="K16" si="8">SUM(H16:J16)</f>
-        <v>0.14421296296495711</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.27129629629780538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1933,7 +2102,10 @@
         <v>44213.878611111111</v>
       </c>
       <c r="F17" s="1">
-        <v>44214.171851851854</v>
+        <v>44215.258518518516</v>
+      </c>
+      <c r="G17" s="1">
+        <v>44215.6175</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" ref="H17" si="9">C17-B17</f>
@@ -1943,9 +2115,23 @@
         <f t="shared" ref="I17" si="10">E17-D17</f>
         <v>0.28870370370714227</v>
       </c>
+      <c r="J17" s="4">
+        <f>G17-F17</f>
+        <v>0.35898148148407927</v>
+      </c>
       <c r="K17" s="4">
         <f t="shared" ref="K17" si="11">SUM(H17:J17)</f>
-        <v>0.31942129629896954</v>
+        <v>0.6784027777830488</v>
+      </c>
+      <c r="L17" s="10">
+        <f>SUM(K15:K17)</f>
+        <v>1.0021990740788169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K18" s="10">
+        <f>SUM(K2:K17)</f>
+        <v>1.5029050926023046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished step 1 of preferred household extraction
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57C1415-F448-4906-9F20-D301F9159D1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EC44BC-81A7-4CE4-B650-DBE17A733991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>readindividuals</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>consolidatepreferredhousehold</t>
+  </si>
+  <si>
+    <t>Larger batch size</t>
+  </si>
+  <si>
+    <t>batchonindividualid HHMemberships</t>
+  </si>
+  <si>
+    <t>batchonindividualid Residencies</t>
+  </si>
+  <si>
+    <t>consolidatepreferredhousehold_new</t>
   </si>
 </sst>
 </file>
@@ -188,7 +200,7 @@
     <numFmt numFmtId="166" formatCode="hh:mm:ss;@"/>
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="dd\ hh:mm:ss;@"/>
+    <numFmt numFmtId="169" formatCode="dd\ hh:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -240,10 +252,10 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -560,32 +572,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="16.59765625" customWidth="1"/>
-    <col min="6" max="6" width="9.3984375" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="16.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.3984375" customWidth="1"/>
+    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -595,16 +607,16 @@
       <c r="C2" s="1">
         <v>44213.747488425928</v>
       </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F11" si="0">C2-B2</f>
+      <c r="H2" s="2">
+        <f t="shared" ref="H2:H11" si="0">C2-B2</f>
         <v>4.398148157633841E-4</v>
       </c>
-      <c r="I2" s="2">
-        <f>SUM(F2:H2)</f>
+      <c r="K2" s="2">
+        <f>SUM(H2:J2)</f>
         <v>4.398148157633841E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -614,16 +626,16 @@
       <c r="C3" s="1">
         <v>44213.747523148151</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <f t="shared" si="0"/>
         <v>3.4722223062999547E-5</v>
       </c>
-      <c r="I3" s="2">
-        <f t="shared" ref="I3:I11" si="1">SUM(F3:H3)</f>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K11" si="1">SUM(H3:J3)</f>
         <v>3.4722223062999547E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -636,27 +648,29 @@
       <c r="D4" s="1">
         <v>44213.753182870372</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
         <v>44213.753449074073</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="1"/>
+      <c r="H4" s="2">
         <f t="shared" si="0"/>
         <v>4.8726851819083095E-3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <f>D4-C4</f>
         <v>7.8703703911742195E-4</v>
       </c>
-      <c r="H4" s="2">
-        <f>E4-D4</f>
+      <c r="J4" s="2">
+        <f>F4-D4</f>
         <v>2.6620370044838637E-4</v>
       </c>
-      <c r="I4" s="2">
+      <c r="K4" s="2">
         <f t="shared" si="1"/>
         <v>5.9259259214741178E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -666,16 +680,16 @@
       <c r="C5" s="1">
         <v>44213.753645833334</v>
       </c>
-      <c r="F5" s="2">
+      <c r="H5" s="2">
         <f t="shared" si="0"/>
         <v>1.9675926159834489E-4</v>
       </c>
-      <c r="I5" s="2">
+      <c r="K5" s="2">
         <f t="shared" si="1"/>
         <v>1.9675926159834489E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -685,16 +699,16 @@
       <c r="C6" s="1">
         <v>44213.753912037035</v>
       </c>
-      <c r="F6" s="2">
+      <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>2.6620370044838637E-4</v>
       </c>
-      <c r="I6" s="2">
+      <c r="K6" s="2">
         <f t="shared" si="1"/>
         <v>2.6620370044838637E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -707,38 +721,40 @@
       <c r="D7" s="1">
         <v>44213.780173611114</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
         <v>44213.803611111114</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="1"/>
+      <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>2.1122685189766344E-2</v>
       </c>
-      <c r="G7" s="2">
-        <f t="shared" ref="G7:H7" si="2">D7-C7</f>
+      <c r="I7" s="2">
+        <f>D7-C7</f>
         <v>5.1388888896326534E-3</v>
       </c>
-      <c r="H7" s="2">
-        <f t="shared" si="2"/>
+      <c r="J7" s="2">
+        <f>F7-D7</f>
         <v>2.34375E-2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="K7" s="2">
         <f t="shared" si="1"/>
         <v>4.9699074079398997E-2</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>411</v>
       </c>
-      <c r="L7">
-        <f>TRUNC(K7/60,0)</f>
+      <c r="N7">
+        <f>TRUNC(M7/60,0)</f>
         <v>6</v>
       </c>
-      <c r="M7">
-        <f>K7-(L7*60)</f>
+      <c r="O7">
+        <f>M7-(N7*60)</f>
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -751,38 +767,40 @@
       <c r="D8" s="1">
         <v>44213.803773148145</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
         <v>44213.804085648146</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="1"/>
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>1.2731480819638819E-4</v>
       </c>
-      <c r="G8" s="2">
-        <f t="shared" ref="G8" si="3">D8-C8</f>
+      <c r="I8" s="2">
+        <f t="shared" ref="I8" si="2">D8-C8</f>
         <v>3.4722223062999547E-5</v>
       </c>
-      <c r="H8" s="2">
-        <f t="shared" ref="H8" si="4">E8-D8</f>
+      <c r="J8" s="2">
+        <f t="shared" ref="J8" si="3">F8-D8</f>
         <v>3.125000002910383E-4</v>
       </c>
-      <c r="I8" s="2">
+      <c r="K8" s="2">
         <f t="shared" si="1"/>
         <v>4.7453703155042604E-4</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>427</v>
       </c>
-      <c r="L8">
-        <f>TRUNC(K8/60,0)</f>
+      <c r="N8">
+        <f>TRUNC(M8/60,0)</f>
         <v>7</v>
       </c>
-      <c r="M8">
-        <f>K8-(L8*60)</f>
+      <c r="O8">
+        <f>M8-(N8*60)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -795,38 +813,40 @@
       <c r="D9" s="1">
         <v>44213.804340277777</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
         <v>44213.804386574076</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="1"/>
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
         <v>2.4305556144099683E-4</v>
       </c>
-      <c r="G9" s="2">
-        <f t="shared" ref="G9" si="5">D9-C9</f>
+      <c r="I9" s="2">
+        <f t="shared" ref="I9" si="4">D9-C9</f>
         <v>1.1574069503694773E-5</v>
       </c>
-      <c r="H9" s="2">
-        <f t="shared" ref="H9" si="6">E9-D9</f>
+      <c r="J9" s="2">
+        <f t="shared" ref="J9" si="5">F9-D9</f>
         <v>4.6296299842651933E-5</v>
       </c>
-      <c r="I9" s="2">
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
         <v>3.0092593078734353E-4</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>1781</v>
       </c>
-      <c r="L9">
-        <f>TRUNC(K9/60,0)</f>
+      <c r="N9">
+        <f>TRUNC(M9/60,0)</f>
         <v>29</v>
       </c>
-      <c r="M9">
-        <f>K9-(L9*60)</f>
+      <c r="O9">
+        <f>M9-(N9*60)</f>
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -839,38 +859,40 @@
       <c r="D10" s="1">
         <v>44213.804513888892</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
         <v>44213.804664351854</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="1"/>
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>1.0416666191304103E-4</v>
       </c>
-      <c r="G10" s="2">
-        <f t="shared" ref="G10:G11" si="7">D10-C10</f>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:I11" si="6">D10-C10</f>
         <v>2.3148153559304774E-5</v>
       </c>
-      <c r="H10" s="2">
-        <f t="shared" ref="H10:H11" si="8">E10-D10</f>
+      <c r="J10" s="2">
+        <f t="shared" ref="J10:J11" si="7">F10-D10</f>
         <v>1.5046296175569296E-4</v>
       </c>
-      <c r="I10" s="2">
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
         <v>2.7777777722803876E-4</v>
       </c>
-      <c r="K10">
-        <v>1810</v>
-      </c>
-      <c r="L10">
-        <f>TRUNC(K10/60,0)</f>
-        <v>30</v>
-      </c>
       <c r="M10">
-        <f>K10-(L10*60)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>9641</v>
+      </c>
+      <c r="N10">
+        <f>TRUNC(M10/60,0)</f>
+        <v>160</v>
+      </c>
+      <c r="O10">
+        <f>M10-(N10*60)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -883,31 +905,33 @@
       <c r="D11" s="1">
         <v>44213.804884259262</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
         <v>44213.805347222224</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="1"/>
+      <c r="H11" s="2">
         <f t="shared" si="0"/>
         <v>1.7361110803904012E-4</v>
       </c>
-      <c r="G11" s="2">
+      <c r="I11" s="2">
+        <f t="shared" si="6"/>
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="7"/>
-        <v>4.6296299842651933E-5</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="8"/>
         <v>4.6296296204673126E-4</v>
       </c>
-      <c r="I11" s="2">
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
         <v>6.8287036992842332E-4</v>
       </c>
-      <c r="J11" s="2">
-        <f>SUM(I2:I11)</f>
+      <c r="L11" s="2">
+        <f>SUM(K2:K11)</f>
         <v>5.8298611111240461E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -920,27 +944,29 @@
       <c r="D12" s="1">
         <v>44213.807557870372</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
         <v>44213.808831018519</v>
       </c>
-      <c r="F12" s="2">
-        <f t="shared" ref="F12:F15" si="9">C12-B12</f>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2">
+        <f t="shared" ref="H12:H15" si="8">C12-B12</f>
         <v>1.7245370327145793E-3</v>
       </c>
-      <c r="G12" s="2">
-        <f t="shared" ref="G12:G15" si="10">D12-C12</f>
+      <c r="I12" s="2">
+        <f t="shared" ref="I12:I14" si="9">D12-C12</f>
         <v>4.8611111560603604E-4</v>
       </c>
-      <c r="H12" s="2">
-        <f t="shared" ref="H12:H15" si="11">E12-D12</f>
+      <c r="J12" s="2">
+        <f t="shared" ref="J12:J14" si="10">F12-D12</f>
         <v>1.2731481474475004E-3</v>
       </c>
-      <c r="I12" s="2">
-        <f t="shared" ref="I12:I14" si="12">SUM(F12:H12)</f>
+      <c r="K12" s="2">
+        <f t="shared" ref="K12:K18" si="11">SUM(H12:J12)</f>
         <v>3.4837962957681157E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -953,27 +979,29 @@
       <c r="D13" s="1">
         <v>44215.502881944441</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
         <v>44215.503263888888</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="1"/>
+      <c r="H13" s="2">
+        <f t="shared" si="8"/>
+        <v>6.2500000058207661E-4</v>
+      </c>
+      <c r="I13" s="2">
         <f t="shared" si="9"/>
-        <v>6.2500000058207661E-4</v>
-      </c>
-      <c r="G13" s="2">
+        <v>1.1574073869269341E-4</v>
+      </c>
+      <c r="J13" s="2">
         <f t="shared" si="10"/>
-        <v>1.1574073869269341E-4</v>
-      </c>
-      <c r="H13" s="2">
+        <v>3.819444464170374E-4</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="11"/>
-        <v>3.819444464170374E-4</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="12"/>
         <v>1.1226851856918074E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -986,67 +1014,186 @@
       <c r="D14" s="1">
         <v>44213.812604166669</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
         <v>44213.814786192132</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="1"/>
+      <c r="H14" s="2">
+        <f t="shared" si="8"/>
+        <v>2.4305555562023073E-3</v>
+      </c>
+      <c r="I14" s="2">
         <f t="shared" si="9"/>
-        <v>2.4305555562023073E-3</v>
-      </c>
-      <c r="G14" s="2">
+        <v>4.9768518510973081E-4</v>
+      </c>
+      <c r="J14" s="2">
         <f t="shared" si="10"/>
-        <v>4.9768518510973081E-4</v>
-      </c>
-      <c r="H14" s="2">
+        <v>2.1820254623889923E-3</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="11"/>
-        <v>2.1820254623889923E-3</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="12"/>
         <v>5.1102662037010305E-3</v>
       </c>
-      <c r="J14" s="2">
-        <f>SUM(I12:I14)</f>
+      <c r="L14" s="2">
+        <f>SUM(K12:K14)</f>
         <v>9.7167476851609536E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="1">
-        <v>44215.540155358794</v>
+        <v>44219.502665462962</v>
       </c>
       <c r="C15" s="1">
-        <v>44215.559965763889</v>
+        <v>44219.615664467594</v>
       </c>
       <c r="D15" s="1">
-        <v>44215.686909722222</v>
+        <v>44219.743531585649</v>
       </c>
       <c r="E15" s="1">
-        <v>44215.696608796294</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="9"/>
-        <v>1.9810405094176531E-2</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="10"/>
-        <v>0.12694395833386807</v>
+        <v>44219.760384479167</v>
+      </c>
+      <c r="F15" s="1">
+        <v>44219.647407581018</v>
+      </c>
+      <c r="G15" s="1">
+        <v>44219.733087175926</v>
       </c>
       <c r="H15" s="2">
+        <f t="shared" si="8"/>
+        <v>0.11299900463200174</v>
+      </c>
+      <c r="I15" s="2">
+        <f>E15-D15</f>
+        <v>1.6852893517352641E-2</v>
+      </c>
+      <c r="J15" s="2">
+        <f>G15-F15</f>
+        <v>8.5679594907560386E-2</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="11"/>
-        <v>9.6990740712499246E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="2">
-        <f>C15-B15</f>
-        <v>1.9810405094176531E-2</v>
-      </c>
-      <c r="D16" s="2">
-        <f>E15-D15</f>
-        <v>9.6990740712499246E-3</v>
+        <v>0.21553149305691477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44227.61346064815</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44227.643240740741</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44227.602999247683</v>
+      </c>
+      <c r="E16" s="1">
+        <v>44227.608685057872</v>
+      </c>
+      <c r="F16" s="1">
+        <v>44227.643240740741</v>
+      </c>
+      <c r="G16" s="1">
+        <v>44227.669293981482</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" ref="H16:J18" si="12">C16-B16</f>
+        <v>2.9780092590954155E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <f>E16-D16</f>
+        <v>5.6858101888792589E-3</v>
+      </c>
+      <c r="J16" s="2">
+        <f>G16-F16</f>
+        <v>2.6053240741021E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="11"/>
+        <v>6.1519143520854414E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44227.731305937501</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44227.750009814816</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44227.750009814816</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44227.753300185184</v>
+      </c>
+      <c r="F17" s="1">
+        <v>44227.753300185184</v>
+      </c>
+      <c r="G17" s="1">
+        <v>44227.766293009263</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="12"/>
+        <v>1.8703877314692363E-2</v>
+      </c>
+      <c r="I17" s="2">
+        <f>E17-D17</f>
+        <v>3.2903703686315566E-3</v>
+      </c>
+      <c r="J17" s="2">
+        <f>G17-F17</f>
+        <v>1.2992824078537524E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="11"/>
+        <v>3.4987071761861444E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44229.358229166668</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44229.469814814816</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44229.579027777778</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44230.594293981485</v>
+      </c>
+      <c r="F18" s="1">
+        <v>44229.469814814816</v>
+      </c>
+      <c r="G18" s="1">
+        <v>44230.552523148152</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="12"/>
+        <v>0.11158564814832062</v>
+      </c>
+      <c r="I18" s="2">
+        <f>E18-D18</f>
+        <v>1.0152662037071423</v>
+      </c>
+      <c r="J18" s="2">
+        <f>G18-F18</f>
+        <v>1.0827083333351766</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="11"/>
+        <v>2.2095601851906395</v>
       </c>
     </row>
   </sheetData>
@@ -1057,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751965E-4A3A-442F-9C21-79FCCBFBF505}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1069,6 +1216,7 @@
     <col min="2" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.19921875" customWidth="1"/>
     <col min="5" max="6" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1485,6 +1633,107 @@
       <c r="J15" s="2">
         <f t="shared" si="15"/>
         <v>0.24242476851941319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44215.336111111108</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44215.36445601852</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44215.370115740741</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44215.388043981482</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17" si="16">C17-B17</f>
+        <v>2.8344907412247267E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" ref="H17" si="17">D17-C17</f>
+        <v>5.6597222210257314E-3</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" ref="I17" si="18">E17-D17</f>
+        <v>1.7928240740729962E-2</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" ref="J17" si="19">SUM(G17:I17)</f>
+        <v>5.193287037400296E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44215.388043981482</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44215.397326388891</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44215.398449074077</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44215.423657407409</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" ref="G18:G19" si="20">C18-B18</f>
+        <v>9.2824074090458453E-3</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H18:H19" si="21">D18-C18</f>
+        <v>1.1226851856918074E-3</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" ref="I18:I19" si="22">E18-D18</f>
+        <v>2.5208333332557231E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" ref="J18:J19" si="23">SUM(G18:I18)</f>
+        <v>3.5613425927294884E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44215.423657407409</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44215.478981481479</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44215.484976099535</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="20"/>
+        <v>5.5324074070085771E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="21"/>
+        <v>5.9946180554106832E-3</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="22"/>
+        <v>-44215.484976099535</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="23"/>
+        <v>-44215.423657407409</v>
       </c>
     </row>
   </sheetData>
@@ -1510,22 +1759,22 @@
     <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.296875" customWidth="1"/>
+    <col min="11" max="12" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="10"/>
       <c r="H1" t="s">
         <v>6</v>
       </c>
@@ -2123,13 +2372,13 @@
         <f t="shared" ref="K17" si="11">SUM(H17:J17)</f>
         <v>0.6784027777830488</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="9">
         <f>SUM(K15:K17)</f>
         <v>1.0021990740788169</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <f>SUM(K2:K17)</f>
         <v>1.5029050926023046</v>
       </c>

</xml_diff>

<commit_message>
Added count of memberships to preferred household days extraction
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EC44BC-81A7-4CE4-B650-DBE17A733991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AE3827-9B3C-4AC8-8E28-8D565171243D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Performance_SNOW" sheetId="1" r:id="rId1"/>
     <sheet name="Performance_CHPC" sheetId="2" r:id="rId2"/>
     <sheet name="Pentaho_SNOW" sheetId="3" r:id="rId3"/>
-    <sheet name="New Algorithm" sheetId="4" r:id="rId4"/>
+    <sheet name="Pentaho_CHPC" sheetId="5" r:id="rId4"/>
+    <sheet name="New Algorithm" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
   <si>
     <t>readindividuals</t>
   </si>
@@ -187,6 +188,60 @@
   </si>
   <si>
     <t>consolidatepreferredhousehold_new</t>
+  </si>
+  <si>
+    <t>Consolidate Preferred HH</t>
+  </si>
+  <si>
+    <t>Recover Resident Days No Membership</t>
+  </si>
+  <si>
+    <t>Set residency flags</t>
+  </si>
+  <si>
+    <t>Add Individual Characteristics</t>
+  </si>
+  <si>
+    <t>Coresident with mother</t>
+  </si>
+  <si>
+    <t>Coresident with father</t>
+  </si>
+  <si>
+    <t>DP09_01 Produce Basic Episodes</t>
+  </si>
+  <si>
+    <t>DP09_02 Fix Basic Episodes</t>
+  </si>
+  <si>
+    <t>DP09_07 Basic Episode QC</t>
+  </si>
+  <si>
+    <t>DP09_03 Produce Anonymisation Maps</t>
+  </si>
+  <si>
+    <t>DP09_04 Anonymise Episodes</t>
+  </si>
+  <si>
+    <t>DP09_05 Produce csv Episode File</t>
+  </si>
+  <si>
+    <t>DP09_06 Produce Stata Episode File</t>
+  </si>
+  <si>
+    <t>DP09-10 Produce Age Yr Delivery Surveillance Episodes</t>
+  </si>
+  <si>
+    <t>DP09-11 Fix Age Yr Delivery Surveillance Episodes</t>
+  </si>
+  <si>
+    <t>DP09_12 Anonymise Yr Age Fertility Episodes</t>
+  </si>
+  <si>
+    <t>DP09-13 Produce Stata YrAge Fertility Episode File</t>
+  </si>
+  <si>
+    <t>consolidatepreferredhousehold_memberships</t>
   </si>
 </sst>
 </file>
@@ -572,21 +627,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="16.59765625" customWidth="1"/>
     <col min="8" max="8" width="9.3984375" customWidth="1"/>
     <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="10"/>
       <c r="H1" t="s">
         <v>5</v>
       </c>
@@ -1102,7 +1169,7 @@
         <v>44227.669293981482</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16:J18" si="12">C16-B16</f>
+        <f t="shared" ref="H16:H19" si="12">C16-B16</f>
         <v>2.9780092590954155E-2</v>
       </c>
       <c r="I16" s="2">
@@ -1196,7 +1263,27 @@
         <v>2.2095601851906395</v>
       </c>
     </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44231.329687500001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44231.464463171294</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="12"/>
+        <v>0.1347756712930277</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1207,7 +1294,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1744,15 +1831,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87CE502-9FA2-453D-9130-46B0AFC0874E}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="H18" sqref="H18:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.19921875" customWidth="1"/>
     <col min="4" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
@@ -2330,7 +2417,7 @@
         <v>0.12708333333284827</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" ref="K16" si="8">SUM(H16:J16)</f>
+        <f t="shared" ref="K16:K34" si="8">SUM(H16:J16)</f>
         <v>0.27129629629780538</v>
       </c>
     </row>
@@ -2357,7 +2444,7 @@
         <v>44215.6175</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" ref="H17" si="9">C17-B17</f>
+        <f t="shared" ref="H17:H34" si="9">C17-B17</f>
         <v>3.071759259182727E-2</v>
       </c>
       <c r="I17" s="4">
@@ -2378,9 +2465,328 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K18" s="9">
-        <f>SUM(K2:K17)</f>
-        <v>1.5029050926023046</v>
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44230.637939814813</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44230.668402777781</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="9"/>
+        <v>3.0462962968158536E-2</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="8"/>
+        <v>3.0462962968158536E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44230.668402777781</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44230.703680555554</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="9"/>
+        <v>3.5277777773444541E-2</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="8"/>
+        <v>3.5277777773444541E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44230.703680555554</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44230.739537037036</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="9"/>
+        <v>3.5856481481459923E-2</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="8"/>
+        <v>3.5856481481459923E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44230.739537037036</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44230.871516203704</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="9"/>
+        <v>0.13197916666831588</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="8"/>
+        <v>0.13197916666831588</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44230.871516203704</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44230.987372685187</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11585648148320615</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="8"/>
+        <v>0.11585648148320615</v>
+      </c>
+      <c r="L23" s="4">
+        <f>SUM(K18:K23)</f>
+        <v>0.34943287037458504</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44230.739537037036</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44230.771828703706</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="9"/>
+        <v>3.2291666670062114E-2</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="8"/>
+        <v>3.2291666670062114E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44230.771828703706</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44230.772337962961</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="9"/>
+        <v>5.0925925461342558E-4</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="8"/>
+        <v>5.0925925461342558E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44230.772337962961</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44230.772430555553</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" si="9"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" si="8"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44230.772430555553</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44230.772488425922</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="9"/>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="8"/>
+        <v>5.7870369346346706E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44230.772488425922</v>
+      </c>
+      <c r="C28" s="1">
+        <v>44230.772546296299</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="9"/>
+        <v>5.787037662230432E-5</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="8"/>
+        <v>5.787037662230432E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44230.772546296299</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44230.772569444445</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="9"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" si="8"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44230.772569444445</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44230.772986111115</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="9"/>
+        <v>4.1666666948003694E-4</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" si="8"/>
+        <v>4.1666666948003694E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44230.772986111115</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44230.903402777774</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" si="9"/>
+        <v>0.13041666665958473</v>
+      </c>
+      <c r="K31" s="4">
+        <f t="shared" si="8"/>
+        <v>0.13041666665958473</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44230.903402777774</v>
+      </c>
+      <c r="C32" s="1">
+        <v>44230.905821759261</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="9"/>
+        <v>2.4189814866986126E-3</v>
+      </c>
+      <c r="K32" s="4">
+        <f t="shared" si="8"/>
+        <v>2.4189814866986126E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44230.905821759261</v>
+      </c>
+      <c r="C33" s="1">
+        <v>44230.906134259261</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="9"/>
+        <v>3.125000002910383E-4</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" si="8"/>
+        <v>3.125000002910383E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44230.906134259261</v>
+      </c>
+      <c r="C34" s="1">
+        <v>44230.909386574072</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="9"/>
+        <v>3.2523148111067712E-3</v>
+      </c>
+      <c r="K34" s="4">
+        <f t="shared" si="8"/>
+        <v>3.2523148111067712E-3</v>
+      </c>
+      <c r="L34" s="4">
+        <f>SUM(K24:K34)</f>
+        <v>0.16984953703649808</v>
       </c>
     </row>
   </sheetData>
@@ -2395,6 +2801,977 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373E5D0C-070B-4F8C-A080-FA6C8B658209}">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="4" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44230.316111111111</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44230.316145833334</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44230.384560185186</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44230.384618055556</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44230.697557870371</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44230.697627314818</v>
+      </c>
+      <c r="H2" s="4">
+        <f>C2-B2</f>
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="I2" s="4">
+        <f>E2-D2</f>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="J2" s="4">
+        <f>G2-F2</f>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="K2" s="4">
+        <f>SUM(H2:J2)</f>
+        <v>1.6203703853534535E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44230.316145833334</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44230.316157407404</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44230.384618055556</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44230.384618055556</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44230.697627314818</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44230.697638888887</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H34" si="0">C3-B3</f>
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="I3" s="4">
+        <f>E3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J12" si="1">G3-F3</f>
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="K3" s="4">
+        <f t="shared" ref="K3:K14" si="2">SUM(H3:J3)</f>
+        <v>2.3148139007389545E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44230.316157407404</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44230.31622685185</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44230.384618055556</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44230.384953703702</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44230.697638888887</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44230.698599537034</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="0"/>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="I4" s="4">
+        <f>E4-D4</f>
+        <v>3.3564814657438546E-4</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
+        <v>9.6064814715646207E-4</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" si="2"/>
+        <v>1.3657407398568466E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44230.31622685185</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44230.31627314815</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44230.384953703702</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44230.385717592595</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" ref="I5:I17" si="3">E5-D5</f>
+        <v>7.638888928340748E-4</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="2"/>
+        <v>8.1018519267672673E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44230.31627314815</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44230.316319444442</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44230.385717592595</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44230.385798611111</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44230.698599537034</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44230.69871527778</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>8.1018515629693866E-5</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1574074596865103E-4</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="2"/>
+        <v>2.4305555416503921E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44230.31627314815</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44230.370439814818</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44230.385717592595</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44230.630671296298</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>5.4166666668606922E-2</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.24495370370277669</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.29912037037138361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44230.316319444442</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44230.316354166665</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44230.385798611111</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44230.386712962965</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44230.69871527778</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44230.757870370369</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="0"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>9.1435185458976775E-4</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="1"/>
+        <v>5.9155092589207925E-2</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="2"/>
+        <v>6.0104166666860692E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44230.316354166665</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44230.316504629627</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44230.386712962965</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44230.387187499997</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44230.757870370369</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44230.758229166669</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5046296175569296E-4</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>4.7453703155042604E-4</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="1"/>
+        <v>3.5879630013369024E-4</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="2"/>
+        <v>9.8379629343980923E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44230.316504629627</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44230.316574074073</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44230.387187499997</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44230.388495370367</v>
+      </c>
+      <c r="F10" s="1">
+        <v>44230.758229166669</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44230.758483796293</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="0"/>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="3"/>
+        <v>1.3078703705104999E-3</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="1"/>
+        <v>2.5462962366873398E-4</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="2"/>
+        <v>1.631944440305233E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44230.316574074073</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44230.316655092596</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44230.388495370367</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44230.388912037037</v>
+      </c>
+      <c r="F11" s="1">
+        <v>44230.758483796293</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44230.758888888886</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+        <v>8.101852290565148E-5</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
+        <v>4.1666666948003694E-4</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="1"/>
+        <v>4.0509259270038456E-4</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="2"/>
+        <v>9.0277778508607298E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44230.316655092596</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44230.316747685189</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44230.388912037037</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44230.389374999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>44230.758888888886</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44230.75990740741</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="0"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="3"/>
+        <v>4.6296296204673126E-4</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0185185237787664E-3</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5740740782348439E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44230.370439814818</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44230.384189814817</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44230.630671296298</v>
+      </c>
+      <c r="E13" s="1">
+        <v>44230.695868055554</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="0"/>
+        <v>1.374999999825377E-2</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="3"/>
+        <v>6.5196759256650694E-2</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="2"/>
+        <v>7.8946759254904464E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44230.384189814817</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44230.384560185186</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44230.695868055554</v>
+      </c>
+      <c r="E14" s="1">
+        <v>44230.697557870371</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="0"/>
+        <v>3.7037036963738501E-4</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="3"/>
+        <v>1.6898148169275373E-3</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="2"/>
+        <v>2.0601851865649223E-3</v>
+      </c>
+      <c r="L14" s="4">
+        <f>SUM(K2:K14)</f>
+        <v>0.447928240741021</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44230.78392361111</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44230.792361111111</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44213.589907407404</v>
+      </c>
+      <c r="E15" s="1">
+        <v>44213.616377314815</v>
+      </c>
+      <c r="F15" s="1">
+        <v>44214.171851851854</v>
+      </c>
+      <c r="G15" s="1">
+        <v>44214.194409722222</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>8.4375000005820766E-3</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="3"/>
+        <v>2.6469907410501037E-2</v>
+      </c>
+      <c r="J15" s="4">
+        <f>G15-F15</f>
+        <v>2.2557870368473232E-2</v>
+      </c>
+      <c r="K15" s="4">
+        <f>SUM(H15:J15)</f>
+        <v>5.7465277779556345E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44230.78392361111</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44230.816874999997</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44213.589907407404</v>
+      </c>
+      <c r="E16" s="1">
+        <v>44213.711527777778</v>
+      </c>
+      <c r="F16" s="1">
+        <v>44214.171851851854</v>
+      </c>
+      <c r="G16" s="1">
+        <v>44214.298935185187</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2951388886431232E-2</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.12162037037342088</v>
+      </c>
+      <c r="J16" s="4">
+        <f>G16-F16</f>
+        <v>0.12708333333284827</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" ref="K16:K34" si="4">SUM(H16:J16)</f>
+        <v>0.28165509259270038</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44230.78392361111</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44230.8278587963</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44213.589907407404</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44213.878611111111</v>
+      </c>
+      <c r="F17" s="1">
+        <v>44215.258518518516</v>
+      </c>
+      <c r="G17" s="1">
+        <v>44215.6175</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.3935185189184267E-2</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.28870370370714227</v>
+      </c>
+      <c r="J17" s="4">
+        <f>G17-F17</f>
+        <v>0.35898148148407927</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="4"/>
+        <v>0.6916203703804058</v>
+      </c>
+      <c r="L17" s="9">
+        <f>SUM(K15:K17)</f>
+        <v>1.0307407407526625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44230.8278587963</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44231.01803240741</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>0.19017361111036735</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19017361111036735</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44231.01803240741</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44231.069027777776</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0995370365853887E-2</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="4"/>
+        <v>5.0995370365853887E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44231.069027777776</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44231.113935185182</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4907407405844424E-2</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="4"/>
+        <v>4.4907407405844424E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44231.113935185182</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44231.161446759259</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.7511574077361729E-2</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="4"/>
+        <v>4.7511574077361729E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44231.161446759259</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44231.351203703707</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.18975694444816327</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18975694444816327</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="4">
+        <f>SUM(K18:K23)</f>
+        <v>0.52334490740759065</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44231.161446759259</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44231.202291666668</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="0"/>
+        <v>4.0844907409336884E-2</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="4"/>
+        <v>4.0844907409336884E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44231.202291666668</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44231.203101851854</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>8.1018518540076911E-4</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="4"/>
+        <v>8.1018518540076911E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44231.203101851854</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44231.203194444446</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" si="0"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" si="4"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44231.203194444446</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44231.203275462962</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="0"/>
+        <v>8.1018515629693866E-5</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="4"/>
+        <v>8.1018515629693866E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44231.203275462962</v>
+      </c>
+      <c r="C28" s="1">
+        <v>44231.203344907408</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="0"/>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="4"/>
+        <v>6.9444446125999093E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44231.203344907408</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44231.203379629631</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="0"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" si="4"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44231.203379629631</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44231.203888888886</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0925925461342558E-4</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" si="4"/>
+        <v>5.0925925461342558E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44231.203888888886</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44231.428657407407</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" si="0"/>
+        <v>0.22476851852115942</v>
+      </c>
+      <c r="K31" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22476851852115942</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44231.428657407407</v>
+      </c>
+      <c r="C32" s="1">
+        <v>44231.432928240742</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2708333348855376E-3</v>
+      </c>
+      <c r="K32" s="4">
+        <f t="shared" si="4"/>
+        <v>4.2708333348855376E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44231.432928240742</v>
+      </c>
+      <c r="C33" s="1">
+        <v>44231.433738425927</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="0"/>
+        <v>8.1018518540076911E-4</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" si="4"/>
+        <v>8.1018518540076911E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44231.433738425927</v>
+      </c>
+      <c r="C34" s="1">
+        <v>44231.441979166666</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="0"/>
+        <v>8.2407407389837317E-3</v>
+      </c>
+      <c r="K34" s="4">
+        <f t="shared" si="4"/>
+        <v>8.2407407389837317E-3</v>
+      </c>
+      <c r="L34" s="4">
+        <f>SUM(K24:K34)</f>
+        <v>0.28053240740700858</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF92E6BD-A1AE-49E2-AC9D-3CA6CC6267FF}">
   <dimension ref="A1:H11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Completed adding residency flags to day records
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AE3827-9B3C-4AC8-8E28-8D565171243D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D1C9E2-532C-4AC8-8666-CD9D20070091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
   <si>
     <t>readindividuals</t>
   </si>
@@ -181,15 +181,6 @@
     <t>Larger batch size</t>
   </si>
   <si>
-    <t>batchonindividualid HHMemberships</t>
-  </si>
-  <si>
-    <t>batchonindividualid Residencies</t>
-  </si>
-  <si>
-    <t>consolidatepreferredhousehold_new</t>
-  </si>
-  <si>
     <t>Consolidate Preferred HH</t>
   </si>
   <si>
@@ -241,14 +232,77 @@
     <t>DP09-13 Produce Stata YrAge Fertility Episode File</t>
   </si>
   <si>
-    <t>consolidatepreferredhousehold_memberships</t>
+    <t>DP08_04 Anonymise Episodes</t>
+  </si>
+  <si>
+    <t>DP08_05 Produce csv Episode File</t>
+  </si>
+  <si>
+    <t>DP08_06 Produce Stata Episode File</t>
+  </si>
+  <si>
+    <t>DP08_01 Produce Episodes</t>
+  </si>
+  <si>
+    <t>DP08_02 Fix Episodes</t>
+  </si>
+  <si>
+    <t>DP06_02 Expand Marital Status</t>
+  </si>
+  <si>
+    <t>DP06-01 Expand Educational Status</t>
+  </si>
+  <si>
+    <t>DP06-04 Expand Employment Status</t>
+  </si>
+  <si>
+    <t>DP07-01 Combine EducationStatus Days</t>
+  </si>
+  <si>
+    <t>DP07-02 Combine Marital Status Days</t>
+  </si>
+  <si>
+    <t>DP07-03 Combine Socioeconomic Status Days</t>
+  </si>
+  <si>
+    <t>DP07-04 Combine Labour Status Days</t>
+  </si>
+  <si>
+    <t>DP06-03 Expand Socioeconomic Status</t>
+  </si>
+  <si>
+    <t>DP04-01 Residency Days Extraction</t>
+  </si>
+  <si>
+    <t>DP04-02 Household Residency Day Extraction</t>
+  </si>
+  <si>
+    <t>DP04-03 Household Membership Day Extraction</t>
+  </si>
+  <si>
+    <t>DP05-01 Consolidate Preferred HH</t>
+  </si>
+  <si>
+    <t>DP05-02 Recover Resident Days No Membership</t>
+  </si>
+  <si>
+    <t>DP05-03 Set residency flags</t>
+  </si>
+  <si>
+    <t>DP05-04 Add Individual Characteristics</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>set residency days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -256,6 +310,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="dd\ hh:mm:ss;@"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -295,7 +350,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -308,6 +363,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -627,33 +686,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="16.59765625" customWidth="1"/>
     <col min="8" max="8" width="9.3984375" customWidth="1"/>
     <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="12"/>
       <c r="H1" t="s">
         <v>5</v>
       </c>
@@ -664,7 +725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -683,7 +744,7 @@
         <v>4.398148157633841E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -702,7 +763,7 @@
         <v>3.4722223062999547E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -737,7 +798,7 @@
         <v>5.9259259214741178E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -756,7 +817,7 @@
         <v>1.9675926159834489E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -775,7 +836,7 @@
         <v>2.6620370044838637E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -821,7 +882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -867,7 +928,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -913,7 +974,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -948,18 +1009,22 @@
         <v>2.7777777722803876E-4</v>
       </c>
       <c r="M10">
-        <v>9641</v>
+        <v>3698</v>
       </c>
       <c r="N10">
-        <f>TRUNC(M10/60,0)</f>
-        <v>160</v>
+        <f>TRUNC(M10/3600,0)</f>
+        <v>1</v>
       </c>
       <c r="O10">
-        <f>M10-(N10*60)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <f>TRUNC((M10-(3600*N10))/60,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f>M10-(3600*N10)-(O10*60)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -998,7 +1063,7 @@
         <v>5.8298611111240461E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1017,7 +1082,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2">
-        <f t="shared" ref="H12:H15" si="8">C12-B12</f>
+        <f t="shared" ref="H12:H16" si="8">C12-B12</f>
         <v>1.7245370327145793E-3</v>
       </c>
       <c r="I12" s="2">
@@ -1029,11 +1094,11 @@
         <v>1.2731481474475004E-3</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" ref="K12:K18" si="11">SUM(H12:J12)</f>
+        <f t="shared" ref="K12:K16" si="11">SUM(H12:J12)</f>
         <v>3.4837962957681157E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1068,7 +1133,7 @@
         <v>1.1226851856918074E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1106,176 +1171,93 @@
         <f>SUM(K12:K14)</f>
         <v>9.7167476851609536E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N14" s="11">
+        <v>804812006</v>
+      </c>
+      <c r="O14">
+        <v>4451</v>
+      </c>
+      <c r="P14" s="11">
+        <f>N14/O14</f>
+        <v>180815.99775331386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="1">
-        <v>44219.502665462962</v>
+        <v>44231.329687500001</v>
       </c>
       <c r="C15" s="1">
-        <v>44219.615664467594</v>
+        <v>44231.464456018519</v>
       </c>
       <c r="D15" s="1">
-        <v>44219.743531585649</v>
+        <v>44231.464456018519</v>
       </c>
       <c r="E15" s="1">
-        <v>44219.760384479167</v>
+        <v>44231.486522939813</v>
       </c>
       <c r="F15" s="1">
-        <v>44219.647407581018</v>
+        <v>44231.486516203702</v>
       </c>
       <c r="G15" s="1">
-        <v>44219.733087175926</v>
+        <v>44231.58798611111</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="8"/>
-        <v>0.11299900463200174</v>
+        <v>0.13476851851737592</v>
       </c>
       <c r="I15" s="2">
-        <f>E15-D15</f>
-        <v>1.6852893517352641E-2</v>
+        <f t="shared" ref="I15:I16" si="12">E15-D15</f>
+        <v>2.2066921294026542E-2</v>
       </c>
       <c r="J15" s="2">
-        <f>G15-F15</f>
-        <v>8.5679594907560386E-2</v>
+        <f t="shared" ref="J15:J16" si="13">G15-F15</f>
+        <v>0.10146990740759065</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="11"/>
-        <v>0.21553149305691477</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.25830534721899312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B16" s="1">
-        <v>44227.61346064815</v>
+        <v>44240.531828703701</v>
       </c>
       <c r="C16" s="1">
-        <v>44227.643240740741</v>
+        <v>44240.719846516207</v>
       </c>
       <c r="D16" s="1">
-        <v>44227.602999247683</v>
+        <v>44240.320055983793</v>
       </c>
       <c r="E16" s="1">
-        <v>44227.608685057872</v>
+        <v>44240.357453067132</v>
       </c>
       <c r="F16" s="1">
-        <v>44227.643240740741</v>
+        <v>44240.719837962963</v>
       </c>
       <c r="G16" s="1">
-        <v>44227.669293981482</v>
+        <v>44240.869258645835</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16:H19" si="12">C16-B16</f>
-        <v>2.9780092590954155E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.18801781250658678</v>
       </c>
       <c r="I16" s="2">
-        <f>E16-D16</f>
-        <v>5.6858101888792589E-3</v>
+        <f t="shared" si="12"/>
+        <v>3.7397083338873927E-2</v>
       </c>
       <c r="J16" s="2">
-        <f>G16-F16</f>
-        <v>2.6053240741021E-2</v>
+        <f t="shared" si="13"/>
+        <v>0.14942068287200527</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="11"/>
-        <v>6.1519143520854414E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44227.731305937501</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44227.750009814816</v>
-      </c>
-      <c r="D17" s="1">
-        <v>44227.750009814816</v>
-      </c>
-      <c r="E17" s="1">
-        <v>44227.753300185184</v>
-      </c>
-      <c r="F17" s="1">
-        <v>44227.753300185184</v>
-      </c>
-      <c r="G17" s="1">
-        <v>44227.766293009263</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" si="12"/>
-        <v>1.8703877314692363E-2</v>
-      </c>
-      <c r="I17" s="2">
-        <f>E17-D17</f>
-        <v>3.2903703686315566E-3</v>
-      </c>
-      <c r="J17" s="2">
-        <f>G17-F17</f>
-        <v>1.2992824078537524E-2</v>
-      </c>
-      <c r="K17" s="2">
-        <f t="shared" si="11"/>
-        <v>3.4987071761861444E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="1">
-        <v>44229.358229166668</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44229.469814814816</v>
-      </c>
-      <c r="D18" s="1">
-        <v>44229.579027777778</v>
-      </c>
-      <c r="E18" s="1">
-        <v>44230.594293981485</v>
-      </c>
-      <c r="F18" s="1">
-        <v>44229.469814814816</v>
-      </c>
-      <c r="G18" s="1">
-        <v>44230.552523148152</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="12"/>
-        <v>0.11158564814832062</v>
-      </c>
-      <c r="I18" s="2">
-        <f>E18-D18</f>
-        <v>1.0152662037071423</v>
-      </c>
-      <c r="J18" s="2">
-        <f>G18-F18</f>
-        <v>1.0827083333351766</v>
-      </c>
-      <c r="K18" s="2">
-        <f t="shared" si="11"/>
-        <v>2.2095601851906395</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="1">
-        <v>44231.329687500001</v>
-      </c>
-      <c r="C19" s="1">
-        <v>44231.464463171294</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="12"/>
-        <v>0.1347756712930277</v>
+        <v>0.37483557871746598</v>
       </c>
     </row>
   </sheetData>
@@ -1834,7 +1816,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:L34"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1850,18 +1832,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="12"/>
       <c r="H1" t="s">
         <v>6</v>
       </c>
@@ -2466,20 +2448,26 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44231.341909722221</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44231.509201388886</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.16729166666482342</v>
       </c>
       <c r="K18" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.16729166666482342</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1">
         <v>44230.637939814813</v>
@@ -2498,7 +2486,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1">
         <v>44230.668402777781</v>
@@ -2517,7 +2505,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1">
         <v>44230.703680555554</v>
@@ -2536,7 +2524,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1">
         <v>44230.739537037036</v>
@@ -2555,7 +2543,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1">
         <v>44230.871516203704</v>
@@ -2573,12 +2561,12 @@
       </c>
       <c r="L23" s="4">
         <f>SUM(K18:K23)</f>
-        <v>0.34943287037458504</v>
+        <v>0.51672453703940846</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1">
         <v>44230.739537037036</v>
@@ -2597,7 +2585,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1">
         <v>44230.771828703706</v>
@@ -2616,7 +2604,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1">
         <v>44230.772337962961</v>
@@ -2635,7 +2623,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1">
         <v>44230.772430555553</v>
@@ -2654,7 +2642,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1">
         <v>44230.772488425922</v>
@@ -2673,7 +2661,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1">
         <v>44230.772546296299</v>
@@ -2692,7 +2680,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1">
         <v>44230.772569444445</v>
@@ -2711,7 +2699,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1">
         <v>44230.772986111115</v>
@@ -2730,7 +2718,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1">
         <v>44230.903402777774</v>
@@ -2749,7 +2737,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1">
         <v>44230.905821759261</v>
@@ -2768,7 +2756,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1">
         <v>44230.906134259261</v>
@@ -2802,10 +2790,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373E5D0C-070B-4F8C-A080-FA6C8B658209}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="K2" sqref="K2:K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2814,33 +2802,36 @@
     <col min="2" max="2" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.19921875" customWidth="1"/>
     <col min="4" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.59765625" customWidth="1"/>
+    <col min="10" max="10" width="11.3984375" customWidth="1"/>
+    <col min="11" max="11" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>7</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2865,19 +2856,19 @@
       <c r="G2" s="1">
         <v>44230.697627314818</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="9">
         <f>C2-B2</f>
         <v>3.4722223062999547E-5</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="9">
         <f>E2-D2</f>
         <v>5.7870369346346706E-5</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="9">
         <f>G2-F2</f>
         <v>6.9444446125999093E-5</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="9">
         <f>SUM(H2:J2)</f>
         <v>1.6203703853534535E-4</v>
       </c>
@@ -2904,19 +2895,19 @@
       <c r="G3" s="1">
         <v>44230.697638888887</v>
       </c>
-      <c r="H3" s="4">
-        <f t="shared" ref="H3:H34" si="0">C3-B3</f>
+      <c r="H3" s="9">
+        <f t="shared" ref="H3:H47" si="0">C3-B3</f>
         <v>1.1574069503694773E-5</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="9">
         <f>E3-D3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="9">
         <f t="shared" ref="J3:J12" si="1">G3-F3</f>
         <v>1.1574069503694773E-5</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="9">
         <f t="shared" ref="K3:K14" si="2">SUM(H3:J3)</f>
         <v>2.3148139007389545E-5</v>
       </c>
@@ -2943,19 +2934,19 @@
       <c r="G4" s="1">
         <v>44230.698599537034</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="9">
         <f t="shared" si="0"/>
         <v>6.9444446125999093E-5</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="9">
         <f>E4-D4</f>
         <v>3.3564814657438546E-4</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="9">
         <f t="shared" si="1"/>
         <v>9.6064814715646207E-4</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="9">
         <f t="shared" si="2"/>
         <v>1.3657407398568466E-3</v>
       </c>
@@ -2976,15 +2967,16 @@
       <c r="E5" s="1">
         <v>44230.385717592595</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="9">
         <f t="shared" si="0"/>
         <v>4.6296299842651933E-5</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="9">
         <f t="shared" ref="I5:I17" si="3">E5-D5</f>
         <v>7.638888928340748E-4</v>
       </c>
-      <c r="K5" s="4">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
         <f t="shared" si="2"/>
         <v>8.1018519267672673E-4</v>
       </c>
@@ -3011,19 +3003,19 @@
       <c r="G6" s="1">
         <v>44230.69871527778</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="9">
         <f t="shared" si="0"/>
         <v>4.6296292566694319E-5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="9">
         <f t="shared" si="3"/>
         <v>8.1018515629693866E-5</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="9">
         <f t="shared" si="1"/>
         <v>1.1574074596865103E-4</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="9">
         <f t="shared" si="2"/>
         <v>2.4305555416503921E-4</v>
       </c>
@@ -3044,15 +3036,16 @@
       <c r="E7" s="1">
         <v>44230.630671296298</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="9">
         <f t="shared" si="0"/>
         <v>5.4166666668606922E-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="9">
         <f t="shared" si="3"/>
         <v>0.24495370370277669</v>
       </c>
-      <c r="K7" s="4">
+      <c r="J7" s="9"/>
+      <c r="K7" s="9">
         <f t="shared" si="2"/>
         <v>0.29912037037138361</v>
       </c>
@@ -3079,19 +3072,19 @@
       <c r="G8" s="1">
         <v>44230.757870370369</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="9">
         <f t="shared" si="0"/>
         <v>3.4722223062999547E-5</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="9">
         <f t="shared" si="3"/>
         <v>9.1435185458976775E-4</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="9">
         <f t="shared" si="1"/>
         <v>5.9155092589207925E-2</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="9">
         <f t="shared" si="2"/>
         <v>6.0104166666860692E-2</v>
       </c>
@@ -3118,19 +3111,19 @@
       <c r="G9" s="1">
         <v>44230.758229166669</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="9">
         <f t="shared" si="0"/>
         <v>1.5046296175569296E-4</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="9">
         <f t="shared" si="3"/>
         <v>4.7453703155042604E-4</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="9">
         <f t="shared" si="1"/>
         <v>3.5879630013369024E-4</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="9">
         <f t="shared" si="2"/>
         <v>9.8379629343980923E-4</v>
       </c>
@@ -3157,19 +3150,19 @@
       <c r="G10" s="1">
         <v>44230.758483796293</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="9">
         <f t="shared" si="0"/>
         <v>6.9444446125999093E-5</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="9">
         <f t="shared" si="3"/>
         <v>1.3078703705104999E-3</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="9">
         <f t="shared" si="1"/>
         <v>2.5462962366873398E-4</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="9">
         <f t="shared" si="2"/>
         <v>1.631944440305233E-3</v>
       </c>
@@ -3196,19 +3189,19 @@
       <c r="G11" s="1">
         <v>44230.758888888886</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="9">
         <f t="shared" si="0"/>
         <v>8.101852290565148E-5</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="9">
         <f t="shared" si="3"/>
         <v>4.1666666948003694E-4</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="9">
         <f t="shared" si="1"/>
         <v>4.0509259270038456E-4</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="9">
         <f t="shared" si="2"/>
         <v>9.0277778508607298E-4</v>
       </c>
@@ -3235,19 +3228,19 @@
       <c r="G12" s="1">
         <v>44230.75990740741</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="9">
         <f t="shared" si="0"/>
         <v>9.2592592409346253E-5</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="9">
         <f t="shared" si="3"/>
         <v>4.6296296204673126E-4</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="9">
         <f t="shared" si="1"/>
         <v>1.0185185237787664E-3</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="9">
         <f t="shared" si="2"/>
         <v>1.5740740782348439E-3</v>
       </c>
@@ -3268,15 +3261,16 @@
       <c r="E13" s="1">
         <v>44230.695868055554</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="9">
         <f t="shared" si="0"/>
         <v>1.374999999825377E-2</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="9">
         <f t="shared" si="3"/>
         <v>6.5196759256650694E-2</v>
       </c>
-      <c r="K13" s="4">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9">
         <f t="shared" si="2"/>
         <v>7.8946759254904464E-2</v>
       </c>
@@ -3297,26 +3291,27 @@
       <c r="E14" s="1">
         <v>44230.697557870371</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="9">
         <f t="shared" si="0"/>
         <v>3.7037036963738501E-4</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="9">
         <f t="shared" si="3"/>
         <v>1.6898148169275373E-3</v>
       </c>
-      <c r="K14" s="4">
+      <c r="J14" s="9"/>
+      <c r="K14" s="9">
         <f t="shared" si="2"/>
         <v>2.0601851865649223E-3</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="9">
         <f>SUM(K2:K14)</f>
         <v>0.447928240741021</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B15" s="1">
         <v>44230.78392361111</v>
@@ -3325,10 +3320,10 @@
         <v>44230.792361111111</v>
       </c>
       <c r="D15" s="1">
-        <v>44213.589907407404</v>
+        <v>44234.272141203706</v>
       </c>
       <c r="E15" s="1">
-        <v>44213.616377314815</v>
+        <v>44234.311354166668</v>
       </c>
       <c r="F15" s="1">
         <v>44214.171851851854</v>
@@ -3336,26 +3331,26 @@
       <c r="G15" s="1">
         <v>44214.194409722222</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="9">
         <f t="shared" si="0"/>
         <v>8.4375000005820766E-3</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="9">
         <f t="shared" si="3"/>
-        <v>2.6469907410501037E-2</v>
-      </c>
-      <c r="J15" s="4">
+        <v>3.9212962961755693E-2</v>
+      </c>
+      <c r="J15" s="9">
         <f>G15-F15</f>
         <v>2.2557870368473232E-2</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="9">
         <f>SUM(H15:J15)</f>
-        <v>5.7465277779556345E-2</v>
+        <v>7.0208333330811001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1">
         <v>44230.78392361111</v>
@@ -3364,10 +3359,10 @@
         <v>44230.816874999997</v>
       </c>
       <c r="D16" s="1">
-        <v>44213.589907407404</v>
+        <v>44234.272141203706</v>
       </c>
       <c r="E16" s="1">
-        <v>44213.711527777778</v>
+        <v>44234.430335648147</v>
       </c>
       <c r="F16" s="1">
         <v>44214.171851851854</v>
@@ -3375,26 +3370,26 @@
       <c r="G16" s="1">
         <v>44214.298935185187</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="9">
         <f t="shared" si="0"/>
         <v>3.2951388886431232E-2</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="9">
         <f t="shared" si="3"/>
-        <v>0.12162037037342088</v>
-      </c>
-      <c r="J16" s="4">
+        <v>0.15819444444059627</v>
+      </c>
+      <c r="J16" s="9">
         <f>G16-F16</f>
         <v>0.12708333333284827</v>
       </c>
-      <c r="K16" s="4">
-        <f t="shared" ref="K16:K34" si="4">SUM(H16:J16)</f>
-        <v>0.28165509259270038</v>
+      <c r="K16" s="9">
+        <f t="shared" ref="K16:K47" si="4">SUM(H16:J16)</f>
+        <v>0.31822916665987577</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B17" s="1">
         <v>44230.78392361111</v>
@@ -3403,10 +3398,10 @@
         <v>44230.8278587963</v>
       </c>
       <c r="D17" s="1">
-        <v>44213.589907407404</v>
+        <v>44234.272141203706</v>
       </c>
       <c r="E17" s="1">
-        <v>44213.878611111111</v>
+        <v>44234.494502314818</v>
       </c>
       <c r="F17" s="1">
         <v>44215.258518518516</v>
@@ -3414,30 +3409,30 @@
       <c r="G17" s="1">
         <v>44215.6175</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="9">
         <f t="shared" si="0"/>
         <v>4.3935185189184267E-2</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="9">
         <f t="shared" si="3"/>
-        <v>0.28870370370714227</v>
-      </c>
-      <c r="J17" s="4">
+        <v>0.22236111111124046</v>
+      </c>
+      <c r="J17" s="9">
         <f>G17-F17</f>
         <v>0.35898148148407927</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="9">
         <f t="shared" si="4"/>
-        <v>0.6916203703804058</v>
+        <v>0.625277777784504</v>
       </c>
       <c r="L17" s="9">
         <f>SUM(K15:K17)</f>
-        <v>1.0307407407526625</v>
+        <v>1.0137152777751908</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1">
         <v>44230.8278587963</v>
@@ -3445,18 +3440,32 @@
       <c r="C18" s="1">
         <v>44231.01803240741</v>
       </c>
-      <c r="H18" s="4">
+      <c r="D18" s="1">
+        <v>44234.494502314818</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44235.202372685184</v>
+      </c>
+      <c r="H18" s="9">
         <f t="shared" si="0"/>
         <v>0.19017361111036735</v>
       </c>
-      <c r="K18" s="4">
+      <c r="I18" s="9">
+        <f t="shared" ref="I18:I23" si="5">E18-D18</f>
+        <v>0.70787037036643596</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" ref="J18:J23" si="6">G18-F18</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
         <f t="shared" si="4"/>
-        <v>0.19017361111036735</v>
+        <v>0.89804398147680331</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1">
         <v>44231.01803240741</v>
@@ -3464,18 +3473,32 @@
       <c r="C19" s="1">
         <v>44231.069027777776</v>
       </c>
-      <c r="H19" s="4">
+      <c r="D19" s="1">
+        <v>44235.202372685184</v>
+      </c>
+      <c r="E19" s="1">
+        <v>44235.444409722222</v>
+      </c>
+      <c r="H19" s="9">
         <f t="shared" si="0"/>
         <v>5.0995370365853887E-2</v>
       </c>
-      <c r="K19" s="4">
+      <c r="I19" s="9">
+        <f t="shared" si="5"/>
+        <v>0.24203703703824431</v>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
         <f t="shared" si="4"/>
-        <v>5.0995370365853887E-2</v>
+        <v>0.29303240740409819</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B20" s="1">
         <v>44231.069027777776</v>
@@ -3483,18 +3506,32 @@
       <c r="C20" s="1">
         <v>44231.113935185182</v>
       </c>
-      <c r="H20" s="4">
+      <c r="D20" s="1">
+        <v>44235.444409722222</v>
+      </c>
+      <c r="E20" s="1">
+        <v>44235.662881944445</v>
+      </c>
+      <c r="H20" s="9">
         <f t="shared" si="0"/>
         <v>4.4907407405844424E-2</v>
       </c>
-      <c r="K20" s="4">
+      <c r="I20" s="9">
+        <f t="shared" si="5"/>
+        <v>0.21847222222277196</v>
+      </c>
+      <c r="J20" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="9">
         <f t="shared" si="4"/>
-        <v>4.4907407405844424E-2</v>
+        <v>0.26337962962861639</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1">
         <v>44231.113935185182</v>
@@ -3502,18 +3539,32 @@
       <c r="C21" s="1">
         <v>44231.161446759259</v>
       </c>
-      <c r="H21" s="4">
+      <c r="D21" s="1">
+        <v>44235.662881944445</v>
+      </c>
+      <c r="E21" s="1">
+        <v>44235.919895833336</v>
+      </c>
+      <c r="H21" s="9">
         <f t="shared" si="0"/>
         <v>4.7511574077361729E-2</v>
       </c>
-      <c r="K21" s="4">
+      <c r="I21" s="9">
+        <f t="shared" si="5"/>
+        <v>0.25701388889137888</v>
+      </c>
+      <c r="J21" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
         <f t="shared" si="4"/>
-        <v>4.7511574077361729E-2</v>
+        <v>0.30452546296874061</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1">
         <v>44231.161446759259</v>
@@ -3521,35 +3572,63 @@
       <c r="C22" s="1">
         <v>44231.351203703707</v>
       </c>
-      <c r="H22" s="4">
+      <c r="D22" s="1">
+        <v>44238.409699074073</v>
+      </c>
+      <c r="E22" s="1">
+        <v>44239.840636574074</v>
+      </c>
+      <c r="H22" s="9">
         <f t="shared" si="0"/>
         <v>0.18975694444816327</v>
       </c>
-      <c r="K22" s="4">
+      <c r="I22" s="9">
+        <f t="shared" si="5"/>
+        <v>1.4309375000011642</v>
+      </c>
+      <c r="J22" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
         <f t="shared" si="4"/>
-        <v>0.18975694444816327</v>
+        <v>1.6206944444493274</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44231.351203703707</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44231.587175925924</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" si="0"/>
+        <v>0.23597222221724223</v>
+      </c>
+      <c r="I23" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K23" s="4">
+      <c r="J23" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="4">
+        <v>0.23597222221724223</v>
+      </c>
+      <c r="L23" s="9">
         <f>SUM(K18:K23)</f>
-        <v>0.52334490740759065</v>
+        <v>3.6156481481448282</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1">
         <v>44231.161446759259</v>
@@ -3557,18 +3636,32 @@
       <c r="C24" s="1">
         <v>44231.202291666668</v>
       </c>
-      <c r="H24" s="4">
+      <c r="D24" s="1">
+        <v>44235.919895833336</v>
+      </c>
+      <c r="E24" s="1">
+        <v>44236.098437499997</v>
+      </c>
+      <c r="H24" s="9">
         <f t="shared" si="0"/>
         <v>4.0844907409336884E-2</v>
       </c>
-      <c r="K24" s="4">
+      <c r="I24" s="9">
+        <f t="shared" ref="I24" si="7">E24-D24</f>
+        <v>0.17854166666074889</v>
+      </c>
+      <c r="J24" s="9">
+        <f t="shared" ref="J24" si="8">G24-F24</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
         <f t="shared" si="4"/>
-        <v>4.0844907409336884E-2</v>
+        <v>0.21938657407008577</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1">
         <v>44231.202291666668</v>
@@ -3576,18 +3669,32 @@
       <c r="C25" s="1">
         <v>44231.203101851854</v>
       </c>
-      <c r="H25" s="4">
+      <c r="D25" s="1">
+        <v>44236.098437499997</v>
+      </c>
+      <c r="E25" s="1">
+        <v>44236.100208333337</v>
+      </c>
+      <c r="H25" s="9">
         <f t="shared" si="0"/>
         <v>8.1018518540076911E-4</v>
       </c>
-      <c r="K25" s="4">
+      <c r="I25" s="9">
+        <f t="shared" ref="I25:I35" si="9">E25-D25</f>
+        <v>1.7708333398331888E-3</v>
+      </c>
+      <c r="J25" s="9">
+        <f t="shared" ref="J25" si="10">G25-F25</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
         <f t="shared" si="4"/>
-        <v>8.1018518540076911E-4</v>
+        <v>2.5810185252339579E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1">
         <v>44231.203101851854</v>
@@ -3595,18 +3702,29 @@
       <c r="C26" s="1">
         <v>44231.203194444446</v>
       </c>
-      <c r="H26" s="4">
+      <c r="D26" s="1">
+        <v>44237.537118055552</v>
+      </c>
+      <c r="E26" s="1">
+        <v>44237.53733796296</v>
+      </c>
+      <c r="H26" s="9">
         <f t="shared" si="0"/>
         <v>9.2592592409346253E-5</v>
       </c>
-      <c r="K26" s="4">
+      <c r="I26" s="9">
+        <f t="shared" si="9"/>
+        <v>2.1990740788169205E-4</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9">
         <f t="shared" si="4"/>
-        <v>9.2592592409346253E-5</v>
+        <v>3.125000002910383E-4</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1">
         <v>44231.203194444446</v>
@@ -3614,18 +3732,29 @@
       <c r="C27" s="1">
         <v>44231.203275462962</v>
       </c>
-      <c r="H27" s="4">
+      <c r="D27" s="1">
+        <v>44237.53733796296</v>
+      </c>
+      <c r="E27" s="1">
+        <v>44237.537534722222</v>
+      </c>
+      <c r="H27" s="9">
         <f t="shared" si="0"/>
         <v>8.1018515629693866E-5</v>
       </c>
-      <c r="K27" s="4">
+      <c r="I27" s="9">
+        <f t="shared" si="9"/>
+        <v>1.9675926159834489E-4</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9">
         <f t="shared" si="4"/>
-        <v>8.1018515629693866E-5</v>
+        <v>2.7777777722803876E-4</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1">
         <v>44231.203275462962</v>
@@ -3633,18 +3762,29 @@
       <c r="C28" s="1">
         <v>44231.203344907408</v>
       </c>
-      <c r="H28" s="4">
+      <c r="D28" s="1">
+        <v>44237.537534722222</v>
+      </c>
+      <c r="E28" s="1">
+        <v>44237.53769675926</v>
+      </c>
+      <c r="H28" s="9">
         <f t="shared" si="0"/>
         <v>6.9444446125999093E-5</v>
       </c>
-      <c r="K28" s="4">
+      <c r="I28" s="9">
+        <f t="shared" si="9"/>
+        <v>1.6203703853534535E-4</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9">
         <f t="shared" si="4"/>
-        <v>6.9444446125999093E-5</v>
+        <v>2.3148148466134444E-4</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1">
         <v>44231.203344907408</v>
@@ -3652,18 +3792,29 @@
       <c r="C29" s="1">
         <v>44231.203379629631</v>
       </c>
-      <c r="H29" s="4">
+      <c r="D29" s="1">
+        <v>44237.53769675926</v>
+      </c>
+      <c r="E29" s="1">
+        <v>44237.537766203706</v>
+      </c>
+      <c r="H29" s="9">
         <f t="shared" si="0"/>
         <v>3.4722223062999547E-5</v>
       </c>
-      <c r="K29" s="4">
+      <c r="I29" s="9">
+        <f t="shared" si="9"/>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9">
         <f t="shared" si="4"/>
-        <v>3.4722223062999547E-5</v>
+        <v>1.0416666918899864E-4</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1">
         <v>44231.203379629631</v>
@@ -3671,18 +3822,29 @@
       <c r="C30" s="1">
         <v>44231.203888888886</v>
       </c>
-      <c r="H30" s="4">
+      <c r="D30" s="1">
+        <v>44237.537766203706</v>
+      </c>
+      <c r="E30" s="1">
+        <v>44237.538761574076</v>
+      </c>
+      <c r="H30" s="9">
         <f t="shared" si="0"/>
         <v>5.0925925461342558E-4</v>
       </c>
-      <c r="K30" s="4">
+      <c r="I30" s="9">
+        <f t="shared" si="9"/>
+        <v>9.9537037021946162E-4</v>
+      </c>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9">
         <f t="shared" si="4"/>
-        <v>5.0925925461342558E-4</v>
+        <v>1.5046296248328872E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1">
         <v>44231.203888888886</v>
@@ -3690,18 +3852,29 @@
       <c r="C31" s="1">
         <v>44231.428657407407</v>
       </c>
-      <c r="H31" s="4">
+      <c r="D31" s="1">
+        <v>44237.538761574076</v>
+      </c>
+      <c r="E31" s="1">
+        <v>44238.354687500003</v>
+      </c>
+      <c r="H31" s="9">
         <f t="shared" si="0"/>
         <v>0.22476851852115942</v>
       </c>
-      <c r="K31" s="4">
+      <c r="I31" s="9">
+        <f t="shared" si="9"/>
+        <v>0.81592592592642177</v>
+      </c>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9">
         <f t="shared" si="4"/>
-        <v>0.22476851852115942</v>
+        <v>1.0406944444475812</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1">
         <v>44231.428657407407</v>
@@ -3709,18 +3882,29 @@
       <c r="C32" s="1">
         <v>44231.432928240742</v>
       </c>
-      <c r="H32" s="4">
+      <c r="D32" s="1">
+        <v>44238.354687500003</v>
+      </c>
+      <c r="E32" s="1">
+        <v>44238.361666666664</v>
+      </c>
+      <c r="H32" s="9">
         <f t="shared" si="0"/>
         <v>4.2708333348855376E-3</v>
       </c>
-      <c r="K32" s="4">
+      <c r="I32" s="9">
+        <f t="shared" si="9"/>
+        <v>6.9791666610399261E-3</v>
+      </c>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9">
         <f t="shared" si="4"/>
-        <v>4.2708333348855376E-3</v>
+        <v>1.1249999995925464E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1">
         <v>44231.432928240742</v>
@@ -3728,18 +3912,29 @@
       <c r="C33" s="1">
         <v>44231.433738425927</v>
       </c>
-      <c r="H33" s="4">
+      <c r="D33" s="1">
+        <v>44238.361666666664</v>
+      </c>
+      <c r="E33" s="1">
+        <v>44238.363553240742</v>
+      </c>
+      <c r="H33" s="9">
         <f t="shared" si="0"/>
         <v>8.1018518540076911E-4</v>
       </c>
-      <c r="K33" s="4">
+      <c r="I33" s="9">
+        <f t="shared" si="9"/>
+        <v>1.8865740785258822E-3</v>
+      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9">
         <f t="shared" si="4"/>
-        <v>8.1018518540076911E-4</v>
+        <v>2.6967592639266513E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1">
         <v>44231.433738425927</v>
@@ -3747,17 +3942,335 @@
       <c r="C34" s="1">
         <v>44231.441979166666</v>
       </c>
-      <c r="H34" s="4">
+      <c r="D34" s="1">
+        <v>44238.363553240742</v>
+      </c>
+      <c r="E34" s="1">
+        <v>44238.380069444444</v>
+      </c>
+      <c r="H34" s="9">
         <f t="shared" si="0"/>
         <v>8.2407407389837317E-3</v>
       </c>
-      <c r="K34" s="4">
+      <c r="I34" s="9">
+        <f t="shared" si="9"/>
+        <v>1.6516203701030463E-2</v>
+      </c>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9">
         <f t="shared" si="4"/>
-        <v>8.2407407389837317E-3</v>
-      </c>
-      <c r="L34" s="4">
+        <v>2.4756944440014195E-2</v>
+      </c>
+      <c r="L34" s="9">
         <f>SUM(K24:K34)</f>
-        <v>0.28053240740700858</v>
+        <v>1.3037962962989695</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44233.051840277774</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44233.459282407406</v>
+      </c>
+      <c r="H35" s="9">
+        <f t="shared" si="0"/>
+        <v>0.40744212963181781</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9">
+        <f t="shared" si="4"/>
+        <v>0.40744212963181781</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44233.459282407406</v>
+      </c>
+      <c r="C36" s="1">
+        <v>44233.462152777778</v>
+      </c>
+      <c r="H36" s="9">
+        <f t="shared" si="0"/>
+        <v>2.8703703719656914E-3</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9">
+        <f t="shared" si="4"/>
+        <v>2.8703703719656914E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44233.462152777778</v>
+      </c>
+      <c r="C37" s="1">
+        <v>44233.462731481479</v>
+      </c>
+      <c r="H37" s="9">
+        <f t="shared" si="0"/>
+        <v>5.7870370073942468E-4</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9">
+        <f t="shared" si="4"/>
+        <v>5.7870370073942468E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44233.462731481479</v>
+      </c>
+      <c r="C38" s="1">
+        <v>44233.463043981479</v>
+      </c>
+      <c r="H38" s="9">
+        <f t="shared" si="0"/>
+        <v>3.125000002910383E-4</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9">
+        <f t="shared" si="4"/>
+        <v>3.125000002910383E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44233.463043981479</v>
+      </c>
+      <c r="C39" s="1">
+        <v>44233.469293981485</v>
+      </c>
+      <c r="H39" s="9">
+        <f t="shared" si="0"/>
+        <v>6.2500000058207661E-3</v>
+      </c>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9">
+        <f t="shared" si="4"/>
+        <v>6.2500000058207661E-3</v>
+      </c>
+      <c r="L39" s="9">
+        <f>SUM(K35:K39)</f>
+        <v>0.41745370371063473</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44231.641152638891</v>
+      </c>
+      <c r="C40" s="1">
+        <v>44231.657498101849</v>
+      </c>
+      <c r="H40" s="9">
+        <f t="shared" si="0"/>
+        <v>1.6345462958270218E-2</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9">
+        <f t="shared" si="4"/>
+        <v>1.6345462958270218E-2</v>
+      </c>
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44231.641152638891</v>
+      </c>
+      <c r="C41" s="1">
+        <v>44231.652906967596</v>
+      </c>
+      <c r="H41" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1754328705137596E-2</v>
+      </c>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9">
+        <f t="shared" si="4"/>
+        <v>1.1754328705137596E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44231.641152638891</v>
+      </c>
+      <c r="C42" s="1">
+        <v>44231.641823900463</v>
+      </c>
+      <c r="H42" s="9">
+        <f t="shared" si="0"/>
+        <v>6.7126157227903605E-4</v>
+      </c>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9">
+        <f t="shared" si="4"/>
+        <v>6.7126157227903605E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44231.641152638891</v>
+      </c>
+      <c r="C43" s="1">
+        <v>44231.654508993059</v>
+      </c>
+      <c r="H43" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3356354167626705E-2</v>
+      </c>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9">
+        <f t="shared" si="4"/>
+        <v>1.3356354167626705E-2</v>
+      </c>
+      <c r="L43" s="9">
+        <f>SUM(K40:K43)</f>
+        <v>4.2127407403313555E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44231.657499305555</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44231.713870914355</v>
+      </c>
+      <c r="H44" s="9">
+        <f t="shared" si="0"/>
+        <v>5.6371608799963724E-2</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9">
+        <f t="shared" si="4"/>
+        <v>5.6371608799963724E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44231.713870914355</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44231.771314675927</v>
+      </c>
+      <c r="H45" s="9">
+        <f t="shared" si="0"/>
+        <v>5.7443761572358198E-2</v>
+      </c>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9">
+        <f t="shared" si="4"/>
+        <v>5.7443761572358198E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44231.771314675927</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44231.985181435186</v>
+      </c>
+      <c r="H46" s="9">
+        <f t="shared" si="0"/>
+        <v>0.2138667592589627</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9">
+        <f t="shared" si="4"/>
+        <v>0.2138667592589627</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44231.985181435186</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44232.056903321762</v>
+      </c>
+      <c r="H47" s="9">
+        <f t="shared" si="0"/>
+        <v>7.1721886575687677E-2</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9">
+        <f t="shared" si="4"/>
+        <v>7.1721886575687677E-2</v>
+      </c>
+      <c r="L47" s="9">
+        <f>SUM(K44:K47)</f>
+        <v>0.3994040162069723</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H48" s="9">
+        <f>SUM(H2:H47)</f>
+        <v>2.0530823495428194</v>
+      </c>
+      <c r="I48" s="9">
+        <f t="shared" ref="I48:J48" si="11">SUM(I2:I47)</f>
+        <v>4.6160185185144655</v>
+      </c>
+      <c r="J48" s="9">
+        <f t="shared" si="11"/>
+        <v>0.57097222222364508</v>
+      </c>
+      <c r="K48" s="9">
+        <f>SUM(K2:K47)</f>
+        <v>7.24007309028093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to do AHRI run
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D1C9E2-532C-4AC8-8666-CD9D20070091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B63AF6B-FFE5-46BB-9F84-F983792C9EDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
+    <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_SNOW" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
   <si>
     <t>readindividuals</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>set residency days</t>
+  </si>
+  <si>
+    <t>add individual characteristics</t>
   </si>
 </sst>
 </file>
@@ -350,7 +353,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -367,6 +370,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -686,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -698,23 +702,24 @@
     <col min="2" max="7" width="16.59765625" customWidth="1"/>
     <col min="8" max="8" width="9.3984375" customWidth="1"/>
     <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
     <col min="14" max="14" width="15.296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="13"/>
       <c r="H1" t="s">
         <v>5</v>
       </c>
@@ -1258,6 +1263,51 @@
       <c r="K16" s="2">
         <f t="shared" si="11"/>
         <v>0.37483557871746598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44241.840636574074</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44241.931319444448</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44241.802060185182</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44241.840636574074</v>
+      </c>
+      <c r="F17" s="1">
+        <v>44241.931319444448</v>
+      </c>
+      <c r="G17" s="1">
+        <v>44241.995416666665</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" ref="H17" si="14">C17-B17</f>
+        <v>9.0682870373711921E-2</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" ref="I17" si="15">E17-D17</f>
+        <v>3.8576388891669922E-2</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" ref="J17" si="16">G17-F17</f>
+        <v>6.4097222217242233E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" ref="K17" si="17">SUM(H17:J17)</f>
+        <v>0.19335648148262408</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K18" s="9">
+        <f>SUM(K2:K17)</f>
+        <v>0.89451276621548459</v>
       </c>
     </row>
   </sheetData>
@@ -1813,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87CE502-9FA2-453D-9130-46B0AFC0874E}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1825,25 +1875,22 @@
     <col min="2" max="2" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.19921875" customWidth="1"/>
     <col min="4" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="13"/>
       <c r="H1" t="s">
         <v>6</v>
       </c>
@@ -2775,6 +2822,42 @@
       <c r="L34" s="4">
         <f>SUM(K24:K34)</f>
         <v>0.16984953703649808</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H35" s="9">
+        <f>SUM(H2:H34)</f>
+        <v>0.78800925926043419</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" ref="I35:K35" si="12">SUM(I2:I34)</f>
+        <v>0.85601851852698019</v>
+      </c>
+      <c r="J35" s="9">
+        <f t="shared" si="12"/>
+        <v>0.54545138889079681</v>
+      </c>
+      <c r="K35" s="9">
+        <f t="shared" si="12"/>
+        <v>2.1894791666782112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H36" s="12">
+        <f>Pentaho_CHPC!H48/Pentaho_SNOW!H35</f>
+        <v>2.6054038393783432</v>
+      </c>
+      <c r="I36" s="12">
+        <f>Pentaho_CHPC!I48/Pentaho_SNOW!I35</f>
+        <v>7.8015819361078131</v>
+      </c>
+      <c r="J36" s="12">
+        <f>Pentaho_CHPC!J48/Pentaho_SNOW!J35</f>
+        <v>1.0467884652099726</v>
+      </c>
+      <c r="K36" s="12">
+        <f>Pentaho_CHPC!K48/Pentaho_SNOW!K35</f>
+        <v>4.2486602861782314</v>
       </c>
     </row>
   </sheetData>
@@ -2792,8 +2875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373E5D0C-070B-4F8C-A080-FA6C8B658209}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K48"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2809,18 +2892,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
@@ -3605,13 +3688,19 @@
       <c r="C23" s="1">
         <v>44231.587175925924</v>
       </c>
+      <c r="D23" s="1">
+        <v>44239.840636574074</v>
+      </c>
+      <c r="E23" s="1">
+        <v>44241.123993055553</v>
+      </c>
       <c r="H23" s="9">
         <f t="shared" si="0"/>
         <v>0.23597222221724223</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.2833564814791316</v>
       </c>
       <c r="J23" s="9">
         <f t="shared" si="6"/>
@@ -3619,11 +3708,11 @@
       </c>
       <c r="K23" s="9">
         <f t="shared" si="4"/>
-        <v>0.23597222221724223</v>
+        <v>1.5193287036963739</v>
       </c>
       <c r="L23" s="9">
         <f>SUM(K18:K23)</f>
-        <v>3.6156481481448282</v>
+        <v>4.8990046296239598</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -3680,7 +3769,7 @@
         <v>8.1018518540076911E-4</v>
       </c>
       <c r="I25" s="9">
-        <f t="shared" ref="I25:I35" si="9">E25-D25</f>
+        <f t="shared" ref="I25:I47" si="9">E25-D25</f>
         <v>1.7708333398331888E-3</v>
       </c>
       <c r="J25" s="9">
@@ -4004,7 +4093,10 @@
         <f t="shared" si="0"/>
         <v>2.8703703719656914E-3</v>
       </c>
-      <c r="I36" s="9"/>
+      <c r="I36" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9">
         <f t="shared" si="4"/>
@@ -4025,7 +4117,10 @@
         <f t="shared" si="0"/>
         <v>5.7870370073942468E-4</v>
       </c>
-      <c r="I37" s="9"/>
+      <c r="I37" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9">
         <f t="shared" si="4"/>
@@ -4046,7 +4141,10 @@
         <f t="shared" si="0"/>
         <v>3.125000002910383E-4</v>
       </c>
-      <c r="I38" s="9"/>
+      <c r="I38" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9">
         <f t="shared" si="4"/>
@@ -4067,7 +4165,10 @@
         <f t="shared" si="0"/>
         <v>6.2500000058207661E-3</v>
       </c>
-      <c r="I39" s="9"/>
+      <c r="I39" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="J39" s="9"/>
       <c r="K39" s="9">
         <f t="shared" si="4"/>
@@ -4088,15 +4189,24 @@
       <c r="C40" s="1">
         <v>44231.657498101849</v>
       </c>
+      <c r="D40" s="1">
+        <v>44241.123993055553</v>
+      </c>
+      <c r="E40" s="1">
+        <v>44241.184386574074</v>
+      </c>
       <c r="H40" s="9">
         <f t="shared" si="0"/>
         <v>1.6345462958270218E-2</v>
       </c>
-      <c r="I40" s="9"/>
+      <c r="I40" s="9">
+        <f t="shared" si="9"/>
+        <v>6.0393518520868383E-2</v>
+      </c>
       <c r="J40" s="9"/>
       <c r="K40" s="9">
         <f t="shared" si="4"/>
-        <v>1.6345462958270218E-2</v>
+        <v>7.6738981479138602E-2</v>
       </c>
       <c r="L40" s="4"/>
     </row>
@@ -4110,15 +4220,24 @@
       <c r="C41" s="1">
         <v>44231.652906967596</v>
       </c>
+      <c r="D41" s="1">
+        <v>44241.123993055553</v>
+      </c>
+      <c r="E41" s="1">
+        <v>44241.187175925923</v>
+      </c>
       <c r="H41" s="9">
         <f t="shared" si="0"/>
         <v>1.1754328705137596E-2</v>
       </c>
-      <c r="I41" s="9"/>
+      <c r="I41" s="9">
+        <f t="shared" si="9"/>
+        <v>6.3182870369928423E-2</v>
+      </c>
       <c r="J41" s="9"/>
       <c r="K41" s="9">
         <f t="shared" si="4"/>
-        <v>1.1754328705137596E-2</v>
+        <v>7.4937199075066019E-2</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -4131,15 +4250,24 @@
       <c r="C42" s="1">
         <v>44231.641823900463</v>
       </c>
+      <c r="D42" s="1">
+        <v>44241.123993055553</v>
+      </c>
+      <c r="E42" s="1">
+        <v>44241.135844907411</v>
+      </c>
       <c r="H42" s="9">
         <f t="shared" si="0"/>
         <v>6.7126157227903605E-4</v>
       </c>
-      <c r="I42" s="9"/>
+      <c r="I42" s="9">
+        <f t="shared" si="9"/>
+        <v>1.1851851857500151E-2</v>
+      </c>
       <c r="J42" s="9"/>
       <c r="K42" s="9">
         <f t="shared" si="4"/>
-        <v>6.7126157227903605E-4</v>
+        <v>1.2523113429779187E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -4152,19 +4280,28 @@
       <c r="C43" s="1">
         <v>44231.654508993059</v>
       </c>
+      <c r="D43" s="1">
+        <v>44241.123993055553</v>
+      </c>
+      <c r="E43" s="1">
+        <v>44241.202187499999</v>
+      </c>
       <c r="H43" s="9">
         <f t="shared" si="0"/>
         <v>1.3356354167626705E-2</v>
       </c>
-      <c r="I43" s="9"/>
+      <c r="I43" s="9">
+        <f t="shared" si="9"/>
+        <v>7.8194444446125999E-2</v>
+      </c>
       <c r="J43" s="9"/>
       <c r="K43" s="9">
         <f t="shared" si="4"/>
-        <v>1.3356354167626705E-2</v>
+        <v>9.1550798613752704E-2</v>
       </c>
       <c r="L43" s="9">
         <f>SUM(K40:K43)</f>
-        <v>4.2127407403313555E-2</v>
+        <v>0.25575009259773651</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -4177,15 +4314,24 @@
       <c r="C44" s="1">
         <v>44231.713870914355</v>
       </c>
+      <c r="D44" s="1">
+        <v>44241.202187499999</v>
+      </c>
+      <c r="E44" s="1">
+        <v>44241.474895833337</v>
+      </c>
       <c r="H44" s="9">
         <f t="shared" si="0"/>
         <v>5.6371608799963724E-2</v>
       </c>
-      <c r="I44" s="9"/>
+      <c r="I44" s="9">
+        <f t="shared" si="9"/>
+        <v>0.27270833333750488</v>
+      </c>
       <c r="J44" s="9"/>
       <c r="K44" s="9">
         <f t="shared" si="4"/>
-        <v>5.6371608799963724E-2</v>
+        <v>0.32907994213746861</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -4198,15 +4344,24 @@
       <c r="C45" s="1">
         <v>44231.771314675927</v>
       </c>
+      <c r="D45" s="1">
+        <v>44241.474895833337</v>
+      </c>
+      <c r="E45" s="1">
+        <v>44241.767488425925</v>
+      </c>
       <c r="H45" s="9">
         <f t="shared" si="0"/>
         <v>5.7443761572358198E-2</v>
       </c>
-      <c r="I45" s="9"/>
+      <c r="I45" s="9">
+        <f t="shared" si="9"/>
+        <v>0.29259259258833481</v>
+      </c>
       <c r="J45" s="9"/>
       <c r="K45" s="9">
         <f t="shared" si="4"/>
-        <v>5.7443761572358198E-2</v>
+        <v>0.35003635416069301</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -4223,7 +4378,10 @@
         <f t="shared" si="0"/>
         <v>0.2138667592589627</v>
       </c>
-      <c r="I46" s="9"/>
+      <c r="I46" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9">
         <f t="shared" si="4"/>
@@ -4244,7 +4402,10 @@
         <f t="shared" si="0"/>
         <v>7.1721886575687677E-2</v>
       </c>
-      <c r="I47" s="9"/>
+      <c r="I47" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="J47" s="9"/>
       <c r="K47" s="9">
         <f t="shared" si="4"/>
@@ -4252,7 +4413,7 @@
       </c>
       <c r="L47" s="9">
         <f>SUM(K44:K47)</f>
-        <v>0.3994040162069723</v>
+        <v>0.96470494213281199</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -4262,7 +4423,7 @@
       </c>
       <c r="I48" s="9">
         <f t="shared" ref="I48:J48" si="11">SUM(I2:I47)</f>
-        <v>4.6160185185144655</v>
+        <v>6.6782986111138598</v>
       </c>
       <c r="J48" s="9">
         <f t="shared" si="11"/>
@@ -4270,7 +4431,7 @@
       </c>
       <c r="K48" s="9">
         <f>SUM(K2:K47)</f>
-        <v>7.24007309028093</v>
+        <v>9.3023531828803243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AHRI run from start to add individual characteristics
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B63AF6B-FFE5-46BB-9F84-F983792C9EDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048C3EED-3480-42D7-8080-D2468CD8794C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
@@ -693,15 +693,14 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="16.59765625" customWidth="1"/>
-    <col min="8" max="8" width="9.3984375" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
     <col min="14" max="14" width="15.296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
@@ -740,13 +739,24 @@
       <c r="C2" s="1">
         <v>44213.747488425928</v>
       </c>
+      <c r="F2" s="1">
+        <v>44248.27752314815</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44248.27789351852</v>
+      </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H11" si="0">C2-B2</f>
         <v>4.398148157633841E-4</v>
       </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <f>G2-F2</f>
+        <v>3.7037036963738501E-4</v>
+      </c>
       <c r="K2" s="2">
         <f>SUM(H2:J2)</f>
-        <v>4.398148157633841E-4</v>
+        <v>8.1018518540076911E-4</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -759,13 +769,23 @@
       <c r="C3" s="1">
         <v>44213.747523148151</v>
       </c>
+      <c r="F3" s="1">
+        <v>44248.27789351852</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44248.277928240743</v>
+      </c>
       <c r="H3" s="2">
         <f t="shared" si="0"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="J3" s="2">
+        <f>G3-F3</f>
         <v>3.4722223062999547E-5</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" ref="K3:K11" si="1">SUM(H3:J3)</f>
-        <v>3.4722223062999547E-5</v>
+        <v>6.9444446125999093E-5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -783,9 +803,11 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <v>44213.753449074073</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>44248.277928240743</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44248.278148148151</v>
+      </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
         <v>4.8726851819083095E-3</v>
@@ -795,12 +817,12 @@
         <v>7.8703703911742195E-4</v>
       </c>
       <c r="J4" s="2">
-        <f>F4-D4</f>
-        <v>2.6620370044838637E-4</v>
+        <f>G4-F4</f>
+        <v>2.1990740788169205E-4</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="1"/>
-        <v>5.9259259214741178E-3</v>
+        <v>5.8796296289074235E-3</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -813,13 +835,23 @@
       <c r="C5" s="1">
         <v>44213.753645833334</v>
       </c>
+      <c r="F5" s="1">
+        <v>44248.278148148151</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44248.278275462966</v>
+      </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
         <v>1.9675926159834489E-4</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" ref="J5:J17" si="2">G5-F5</f>
+        <v>1.273148154723458E-4</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="1"/>
-        <v>1.9675926159834489E-4</v>
+        <v>3.2407407707069069E-4</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -832,13 +864,23 @@
       <c r="C6" s="1">
         <v>44213.753912037035</v>
       </c>
+      <c r="F6" s="1">
+        <v>44248.278275462966</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44248.278402777774</v>
+      </c>
       <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>2.6620370044838637E-4</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2731480819638819E-4</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="1"/>
-        <v>2.6620370044838637E-4</v>
+        <v>3.9351850864477456E-4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -856,9 +898,11 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>44213.803611111114</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>44248.278402777774</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44248.301840277774</v>
+      </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>2.1122685189766344E-2</v>
@@ -868,7 +912,7 @@
         <v>5.1388888896326534E-3</v>
       </c>
       <c r="J7" s="2">
-        <f>F7-D7</f>
+        <f t="shared" si="2"/>
         <v>2.34375E-2</v>
       </c>
       <c r="K7" s="2">
@@ -902,24 +946,26 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <v>44213.804085648146</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>44248.301840277774</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44248.302141203705</v>
+      </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>1.2731480819638819E-4</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" ref="I8" si="2">D8-C8</f>
+        <f t="shared" ref="I8" si="3">D8-C8</f>
         <v>3.4722223062999547E-5</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" ref="J8" si="3">F8-D8</f>
-        <v>3.125000002910383E-4</v>
+        <f t="shared" si="2"/>
+        <v>3.0092593078734353E-4</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>4.7453703155042604E-4</v>
+        <v>4.6296296204673126E-4</v>
       </c>
       <c r="M8">
         <v>427</v>
@@ -948,9 +994,11 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
-        <v>44213.804386574076</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>44248.302141203705</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44248.302349537036</v>
+      </c>
       <c r="H9" s="2">
         <f t="shared" si="0"/>
         <v>2.4305556144099683E-4</v>
@@ -960,12 +1008,12 @@
         <v>1.1574069503694773E-5</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" ref="J9" si="5">F9-D9</f>
-        <v>4.6296299842651933E-5</v>
+        <f t="shared" si="2"/>
+        <v>2.0833333110203966E-4</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>3.0092593078734353E-4</v>
+        <v>4.6296296204673126E-4</v>
       </c>
       <c r="M9">
         <v>1781</v>
@@ -994,19 +1042,21 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
-        <v>44213.804664351854</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>44248.302349537036</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44248.302499999998</v>
+      </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>1.0416666191304103E-4</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" ref="I10:I11" si="6">D10-C10</f>
+        <f t="shared" ref="I10:I11" si="5">D10-C10</f>
         <v>2.3148153559304774E-5</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" ref="J10:J11" si="7">F10-D10</f>
+        <f t="shared" si="2"/>
         <v>1.5046296175569296E-4</v>
       </c>
       <c r="K10" s="2">
@@ -1044,28 +1094,30 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
-        <v>44213.805347222224</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>44248.302499999998</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44248.302905092591</v>
+      </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
         <v>1.7361110803904012E-4</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4.6296299842651933E-5</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="7"/>
-        <v>4.6296296204673126E-4</v>
+        <f t="shared" si="2"/>
+        <v>4.0509259270038456E-4</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>6.8287036992842332E-4</v>
+        <v>6.2500000058207661E-4</v>
       </c>
       <c r="L11" s="2">
         <f>SUM(K2:K11)</f>
-        <v>5.8298611111240461E-2</v>
+        <v>5.9004629627452232E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1083,24 +1135,26 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
-        <v>44213.808831018519</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>44248.302905092591</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44248.308738425927</v>
+      </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H12:H16" si="8">C12-B12</f>
+        <f t="shared" ref="H12:H16" si="6">C12-B12</f>
         <v>1.7245370327145793E-3</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" ref="I12:I14" si="9">D12-C12</f>
+        <f t="shared" ref="I12:I14" si="7">D12-C12</f>
         <v>4.8611111560603604E-4</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" ref="J12:J14" si="10">F12-D12</f>
-        <v>1.2731481474475004E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.8333333363407291E-3</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" ref="K12:K16" si="11">SUM(H12:J12)</f>
-        <v>3.4837962957681157E-3</v>
+        <f t="shared" ref="K12:K16" si="8">SUM(H12:J12)</f>
+        <v>8.0439814846613444E-3</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1118,24 +1172,26 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
-        <v>44215.503263888888</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>44248.308738425927</v>
+      </c>
+      <c r="G13" s="1">
+        <v>44248.30909722222</v>
+      </c>
       <c r="H13" s="2">
+        <f t="shared" si="6"/>
+        <v>6.2500000058207661E-4</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1574073869269341E-4</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="2"/>
+        <v>3.5879629285773262E-4</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="8"/>
-        <v>6.2500000058207661E-4</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="9"/>
-        <v>1.1574073869269341E-4</v>
-      </c>
-      <c r="J13" s="2">
-        <f t="shared" si="10"/>
-        <v>3.819444464170374E-4</v>
-      </c>
-      <c r="K13" s="2">
-        <f t="shared" si="11"/>
-        <v>1.1226851856918074E-3</v>
+        <v>1.0995370321325026E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -1153,28 +1209,30 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
-        <v>44213.814786192132</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>44248.30909722222</v>
+      </c>
+      <c r="G14" s="1">
+        <v>44248.322638333331</v>
+      </c>
       <c r="H14" s="2">
+        <f t="shared" si="6"/>
+        <v>2.4305555562023073E-3</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="7"/>
+        <v>4.9768518510973081E-4</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="2"/>
+        <v>1.35411111114081E-2</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="8"/>
-        <v>2.4305555562023073E-3</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="9"/>
-        <v>4.9768518510973081E-4</v>
-      </c>
-      <c r="J14" s="2">
-        <f t="shared" si="10"/>
-        <v>2.1820254623889923E-3</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" si="11"/>
-        <v>5.1102662037010305E-3</v>
+        <v>1.6469351852720138E-2</v>
       </c>
       <c r="L14" s="2">
         <f>SUM(K12:K14)</f>
-        <v>9.7167476851609536E-3</v>
+        <v>2.5612870369513985E-2</v>
       </c>
       <c r="N14" s="11">
         <v>804812006</v>
@@ -1204,26 +1262,26 @@
         <v>44231.486522939813</v>
       </c>
       <c r="F15" s="1">
-        <v>44231.486516203702</v>
+        <v>44248.322638333331</v>
       </c>
       <c r="G15" s="1">
-        <v>44231.58798611111</v>
+        <v>44248.464386574073</v>
       </c>
       <c r="H15" s="2">
+        <f t="shared" si="6"/>
+        <v>0.13476851851737592</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" ref="I15:I16" si="9">E15-D15</f>
+        <v>2.2066921294026542E-2</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14174824074143544</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="8"/>
-        <v>0.13476851851737592</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" ref="I15:I16" si="12">E15-D15</f>
-        <v>2.2066921294026542E-2</v>
-      </c>
-      <c r="J15" s="2">
-        <f t="shared" ref="J15:J16" si="13">G15-F15</f>
-        <v>0.10146990740759065</v>
-      </c>
-      <c r="K15" s="2">
-        <f t="shared" si="11"/>
-        <v>0.25830534721899312</v>
+        <v>0.2985836805528379</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -1243,26 +1301,26 @@
         <v>44240.357453067132</v>
       </c>
       <c r="F16" s="1">
-        <v>44240.719837962963</v>
+        <v>44248.464386574073</v>
       </c>
       <c r="G16" s="1">
-        <v>44240.869258645835</v>
+        <v>44248.623757094909</v>
       </c>
       <c r="H16" s="2">
+        <f t="shared" si="6"/>
+        <v>0.18801781250658678</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="9"/>
+        <v>3.7397083338873927E-2</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1593705208360916</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="8"/>
-        <v>0.18801781250658678</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="12"/>
-        <v>3.7397083338873927E-2</v>
-      </c>
-      <c r="J16" s="2">
-        <f t="shared" si="13"/>
-        <v>0.14942068287200527</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" si="11"/>
-        <v>0.37483557871746598</v>
+        <v>0.38478541668155231</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1282,32 +1340,44 @@
         <v>44241.840636574074</v>
       </c>
       <c r="F17" s="1">
-        <v>44241.931319444448</v>
+        <v>44248.623749999999</v>
       </c>
       <c r="G17" s="1">
-        <v>44241.995416666665</v>
+        <v>44248.688449074078</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17" si="14">C17-B17</f>
+        <f t="shared" ref="H17" si="10">C17-B17</f>
         <v>9.0682870373711921E-2</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" ref="I17" si="15">E17-D17</f>
+        <f t="shared" ref="I17" si="11">E17-D17</f>
         <v>3.8576388891669922E-2</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" ref="J17" si="16">G17-F17</f>
-        <v>6.4097222217242233E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.4699074078816921E-2</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ref="K17" si="17">SUM(H17:J17)</f>
-        <v>0.19335648148262408</v>
+        <f t="shared" ref="K17" si="12">SUM(H17:J17)</f>
+        <v>0.19395833334419876</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H18" s="9">
+        <f>SUM(H2:H17)</f>
+        <v>0.44583031249931082</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="shared" ref="I18:J18" si="13">SUM(I2:I17)</f>
+        <v>0.10518159723869758</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="13"/>
+        <v>0.41093302083754679</v>
+      </c>
       <c r="K18" s="9">
         <f>SUM(K2:K17)</f>
-        <v>0.89451276621548459</v>
+        <v>0.96194493057555519</v>
       </c>
     </row>
   </sheetData>
@@ -1323,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751965E-4A3A-442F-9C21-79FCCBFBF505}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1336,7 +1406,7 @@
     <col min="4" max="4" width="16.19921875" customWidth="1"/>
     <col min="5" max="6" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1853,6 +1923,12 @@
       <c r="J19" s="2">
         <f t="shared" si="23"/>
         <v>-44215.423657407409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G20" s="2">
+        <f>SUM(G2:G19)</f>
+        <v>0.32274305557803018</v>
       </c>
     </row>
   </sheetData>
@@ -2849,15 +2925,15 @@
       </c>
       <c r="I36" s="12">
         <f>Pentaho_CHPC!I48/Pentaho_SNOW!I35</f>
-        <v>7.8015819361078131</v>
+        <v>11.086073553162466</v>
       </c>
       <c r="J36" s="12">
         <f>Pentaho_CHPC!J48/Pentaho_SNOW!J35</f>
-        <v>1.0467884652099726</v>
+        <v>0.82867570606700247</v>
       </c>
       <c r="K36" s="12">
         <f>Pentaho_CHPC!K48/Pentaho_SNOW!K35</f>
-        <v>4.2486602861782314</v>
+        <v>5.4784576652604908</v>
       </c>
     </row>
   </sheetData>
@@ -2873,10 +2949,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373E5D0C-070B-4F8C-A080-FA6C8B658209}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2889,6 +2965,7 @@
     <col min="10" max="10" width="11.3984375" customWidth="1"/>
     <col min="11" max="11" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.296875" customWidth="1"/>
+    <col min="13" max="14" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -2987,7 +3064,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="9">
-        <f t="shared" ref="J3:J12" si="1">G3-F3</f>
+        <f t="shared" ref="J3:J13" si="1">G3-F3</f>
         <v>1.1574069503694773E-5</v>
       </c>
       <c r="K3" s="9">
@@ -3228,10 +3305,10 @@
         <v>44230.388495370367</v>
       </c>
       <c r="F10" s="1">
-        <v>44230.758229166669</v>
+        <v>44248.469722222224</v>
       </c>
       <c r="G10" s="1">
-        <v>44230.758483796293</v>
+        <v>44248.470057870371</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
@@ -3243,11 +3320,11 @@
       </c>
       <c r="J10" s="9">
         <f t="shared" si="1"/>
-        <v>2.5462962366873398E-4</v>
+        <v>3.3564814657438546E-4</v>
       </c>
       <c r="K10" s="9">
         <f t="shared" si="2"/>
-        <v>1.631944440305233E-3</v>
+        <v>1.7129629632108845E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -3267,10 +3344,10 @@
         <v>44230.388912037037</v>
       </c>
       <c r="F11" s="1">
-        <v>44230.758483796293</v>
+        <v>44248.470057870371</v>
       </c>
       <c r="G11" s="1">
-        <v>44230.758888888886</v>
+        <v>44248.470335648148</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" si="0"/>
@@ -3282,11 +3359,11 @@
       </c>
       <c r="J11" s="9">
         <f t="shared" si="1"/>
-        <v>4.0509259270038456E-4</v>
+        <v>2.7777777722803876E-4</v>
       </c>
       <c r="K11" s="9">
         <f t="shared" si="2"/>
-        <v>9.0277778508607298E-4</v>
+        <v>7.7546296961372718E-4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -3306,10 +3383,10 @@
         <v>44230.389374999999</v>
       </c>
       <c r="F12" s="1">
-        <v>44230.758888888886</v>
+        <v>44248.470335648148</v>
       </c>
       <c r="G12" s="1">
-        <v>44230.75990740741</v>
+        <v>44248.470902777779</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
@@ -3321,11 +3398,11 @@
       </c>
       <c r="J12" s="9">
         <f t="shared" si="1"/>
-        <v>1.0185185237787664E-3</v>
+        <v>5.671296312357299E-4</v>
       </c>
       <c r="K12" s="9">
         <f t="shared" si="2"/>
-        <v>1.5740740782348439E-3</v>
+        <v>1.1226851856918074E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -3344,6 +3421,12 @@
       <c r="E13" s="1">
         <v>44230.695868055554</v>
       </c>
+      <c r="F13" s="1">
+        <v>44248.470902777779</v>
+      </c>
+      <c r="G13" s="1">
+        <v>44248.472129629627</v>
+      </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
         <v>1.374999999825377E-2</v>
@@ -3352,10 +3435,13 @@
         <f t="shared" si="3"/>
         <v>6.5196759256650694E-2</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="9">
+        <f t="shared" si="1"/>
+        <v>1.2268518476048484E-3</v>
+      </c>
       <c r="K13" s="9">
         <f t="shared" si="2"/>
-        <v>7.8946759254904464E-2</v>
+        <v>8.0173611102509312E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -3389,7 +3475,7 @@
       </c>
       <c r="L14" s="9">
         <f>SUM(K2:K14)</f>
-        <v>0.447928240741021</v>
+        <v>0.44865740740351612</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -3409,10 +3495,10 @@
         <v>44234.311354166668</v>
       </c>
       <c r="F15" s="1">
-        <v>44214.171851851854</v>
+        <v>44248.475312499999</v>
       </c>
       <c r="G15" s="1">
-        <v>44214.194409722222</v>
+        <v>44248.500347222223</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" si="0"/>
@@ -3424,11 +3510,11 @@
       </c>
       <c r="J15" s="9">
         <f>G15-F15</f>
-        <v>2.2557870368473232E-2</v>
+        <v>2.5034722224518191E-2</v>
       </c>
       <c r="K15" s="9">
         <f>SUM(H15:J15)</f>
-        <v>7.0208333330811001E-2</v>
+        <v>7.2685185186855961E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -3448,10 +3534,10 @@
         <v>44234.430335648147</v>
       </c>
       <c r="F16" s="1">
-        <v>44214.171851851854</v>
+        <v>44248.475312499999</v>
       </c>
       <c r="G16" s="1">
-        <v>44214.298935185187</v>
+        <v>44248.595509259256</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="0"/>
@@ -3463,14 +3549,14 @@
       </c>
       <c r="J16" s="9">
         <f>G16-F16</f>
-        <v>0.12708333333284827</v>
+        <v>0.12019675925694173</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" ref="K16:K47" si="4">SUM(H16:J16)</f>
-        <v>0.31822916665987577</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K16:K17" si="4">SUM(H16:J16)</f>
+        <v>0.31134259258396924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -3487,10 +3573,10 @@
         <v>44234.494502314818</v>
       </c>
       <c r="F17" s="1">
-        <v>44215.258518518516</v>
+        <v>44248.475312499999</v>
       </c>
       <c r="G17" s="1">
-        <v>44215.6175</v>
+        <v>44248.719004629631</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" si="0"/>
@@ -3502,18 +3588,18 @@
       </c>
       <c r="J17" s="9">
         <f>G17-F17</f>
-        <v>0.35898148148407927</v>
+        <v>0.24369212963210884</v>
       </c>
       <c r="K17" s="9">
         <f t="shared" si="4"/>
-        <v>0.625277777784504</v>
+        <v>0.50998842593253357</v>
       </c>
       <c r="L17" s="9">
         <f>SUM(K15:K17)</f>
-        <v>1.0137152777751908</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.89401620370335877</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -3542,11 +3628,11 @@
         <v>0</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K16:K47" si="7">SUM(H18:J18)</f>
         <v>0.89804398147680331</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -3575,11 +3661,11 @@
         <v>0</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.29303240740409819</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -3608,11 +3694,11 @@
         <v>0</v>
       </c>
       <c r="K20" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.26337962962861639</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -3641,11 +3727,19 @@
         <v>0</v>
       </c>
       <c r="K21" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.30452546296874061</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="9">
+        <f>SUM(H2:H21)</f>
+        <v>0.48783564814948477</v>
+      </c>
+      <c r="N21" s="9">
+        <f>SUM(I2:I21)</f>
+        <v>2.1618171296213404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3674,11 +3768,11 @@
         <v>0</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.6206944444493274</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -3707,7 +3801,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.5193287036963739</v>
       </c>
       <c r="L23" s="9">
@@ -3715,7 +3809,7 @@
         <v>4.8990046296239598</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -3736,19 +3830,19 @@
         <v>4.0844907409336884E-2</v>
       </c>
       <c r="I24" s="9">
-        <f t="shared" ref="I24" si="7">E24-D24</f>
+        <f t="shared" ref="I24" si="8">E24-D24</f>
         <v>0.17854166666074889</v>
       </c>
       <c r="J24" s="9">
-        <f t="shared" ref="J24" si="8">G24-F24</f>
+        <f t="shared" ref="J24" si="9">G24-F24</f>
         <v>0</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.21938657407008577</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -3769,19 +3863,19 @@
         <v>8.1018518540076911E-4</v>
       </c>
       <c r="I25" s="9">
-        <f t="shared" ref="I25:I47" si="9">E25-D25</f>
+        <f t="shared" ref="I25:I47" si="10">E25-D25</f>
         <v>1.7708333398331888E-3</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" ref="J25" si="10">G25-F25</f>
+        <f t="shared" ref="J25" si="11">G25-F25</f>
         <v>0</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.5810185252339579E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -3802,16 +3896,16 @@
         <v>9.2592592409346253E-5</v>
       </c>
       <c r="I26" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.1990740788169205E-4</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.125000002910383E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -3832,16 +3926,16 @@
         <v>8.1018515629693866E-5</v>
       </c>
       <c r="I27" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.9675926159834489E-4</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.7777777722803876E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -3862,16 +3956,16 @@
         <v>6.9444446125999093E-5</v>
       </c>
       <c r="I28" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6203703853534535E-4</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.3148148466134444E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -3892,16 +3986,16 @@
         <v>3.4722223062999547E-5</v>
       </c>
       <c r="I29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.9444446125999093E-5</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.0416666918899864E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -3922,16 +4016,20 @@
         <v>5.0925925461342558E-4</v>
       </c>
       <c r="I30" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.9537037021946162E-4</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.5046296248328872E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L30" s="9">
+        <f>SUM(K24:K30)</f>
+        <v>0.22439814815152204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -3952,16 +4050,16 @@
         <v>0.22476851852115942</v>
       </c>
       <c r="I31" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.81592592592642177</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.0406944444475812</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -3982,12 +4080,12 @@
         <v>4.2708333348855376E-3</v>
       </c>
       <c r="I32" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.9791666610399261E-3</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.1249999995925464E-2</v>
       </c>
     </row>
@@ -4012,12 +4110,12 @@
         <v>8.1018518540076911E-4</v>
       </c>
       <c r="I33" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.8865740785258822E-3</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.6967592639266513E-3</v>
       </c>
     </row>
@@ -4042,17 +4140,17 @@
         <v>8.2407407389837317E-3</v>
       </c>
       <c r="I34" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6516203701030463E-2</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.4756944440014195E-2</v>
       </c>
       <c r="L34" s="9">
-        <f>SUM(K24:K34)</f>
-        <v>1.3037962962989695</v>
+        <f>SUM(K31:K34)</f>
+        <v>1.0793981481474475</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -4065,18 +4163,24 @@
       <c r="C35" s="1">
         <v>44233.459282407406</v>
       </c>
+      <c r="D35" s="1">
+        <v>44245.133668981478</v>
+      </c>
+      <c r="E35" s="1">
+        <v>44246.082511574074</v>
+      </c>
       <c r="H35" s="9">
         <f t="shared" si="0"/>
         <v>0.40744212963181781</v>
       </c>
       <c r="I35" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>0.94884259259561077</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9">
-        <f t="shared" si="4"/>
-        <v>0.40744212963181781</v>
+        <f t="shared" si="7"/>
+        <v>1.3562847222274286</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -4089,18 +4193,24 @@
       <c r="C36" s="1">
         <v>44233.462152777778</v>
       </c>
+      <c r="D36" s="1">
+        <v>44246.082511574074</v>
+      </c>
+      <c r="E36" s="1">
+        <v>44246.091238425928</v>
+      </c>
       <c r="H36" s="9">
         <f t="shared" si="0"/>
         <v>2.8703703719656914E-3</v>
       </c>
       <c r="I36" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>8.7268518545897678E-3</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9">
-        <f t="shared" si="4"/>
-        <v>2.8703703719656914E-3</v>
+        <f t="shared" si="7"/>
+        <v>1.1597222226555459E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -4113,18 +4223,24 @@
       <c r="C37" s="1">
         <v>44233.462731481479</v>
       </c>
+      <c r="D37" s="1">
+        <v>44246.091238425928</v>
+      </c>
+      <c r="E37" s="1">
+        <v>44246.094328703701</v>
+      </c>
       <c r="H37" s="9">
         <f t="shared" si="0"/>
         <v>5.7870370073942468E-4</v>
       </c>
       <c r="I37" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.0902777725714259E-3</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9">
-        <f t="shared" si="4"/>
-        <v>5.7870370073942468E-4</v>
+        <f t="shared" si="7"/>
+        <v>3.6689814733108506E-3</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -4137,18 +4253,24 @@
       <c r="C38" s="1">
         <v>44233.463043981479</v>
       </c>
+      <c r="D38" s="1">
+        <v>44246.094328703701</v>
+      </c>
+      <c r="E38" s="1">
+        <v>44246.096168981479</v>
+      </c>
       <c r="H38" s="9">
         <f t="shared" si="0"/>
         <v>3.125000002910383E-4</v>
       </c>
       <c r="I38" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1.8402777786832303E-3</v>
       </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9">
-        <f t="shared" si="4"/>
-        <v>3.125000002910383E-4</v>
+        <f t="shared" si="7"/>
+        <v>2.1527777789742686E-3</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -4161,22 +4283,28 @@
       <c r="C39" s="1">
         <v>44233.469293981485</v>
       </c>
+      <c r="D39" s="1">
+        <v>44246.096168981479</v>
+      </c>
+      <c r="E39" s="1">
+        <v>44246.127210648148</v>
+      </c>
       <c r="H39" s="9">
         <f t="shared" si="0"/>
         <v>6.2500000058207661E-3</v>
       </c>
       <c r="I39" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>3.104166666889796E-2</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="9">
-        <f t="shared" si="4"/>
-        <v>6.2500000058207661E-3</v>
+        <f t="shared" si="7"/>
+        <v>3.7291666674718726E-2</v>
       </c>
       <c r="L39" s="9">
         <f>SUM(K35:K39)</f>
-        <v>0.41745370371063473</v>
+        <v>1.4109953703809879</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -4200,12 +4328,12 @@
         <v>1.6345462958270218E-2</v>
       </c>
       <c r="I40" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.0393518520868383E-2</v>
       </c>
       <c r="J40" s="9"/>
       <c r="K40" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.6738981479138602E-2</v>
       </c>
       <c r="L40" s="4"/>
@@ -4231,12 +4359,12 @@
         <v>1.1754328705137596E-2</v>
       </c>
       <c r="I41" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.3182870369928423E-2</v>
       </c>
       <c r="J41" s="9"/>
       <c r="K41" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.4937199075066019E-2</v>
       </c>
     </row>
@@ -4261,12 +4389,12 @@
         <v>6.7126157227903605E-4</v>
       </c>
       <c r="I42" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1851851857500151E-2</v>
       </c>
       <c r="J42" s="9"/>
       <c r="K42" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.2523113429779187E-2</v>
       </c>
     </row>
@@ -4291,12 +4419,12 @@
         <v>1.3356354167626705E-2</v>
       </c>
       <c r="I43" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.8194444446125999E-2</v>
       </c>
       <c r="J43" s="9"/>
       <c r="K43" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.1550798613752704E-2</v>
       </c>
       <c r="L43" s="9">
@@ -4325,12 +4453,12 @@
         <v>5.6371608799963724E-2</v>
       </c>
       <c r="I44" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.27270833333750488</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.32907994213746861</v>
       </c>
     </row>
@@ -4355,12 +4483,12 @@
         <v>5.7443761572358198E-2</v>
       </c>
       <c r="I45" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.29259259258833481</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.35003635416069301</v>
       </c>
     </row>
@@ -4374,18 +4502,24 @@
       <c r="C46" s="1">
         <v>44231.985181435186</v>
       </c>
+      <c r="D46" s="1">
+        <v>44243.315625000003</v>
+      </c>
+      <c r="E46" s="1">
+        <v>44244.765196759261</v>
+      </c>
       <c r="H46" s="9">
         <f t="shared" si="0"/>
         <v>0.2138667592589627</v>
       </c>
       <c r="I46" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1.4495717592581059</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9">
-        <f t="shared" si="4"/>
-        <v>0.2138667592589627</v>
+        <f t="shared" si="7"/>
+        <v>1.6634385185170686</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -4398,22 +4532,28 @@
       <c r="C47" s="1">
         <v>44232.056903321762</v>
       </c>
+      <c r="D47" s="1">
+        <v>44244.765196759261</v>
+      </c>
+      <c r="E47" s="1">
+        <v>44245.133668981478</v>
+      </c>
       <c r="H47" s="9">
         <f t="shared" si="0"/>
         <v>7.1721886575687677E-2</v>
       </c>
       <c r="I47" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>0.3684722222169512</v>
       </c>
       <c r="J47" s="9"/>
       <c r="K47" s="9">
-        <f t="shared" si="4"/>
-        <v>7.1721886575687677E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.44019410879263887</v>
       </c>
       <c r="L47" s="9">
         <f>SUM(K44:K47)</f>
-        <v>0.96470494213281199</v>
+        <v>2.7827489236078691</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -4422,16 +4562,16 @@
         <v>2.0530823495428194</v>
       </c>
       <c r="I48" s="9">
-        <f t="shared" ref="I48:J48" si="11">SUM(I2:I47)</f>
-        <v>6.6782986111138598</v>
+        <f t="shared" ref="I48:J48" si="12">SUM(I2:I47)</f>
+        <v>9.48988425925927</v>
       </c>
       <c r="J48" s="9">
-        <f t="shared" si="11"/>
-        <v>0.57097222222364508</v>
+        <f t="shared" si="12"/>
+        <v>0.45200231481430819</v>
       </c>
       <c r="K48" s="9">
         <f>SUM(K2:K47)</f>
-        <v>9.3023531828803243</v>
+        <v>11.994968923616398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sort batch prior to setting residency flags
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048C3EED-3480-42D7-8080-D2468CD8794C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD68941-6E1E-4D48-8D68-80FD8DA95007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
+    <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_SNOW" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
   <si>
     <t>readindividuals</t>
   </si>
@@ -295,17 +295,26 @@
     <t>Total</t>
   </si>
   <si>
-    <t>set residency days</t>
-  </si>
-  <si>
     <t>add individual characteristics</t>
+  </si>
+  <si>
+    <t>set residency flags</t>
+  </si>
+  <si>
+    <t>DP05_06 Coresident with father</t>
+  </si>
+  <si>
+    <t>DP05_05 Coresident with mother</t>
+  </si>
+  <si>
+    <t>create basic episodes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -313,7 +322,6 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="dd\ hh:mm:ss;@"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -353,7 +361,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -369,7 +377,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -690,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -707,18 +714,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="12"/>
       <c r="H1" t="s">
         <v>5</v>
       </c>
@@ -726,6 +733,15 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -758,6 +774,16 @@
         <f>SUM(H2:J2)</f>
         <v>8.1018518540076911E-4</v>
       </c>
+      <c r="M2" s="2">
+        <v>4.398148157633841E-4</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2">
+        <v>3.7037036963738501E-4</v>
+      </c>
+      <c r="P2" s="2">
+        <v>8.1018518540076911E-4</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -787,6 +813,16 @@
         <f t="shared" ref="K3:K11" si="1">SUM(H3:J3)</f>
         <v>6.9444446125999093E-5</v>
       </c>
+      <c r="M3" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="P3" s="2">
+        <v>6.9444446125999093E-5</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -824,6 +860,18 @@
         <f t="shared" si="1"/>
         <v>5.8796296289074235E-3</v>
       </c>
+      <c r="M4" s="2">
+        <v>4.8726851819083095E-3</v>
+      </c>
+      <c r="N4" s="2">
+        <v>7.8703703911742195E-4</v>
+      </c>
+      <c r="O4" s="2">
+        <v>2.1990740788169205E-4</v>
+      </c>
+      <c r="P4" s="2">
+        <v>5.8796296289074235E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -853,6 +901,16 @@
         <f t="shared" si="1"/>
         <v>3.2407407707069069E-4</v>
       </c>
+      <c r="M5" s="2">
+        <v>1.9675926159834489E-4</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
+        <v>1.273148154723458E-4</v>
+      </c>
+      <c r="P5" s="2">
+        <v>3.2407407707069069E-4</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -882,6 +940,16 @@
         <f t="shared" si="1"/>
         <v>3.9351850864477456E-4</v>
       </c>
+      <c r="M6" s="2">
+        <v>2.6620370044838637E-4</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
+        <v>1.2731480819638819E-4</v>
+      </c>
+      <c r="P6" s="2">
+        <v>3.9351850864477456E-4</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -919,16 +987,17 @@
         <f t="shared" si="1"/>
         <v>4.9699074079398997E-2</v>
       </c>
-      <c r="M7">
-        <v>411</v>
-      </c>
-      <c r="N7">
-        <f>TRUNC(M7/60,0)</f>
-        <v>6</v>
-      </c>
-      <c r="O7">
-        <f>M7-(N7*60)</f>
-        <v>51</v>
+      <c r="M7" s="2">
+        <v>2.1122685189766344E-2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>5.1388888896326534E-3</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2.34375E-2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>4.9699074079398997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -967,16 +1036,17 @@
         <f t="shared" si="1"/>
         <v>4.6296296204673126E-4</v>
       </c>
-      <c r="M8">
-        <v>427</v>
-      </c>
-      <c r="N8">
-        <f>TRUNC(M8/60,0)</f>
-        <v>7</v>
-      </c>
-      <c r="O8">
-        <f>M8-(N8*60)</f>
-        <v>7</v>
+      <c r="M8" s="2">
+        <v>1.2731480819638819E-4</v>
+      </c>
+      <c r="N8" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="O8" s="2">
+        <v>3.0092593078734353E-4</v>
+      </c>
+      <c r="P8" s="2">
+        <v>4.6296296204673126E-4</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1015,16 +1085,17 @@
         <f t="shared" si="1"/>
         <v>4.6296296204673126E-4</v>
       </c>
-      <c r="M9">
-        <v>1781</v>
-      </c>
-      <c r="N9">
-        <f>TRUNC(M9/60,0)</f>
-        <v>29</v>
-      </c>
-      <c r="O9">
-        <f>M9-(N9*60)</f>
-        <v>41</v>
+      <c r="M9" s="2">
+        <v>2.4305556144099683E-4</v>
+      </c>
+      <c r="N9" s="2">
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2.0833333110203966E-4</v>
+      </c>
+      <c r="P9" s="2">
+        <v>4.6296296204673126E-4</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1063,20 +1134,17 @@
         <f t="shared" si="1"/>
         <v>2.7777777722803876E-4</v>
       </c>
-      <c r="M10">
-        <v>3698</v>
-      </c>
-      <c r="N10">
-        <f>TRUNC(M10/3600,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <f>TRUNC((M10-(3600*N10))/60,0)</f>
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <f>M10-(3600*N10)-(O10*60)</f>
-        <v>38</v>
+      <c r="M10" s="2">
+        <v>1.0416666191304103E-4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2.3148153559304774E-5</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1.5046296175569296E-4</v>
+      </c>
+      <c r="P10" s="2">
+        <v>2.7777777722803876E-4</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1119,6 +1187,18 @@
         <f>SUM(K2:K11)</f>
         <v>5.9004629627452232E-2</v>
       </c>
+      <c r="M11" s="2">
+        <v>1.7361110803904012E-4</v>
+      </c>
+      <c r="N11" s="2">
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="O11" s="2">
+        <v>4.0509259270038456E-4</v>
+      </c>
+      <c r="P11" s="2">
+        <v>6.2500000058207661E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1156,6 +1236,18 @@
         <f t="shared" ref="K12:K16" si="8">SUM(H12:J12)</f>
         <v>8.0439814846613444E-3</v>
       </c>
+      <c r="M12" s="2">
+        <v>1.7245370327145793E-3</v>
+      </c>
+      <c r="N12" s="2">
+        <v>4.8611111560603604E-4</v>
+      </c>
+      <c r="O12" s="2">
+        <v>5.8333333363407291E-3</v>
+      </c>
+      <c r="P12" s="2">
+        <v>8.0439814846613444E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1193,6 +1285,18 @@
         <f t="shared" si="8"/>
         <v>1.0995370321325026E-3</v>
       </c>
+      <c r="M13" s="2">
+        <v>6.2500000058207661E-4</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1.1574073869269341E-4</v>
+      </c>
+      <c r="O13" s="2">
+        <v>3.5879629285773262E-4</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1.0995370321325026E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1234,15 +1338,17 @@
         <f>SUM(K12:K14)</f>
         <v>2.5612870369513985E-2</v>
       </c>
-      <c r="N14" s="11">
-        <v>804812006</v>
-      </c>
-      <c r="O14">
-        <v>4451</v>
-      </c>
-      <c r="P14" s="11">
-        <f>N14/O14</f>
-        <v>180815.99775331386</v>
+      <c r="M14" s="2">
+        <v>2.4305555562023073E-3</v>
+      </c>
+      <c r="N14" s="2">
+        <v>4.9768518510973081E-4</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1.35411111114081E-2</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1.6469351852720138E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1283,101 +1389,188 @@
         <f t="shared" si="8"/>
         <v>0.2985836805528379</v>
       </c>
+      <c r="M15" s="2">
+        <v>0.13476851851737592</v>
+      </c>
+      <c r="N15" s="2">
+        <v>2.2066921294026542E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.14174824074143544</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0.2985836805528379</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B16" s="1">
-        <v>44240.531828703701</v>
+        <v>44263.666504629633</v>
       </c>
       <c r="C16" s="1">
-        <v>44240.719846516207</v>
+        <v>44263.881840277776</v>
       </c>
       <c r="D16" s="1">
-        <v>44240.320055983793</v>
+        <v>44263.881840277776</v>
       </c>
       <c r="E16" s="1">
-        <v>44240.357453067132</v>
+        <v>44263.921747685185</v>
       </c>
       <c r="F16" s="1">
-        <v>44248.464386574073</v>
+        <v>44263.921747685185</v>
       </c>
       <c r="G16" s="1">
-        <v>44248.623757094909</v>
+        <v>44264.094143518516</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="6"/>
-        <v>0.18801781250658678</v>
+        <v>0.21533564814308193</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="9"/>
-        <v>3.7397083338873927E-2</v>
+        <v>3.9907407408463769E-2</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="2"/>
-        <v>0.1593705208360916</v>
+        <v>0.17239583333139308</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="8"/>
-        <v>0.38478541668155231</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.42763888888293877</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.19711535879469011</v>
+      </c>
+      <c r="N16" s="2">
+        <v>3.8494988431921229E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.16383101852261461</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.39944136574922595</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1">
-        <v>44241.840636574074</v>
+        <v>44264.110439814816</v>
       </c>
       <c r="C17" s="1">
-        <v>44241.931319444448</v>
+        <v>44264.192407407405</v>
       </c>
       <c r="D17" s="1">
-        <v>44241.802060185182</v>
+        <v>44264.094143518516</v>
       </c>
       <c r="E17" s="1">
-        <v>44241.840636574074</v>
+        <v>44264.110439814816</v>
       </c>
       <c r="F17" s="1">
-        <v>44248.623749999999</v>
+        <v>44250.034444444442</v>
       </c>
       <c r="G17" s="1">
-        <v>44248.688449074078</v>
+        <v>44250.092939814815</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17" si="10">C17-B17</f>
-        <v>9.0682870373711921E-2</v>
+        <v>8.1967592588625848E-2</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" ref="I17" si="11">E17-D17</f>
-        <v>3.8576388891669922E-2</v>
+        <v>1.6296296300424729E-2</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="2"/>
-        <v>6.4699074078816921E-2</v>
+        <v>5.8495370372838806E-2</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" ref="K17" si="12">SUM(H17:J17)</f>
-        <v>0.19395833334419876</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H18" s="9">
-        <f>SUM(H2:H17)</f>
-        <v>0.44583031249931082</v>
-      </c>
-      <c r="I18" s="9">
-        <f t="shared" ref="I18:J18" si="13">SUM(I2:I17)</f>
-        <v>0.10518159723869758</v>
-      </c>
-      <c r="J18" s="9">
-        <f t="shared" si="13"/>
-        <v>0.41093302083754679</v>
-      </c>
-      <c r="K18" s="9">
+        <v>0.15675925926188938</v>
+      </c>
+      <c r="M17" s="2">
+        <v>8.6979166662786156E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1.7129629632108845E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>5.8495370372838806E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.16260416666773381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44259.901886574073</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44259.944791666669</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44256.625335648147</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44256.635081018518</v>
+      </c>
+      <c r="F18" s="1">
+        <v>44263.50886574074</v>
+      </c>
+      <c r="G18" s="1">
+        <v>44263.538287037038</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H18" si="13">C18-B18</f>
+        <v>4.2905092595901806E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" ref="I18" si="14">E18-D18</f>
+        <v>9.7453703710925765E-3</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" ref="J18" si="15">G18-F18</f>
+        <v>2.9421296298096422E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" ref="K18" si="16">SUM(H18:J18)</f>
+        <v>8.2071759265090805E-2</v>
+      </c>
+      <c r="M18" s="2">
+        <v>4.2905092595901806E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>9.7453703710925765E-3</v>
+      </c>
+      <c r="O18" s="2">
+        <v>2.9421296298096422E-2</v>
+      </c>
+      <c r="P18" s="2">
+        <v>8.2071759265090805E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H19" s="9">
+        <f>SUM(H2:H18)</f>
+        <v>0.5073379629466217</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="shared" ref="I19:J19" si="17">SUM(I2:I18)</f>
+        <v>9.5157199088134803E-2</v>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" si="17"/>
+        <v>0.44717592592496658</v>
+      </c>
+      <c r="K19" s="9">
         <f>SUM(K2:K17)</f>
-        <v>0.96194493057555519</v>
+        <v>0.96759932869463228</v>
       </c>
     </row>
   </sheetData>
@@ -1942,7 +2135,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1955,18 +2148,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="12"/>
       <c r="H1" t="s">
         <v>6</v>
       </c>
@@ -1982,10 +2175,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="1">
-        <v>44207.611828703702</v>
+        <v>44255.730567129627</v>
       </c>
       <c r="C2" s="1">
-        <v>44207.611851851849</v>
+        <v>44255.730572916669</v>
       </c>
       <c r="D2" s="1">
         <v>44207.661539351851</v>
@@ -2001,7 +2194,7 @@
       </c>
       <c r="H2" s="4">
         <f>C2-B2</f>
-        <v>2.314814628334716E-5</v>
+        <v>5.7870420278050005E-6</v>
       </c>
       <c r="I2" s="4">
         <f>E2-D2</f>
@@ -2013,7 +2206,7 @@
       </c>
       <c r="K2" s="4">
         <f>SUM(H2:J2)</f>
-        <v>1.1574073869269341E-4</v>
+        <v>9.8379634437151253E-5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2021,10 +2214,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="1">
-        <v>44207.611851851849</v>
+        <v>44255.730572916669</v>
       </c>
       <c r="C3" s="1">
-        <v>44207.611863425926</v>
+        <v>44255.730590277781</v>
       </c>
       <c r="D3" s="1">
         <v>44207.661574074074</v>
@@ -2040,7 +2233,7 @@
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H14" si="0">C3-B3</f>
-        <v>1.1574076779652387E-5</v>
+        <v>1.7361111531499773E-5</v>
       </c>
       <c r="I3" s="4">
         <f>E3-D3</f>
@@ -2052,7 +2245,7 @@
       </c>
       <c r="K3" s="4">
         <f t="shared" ref="K3:K14" si="2">SUM(H3:J3)</f>
-        <v>1.1574076779652387E-5</v>
+        <v>1.7361111531499773E-5</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2060,10 +2253,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>44207.611863425926</v>
+        <v>44255.730590277781</v>
       </c>
       <c r="C4" s="1">
-        <v>44207.611909722225</v>
+        <v>44255.730636574073</v>
       </c>
       <c r="D4" s="1">
         <v>44207.661574074074</v>
@@ -2079,7 +2272,7 @@
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>4.6296299842651933E-5</v>
+        <v>4.6296292566694319E-5</v>
       </c>
       <c r="I4" s="4">
         <f>E4-D4</f>
@@ -2091,7 +2284,7 @@
       </c>
       <c r="K4" s="4">
         <f t="shared" si="2"/>
-        <v>1.5856481550144963E-3</v>
+        <v>1.5856481477385387E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2099,10 +2292,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>44207.611909722225</v>
+        <v>44255.730636574073</v>
       </c>
       <c r="C5" s="1">
-        <v>44207.611944444441</v>
+        <v>44255.730671296296</v>
       </c>
       <c r="D5" s="1">
         <v>44207.661770833336</v>
@@ -2112,7 +2305,7 @@
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>3.4722215787041932E-5</v>
+        <v>3.4722223062999547E-5</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" ref="I5:I14" si="3">E5-D5</f>
@@ -2120,7 +2313,7 @@
       </c>
       <c r="K5" s="4">
         <f t="shared" si="2"/>
-        <v>5.7870362070389092E-5</v>
+        <v>5.7870369346346706E-5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2128,10 +2321,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="1">
-        <v>44207.611944444441</v>
+        <v>44255.730671296296</v>
       </c>
       <c r="C6" s="1">
-        <v>44207.611967592595</v>
+        <v>44255.730682870373</v>
       </c>
       <c r="D6" s="1">
         <v>44207.662488425929</v>
@@ -2147,7 +2340,7 @@
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>2.3148153559304774E-5</v>
+        <v>1.1574076779652387E-5</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="3"/>
@@ -2159,7 +2352,7 @@
       </c>
       <c r="K6" s="4">
         <f t="shared" si="2"/>
-        <v>1.1574073869269341E-4</v>
+        <v>1.0416666191304103E-4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2167,10 +2360,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>44207.611944444441</v>
+        <v>44255.730671296296</v>
       </c>
       <c r="C7" s="1">
-        <v>44207.644085648149</v>
+        <v>44255.762719907405</v>
       </c>
       <c r="D7" s="1">
         <v>44208.46166666667</v>
@@ -2180,7 +2373,7 @@
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>3.2141203708306421E-2</v>
+        <v>3.2048611108621117E-2</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="3"/>
@@ -2188,7 +2381,7 @@
       </c>
       <c r="K7" s="4">
         <f t="shared" si="2"/>
-        <v>0.39409722222626442</v>
+        <v>0.39400462962657912</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2196,10 +2389,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="1">
-        <v>44207.611967592595</v>
+        <v>44255.730682870373</v>
       </c>
       <c r="C8" s="1">
-        <v>44207.611990740741</v>
+        <v>44255.730706018519</v>
       </c>
       <c r="D8" s="1">
         <v>44207.662534722222</v>
@@ -2235,10 +2428,10 @@
         <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>44207.611990740741</v>
+        <v>44255.730706018519</v>
       </c>
       <c r="C9" s="1">
-        <v>44207.612071759257</v>
+        <v>44255.730787037035</v>
       </c>
       <c r="D9" s="1">
         <v>44207.664143518516</v>
@@ -2274,10 +2467,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="1">
-        <v>44207.612071759257</v>
+        <v>44255.730787037035</v>
       </c>
       <c r="C10" s="1">
-        <v>44207.612118055556</v>
+        <v>44255.730844907404</v>
       </c>
       <c r="D10" s="1">
         <v>44207.664375</v>
@@ -2293,7 +2486,7 @@
       </c>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>4.6296299842651933E-5</v>
+        <v>5.7870369346346706E-5</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="3"/>
@@ -2305,7 +2498,7 @@
       </c>
       <c r="K10" s="4">
         <f t="shared" si="2"/>
-        <v>1.122685192967765E-3</v>
+        <v>1.1342592624714598E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2313,10 +2506,10 @@
         <v>22</v>
       </c>
       <c r="B11" s="1">
-        <v>44207.612118055556</v>
+        <v>44255.730844907404</v>
       </c>
       <c r="C11" s="1">
-        <v>44207.612175925926</v>
+        <v>44255.730902777781</v>
       </c>
       <c r="D11" s="1">
         <v>44207.665289351855</v>
@@ -2332,7 +2525,7 @@
       </c>
       <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>5.7870369346346706E-5</v>
+        <v>5.787037662230432E-5</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="3"/>
@@ -2344,7 +2537,7 @@
       </c>
       <c r="K11" s="4">
         <f t="shared" si="2"/>
-        <v>4.7453703155042604E-4</v>
+        <v>4.7453703882638365E-4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2352,10 +2545,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="1">
-        <v>44207.612175925926</v>
+        <v>44255.730902777781</v>
       </c>
       <c r="C12" s="1">
-        <v>44207.612256944441</v>
+        <v>44255.730983796297</v>
       </c>
       <c r="D12" s="1">
         <v>44207.665462962963</v>
@@ -2391,10 +2584,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="1">
-        <v>44207.644085648149</v>
+        <v>44255.762719907405</v>
       </c>
       <c r="C13" s="1">
-        <v>44207.655844907407</v>
+        <v>44255.774062500001</v>
       </c>
       <c r="D13" s="1">
         <v>44208.823622685188</v>
@@ -2404,7 +2597,7 @@
       </c>
       <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>1.1759259257814847E-2</v>
+        <v>1.1342592595610768E-2</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="3"/>
@@ -2412,7 +2605,7 @@
       </c>
       <c r="K13" s="4">
         <f t="shared" si="2"/>
-        <v>6.454861110978527E-2</v>
+        <v>6.4131944447581191E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2420,10 +2613,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="1">
-        <v>44207.655844907407</v>
+        <v>44255.774062500001</v>
       </c>
       <c r="C14" s="1">
-        <v>44207.656168981484</v>
+        <v>44255.774375000001</v>
       </c>
       <c r="D14" s="1">
         <v>44208.87641203704</v>
@@ -2433,7 +2626,7 @@
       </c>
       <c r="H14" s="4">
         <f t="shared" si="0"/>
-        <v>3.2407407707069069E-4</v>
+        <v>3.125000002910383E-4</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="3"/>
@@ -2441,11 +2634,11 @@
       </c>
       <c r="K14" s="4">
         <f t="shared" si="2"/>
-        <v>1.3194444472901523E-3</v>
+        <v>1.3078703705104999E-3</v>
       </c>
       <c r="L14" s="4">
         <f>SUM(K2:K14)</f>
-        <v>0.50070601852348773</v>
+        <v>0.500173611115315</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2453,10 +2646,10 @@
         <v>39</v>
       </c>
       <c r="B15" s="1">
-        <v>44213.924895833334</v>
+        <v>44255.89539351852</v>
       </c>
       <c r="C15" s="1">
-        <v>44213.928368055553</v>
+        <v>44255.898668981485</v>
       </c>
       <c r="D15" s="1">
         <v>44213.589907407404</v>
@@ -2472,7 +2665,7 @@
       </c>
       <c r="H15" s="4">
         <f t="shared" ref="H15" si="4">C15-B15</f>
-        <v>3.4722222189884633E-3</v>
+        <v>3.275462964666076E-3</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" ref="I15" si="5">E15-D15</f>
@@ -2484,7 +2677,7 @@
       </c>
       <c r="K15" s="4">
         <f>SUM(H15:J15)</f>
-        <v>5.2499999997962732E-2</v>
+        <v>5.2303240743640345E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2492,10 +2685,10 @@
         <v>43</v>
       </c>
       <c r="B16" s="1">
-        <v>44213.924895833334</v>
+        <v>44255.89539351852</v>
       </c>
       <c r="C16" s="1">
-        <v>44213.947488425925</v>
+        <v>44255.918888888889</v>
       </c>
       <c r="D16" s="1">
         <v>44213.589907407404</v>
@@ -2511,7 +2704,7 @@
       </c>
       <c r="H16" s="4">
         <f t="shared" ref="H16" si="6">C16-B16</f>
-        <v>2.2592592591536231E-2</v>
+        <v>2.3495370369346347E-2</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" ref="I16" si="7">E16-D16</f>
@@ -2523,7 +2716,7 @@
       </c>
       <c r="K16" s="4">
         <f t="shared" ref="K16:K34" si="8">SUM(H16:J16)</f>
-        <v>0.27129629629780538</v>
+        <v>0.2721990740756155</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2531,10 +2724,10 @@
         <v>44</v>
       </c>
       <c r="B17" s="1">
-        <v>44213.924895833334</v>
+        <v>44255.89539351852</v>
       </c>
       <c r="C17" s="1">
-        <v>44213.955613425926</v>
+        <v>44255.92728009259</v>
       </c>
       <c r="D17" s="1">
         <v>44213.589907407404</v>
@@ -2550,7 +2743,7 @@
       </c>
       <c r="H17" s="4">
         <f t="shared" ref="H17:H34" si="9">C17-B17</f>
-        <v>3.071759259182727E-2</v>
+        <v>3.1886574070085771E-2</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" ref="I17" si="10">E17-D17</f>
@@ -2562,11 +2755,11 @@
       </c>
       <c r="K17" s="4">
         <f t="shared" ref="K17" si="11">SUM(H17:J17)</f>
-        <v>0.6784027777830488</v>
+        <v>0.67957175926130731</v>
       </c>
       <c r="L17" s="9">
         <f>SUM(K15:K17)</f>
-        <v>1.0021990740788169</v>
+        <v>1.0040740740805632</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2574,18 +2767,18 @@
         <v>47</v>
       </c>
       <c r="B18" s="1">
-        <v>44231.341909722221</v>
+        <v>44255.927295208334</v>
       </c>
       <c r="C18" s="1">
-        <v>44231.509201388886</v>
+        <v>44256.088991574077</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="9"/>
-        <v>0.16729166666482342</v>
+        <v>0.16169636574340984</v>
       </c>
       <c r="K18" s="4">
         <f t="shared" si="8"/>
-        <v>0.16729166666482342</v>
+        <v>0.16169636574340984</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2593,18 +2786,18 @@
         <v>48</v>
       </c>
       <c r="B19" s="1">
-        <v>44230.637939814813</v>
+        <v>44256.219074074077</v>
       </c>
       <c r="C19" s="1">
-        <v>44230.668402777781</v>
+        <v>44256.246944444443</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="9"/>
-        <v>3.0462962968158536E-2</v>
+        <v>2.7870370366144925E-2</v>
       </c>
       <c r="K19" s="4">
         <f t="shared" si="8"/>
-        <v>3.0462962968158536E-2</v>
+        <v>2.7870370366144925E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2612,18 +2805,18 @@
         <v>49</v>
       </c>
       <c r="B20" s="1">
-        <v>44230.668402777781</v>
+        <v>44256.246944444443</v>
       </c>
       <c r="C20" s="1">
-        <v>44230.703680555554</v>
+        <v>44256.280127314814</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="9"/>
-        <v>3.5277777773444541E-2</v>
+        <v>3.3182870371092577E-2</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="8"/>
-        <v>3.5277777773444541E-2</v>
+        <v>3.3182870371092577E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2631,18 +2824,18 @@
         <v>50</v>
       </c>
       <c r="B21" s="1">
-        <v>44230.703680555554</v>
+        <v>44256.280127314814</v>
       </c>
       <c r="C21" s="1">
-        <v>44230.739537037036</v>
+        <v>44256.317476851851</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="9"/>
-        <v>3.5856481481459923E-2</v>
+        <v>3.7349537036789116E-2</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="8"/>
-        <v>3.5856481481459923E-2</v>
+        <v>3.7349537036789116E-2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2684,7 +2877,7 @@
       </c>
       <c r="L23" s="4">
         <f>SUM(K18:K23)</f>
-        <v>0.51672453703940846</v>
+        <v>0.5079347916689585</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2692,18 +2885,18 @@
         <v>53</v>
       </c>
       <c r="B24" s="1">
-        <v>44230.739537037036</v>
+        <v>44256.317476851851</v>
       </c>
       <c r="C24" s="1">
-        <v>44230.771828703706</v>
+        <v>44256.343692129631</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="9"/>
-        <v>3.2291666670062114E-2</v>
+        <v>2.6215277779556345E-2</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" si="8"/>
-        <v>3.2291666670062114E-2</v>
+        <v>2.6215277779556345E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2711,18 +2904,18 @@
         <v>54</v>
       </c>
       <c r="B25" s="1">
-        <v>44230.771828703706</v>
+        <v>44256.343692129631</v>
       </c>
       <c r="C25" s="1">
-        <v>44230.772337962961</v>
+        <v>44256.344131944446</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="9"/>
-        <v>5.0925925461342558E-4</v>
+        <v>4.398148157633841E-4</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="8"/>
-        <v>5.0925925461342558E-4</v>
+        <v>4.398148157633841E-4</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2730,18 +2923,18 @@
         <v>55</v>
       </c>
       <c r="B26" s="1">
-        <v>44230.772337962961</v>
+        <v>44256.344131944446</v>
       </c>
       <c r="C26" s="1">
-        <v>44230.772430555553</v>
+        <v>44256.344189814816</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="9"/>
-        <v>9.2592592409346253E-5</v>
+        <v>5.7870369346346706E-5</v>
       </c>
       <c r="K26" s="4">
         <f t="shared" si="8"/>
-        <v>9.2592592409346253E-5</v>
+        <v>5.7870369346346706E-5</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2749,18 +2942,18 @@
         <v>56</v>
       </c>
       <c r="B27" s="1">
-        <v>44230.772430555553</v>
+        <v>44256.344189814816</v>
       </c>
       <c r="C27" s="1">
-        <v>44230.772488425922</v>
+        <v>44256.344236111108</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="9"/>
-        <v>5.7870369346346706E-5</v>
+        <v>4.6296292566694319E-5</v>
       </c>
       <c r="K27" s="4">
         <f t="shared" si="8"/>
-        <v>5.7870369346346706E-5</v>
+        <v>4.6296292566694319E-5</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2768,18 +2961,18 @@
         <v>57</v>
       </c>
       <c r="B28" s="1">
-        <v>44230.772488425922</v>
+        <v>44256.344236111108</v>
       </c>
       <c r="C28" s="1">
-        <v>44230.772546296299</v>
+        <v>44256.344270833331</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="9"/>
-        <v>5.787037662230432E-5</v>
+        <v>3.4722223062999547E-5</v>
       </c>
       <c r="K28" s="4">
         <f t="shared" si="8"/>
-        <v>5.787037662230432E-5</v>
+        <v>3.4722223062999547E-5</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -2787,18 +2980,18 @@
         <v>58</v>
       </c>
       <c r="B29" s="1">
-        <v>44230.772546296299</v>
+        <v>44256.344270833331</v>
       </c>
       <c r="C29" s="1">
-        <v>44230.772569444445</v>
+        <v>44256.344293981485</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="9"/>
-        <v>2.314814628334716E-5</v>
+        <v>2.3148153559304774E-5</v>
       </c>
       <c r="K29" s="4">
         <f t="shared" si="8"/>
-        <v>2.314814628334716E-5</v>
+        <v>2.3148153559304774E-5</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -2806,18 +2999,18 @@
         <v>59</v>
       </c>
       <c r="B30" s="1">
-        <v>44230.772569444445</v>
+        <v>44256.344293981485</v>
       </c>
       <c r="C30" s="1">
-        <v>44230.772986111115</v>
+        <v>44256.344664351855</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="9"/>
-        <v>4.1666666948003694E-4</v>
+        <v>3.7037036963738501E-4</v>
       </c>
       <c r="K30" s="4">
         <f t="shared" si="8"/>
-        <v>4.1666666948003694E-4</v>
+        <v>3.7037036963738501E-4</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2825,18 +3018,18 @@
         <v>60</v>
       </c>
       <c r="B31" s="1">
-        <v>44230.772986111115</v>
+        <v>44256.344664351855</v>
       </c>
       <c r="C31" s="1">
-        <v>44230.903402777774</v>
+        <v>44256.463958333334</v>
       </c>
       <c r="H31" s="4">
         <f t="shared" si="9"/>
-        <v>0.13041666665958473</v>
+        <v>0.11929398147913162</v>
       </c>
       <c r="K31" s="4">
         <f t="shared" si="8"/>
-        <v>0.13041666665958473</v>
+        <v>0.11929398147913162</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -2844,18 +3037,18 @@
         <v>61</v>
       </c>
       <c r="B32" s="1">
-        <v>44230.903402777774</v>
+        <v>44256.463958333334</v>
       </c>
       <c r="C32" s="1">
-        <v>44230.905821759261</v>
+        <v>44256.466215277775</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="9"/>
-        <v>2.4189814866986126E-3</v>
+        <v>2.2569444408873096E-3</v>
       </c>
       <c r="K32" s="4">
         <f t="shared" si="8"/>
-        <v>2.4189814866986126E-3</v>
+        <v>2.2569444408873096E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -2863,18 +3056,18 @@
         <v>62</v>
       </c>
       <c r="B33" s="1">
-        <v>44230.905821759261</v>
+        <v>44256.466215277775</v>
       </c>
       <c r="C33" s="1">
-        <v>44230.906134259261</v>
+        <v>44256.466504629629</v>
       </c>
       <c r="H33" s="4">
         <f t="shared" si="9"/>
-        <v>3.125000002910383E-4</v>
+        <v>2.8935185400769114E-4</v>
       </c>
       <c r="K33" s="4">
         <f t="shared" si="8"/>
-        <v>3.125000002910383E-4</v>
+        <v>2.8935185400769114E-4</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2882,28 +3075,28 @@
         <v>63</v>
       </c>
       <c r="B34" s="1">
-        <v>44230.906134259261</v>
+        <v>44256.466504629629</v>
       </c>
       <c r="C34" s="1">
-        <v>44230.909386574072</v>
+        <v>44256.469699074078</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="9"/>
-        <v>3.2523148111067712E-3</v>
+        <v>3.1944444490363821E-3</v>
       </c>
       <c r="K34" s="4">
         <f t="shared" si="8"/>
-        <v>3.2523148111067712E-3</v>
+        <v>3.1944444490363821E-3</v>
       </c>
       <c r="L34" s="4">
         <f>SUM(K24:K34)</f>
-        <v>0.16984953703649808</v>
+        <v>0.15222222222655546</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H35" s="9">
         <f>SUM(H2:H34)</f>
-        <v>0.78800925926043419</v>
+        <v>0.76293479167361511</v>
       </c>
       <c r="I35" s="9">
         <f t="shared" ref="I35:K35" si="12">SUM(I2:I34)</f>
@@ -2915,25 +3108,25 @@
       </c>
       <c r="K35" s="9">
         <f t="shared" si="12"/>
-        <v>2.1894791666782112</v>
+        <v>2.1644046990913921</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H36" s="12">
-        <f>Pentaho_CHPC!H48/Pentaho_SNOW!H35</f>
-        <v>2.6054038393783432</v>
-      </c>
-      <c r="I36" s="12">
+      <c r="H36" s="11">
+        <f>H35/Performance_SNOW!I19</f>
+        <v>8.0176255604894724</v>
+      </c>
+      <c r="I36" s="11">
         <f>Pentaho_CHPC!I48/Pentaho_SNOW!I35</f>
         <v>11.086073553162466</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="11">
         <f>Pentaho_CHPC!J48/Pentaho_SNOW!J35</f>
-        <v>0.82867570606700247</v>
-      </c>
-      <c r="K36" s="12">
+        <v>15.404650858265022</v>
+      </c>
+      <c r="K36" s="11">
         <f>Pentaho_CHPC!K48/Pentaho_SNOW!K35</f>
-        <v>5.4784576652604908</v>
+        <v>9.2152150765490237</v>
       </c>
     </row>
   </sheetData>
@@ -2951,8 +3144,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373E5D0C-070B-4F8C-A080-FA6C8B658209}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2962,25 +3158,24 @@
     <col min="3" max="3" width="17.19921875" customWidth="1"/>
     <col min="4" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11.59765625" customWidth="1"/>
-    <col min="10" max="10" width="11.3984375" customWidth="1"/>
-    <col min="11" max="11" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.296875" customWidth="1"/>
     <col min="13" max="14" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="12"/>
       <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
@@ -3615,6 +3810,12 @@
       <c r="E18" s="1">
         <v>44235.202372685184</v>
       </c>
+      <c r="F18" s="1">
+        <v>44248.719004629631</v>
+      </c>
+      <c r="G18" s="1">
+        <v>44249.663217592592</v>
+      </c>
       <c r="H18" s="9">
         <f t="shared" si="0"/>
         <v>0.19017361111036735</v>
@@ -3625,11 +3826,11 @@
       </c>
       <c r="J18" s="9">
         <f t="shared" ref="J18:J23" si="6">G18-F18</f>
-        <v>0</v>
+        <v>0.94421296296059154</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" ref="K16:K47" si="7">SUM(H18:J18)</f>
-        <v>0.89804398147680331</v>
+        <f t="shared" ref="K18:K47" si="7">SUM(H18:J18)</f>
+        <v>1.8422569444373948</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -3648,6 +3849,12 @@
       <c r="E19" s="1">
         <v>44235.444409722222</v>
       </c>
+      <c r="F19" s="1">
+        <v>44249.663217592592</v>
+      </c>
+      <c r="G19" s="1">
+        <v>44249.853379629632</v>
+      </c>
       <c r="H19" s="9">
         <f t="shared" si="0"/>
         <v>5.0995370365853887E-2</v>
@@ -3658,11 +3865,11 @@
       </c>
       <c r="J19" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.19016203704086365</v>
       </c>
       <c r="K19" s="9">
         <f t="shared" si="7"/>
-        <v>0.29303240740409819</v>
+        <v>0.48319444444496185</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -3681,6 +3888,12 @@
       <c r="E20" s="1">
         <v>44235.662881944445</v>
       </c>
+      <c r="F20" s="1">
+        <v>44249.853379629632</v>
+      </c>
+      <c r="G20" s="1">
+        <v>44250.06890046296</v>
+      </c>
       <c r="H20" s="9">
         <f t="shared" si="0"/>
         <v>4.4907407405844424E-2</v>
@@ -3691,11 +3904,11 @@
       </c>
       <c r="J20" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.21552083332790062</v>
       </c>
       <c r="K20" s="9">
         <f t="shared" si="7"/>
-        <v>0.26337962962861639</v>
+        <v>0.478900462956517</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -3714,6 +3927,12 @@
       <c r="E21" s="1">
         <v>44235.919895833336</v>
       </c>
+      <c r="F21" s="1">
+        <v>44250.06890046296</v>
+      </c>
+      <c r="G21" s="1">
+        <v>44250.284363425926</v>
+      </c>
       <c r="H21" s="9">
         <f t="shared" si="0"/>
         <v>4.7511574077361729E-2</v>
@@ -3724,11 +3943,11 @@
       </c>
       <c r="J21" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.21546296296583023</v>
       </c>
       <c r="K21" s="9">
         <f t="shared" si="7"/>
-        <v>0.30452546296874061</v>
+        <v>0.51998842593457084</v>
       </c>
       <c r="M21" s="9">
         <f>SUM(H2:H21)</f>
@@ -3741,7 +3960,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1">
         <v>44231.161446759259</v>
@@ -3754,6 +3973,12 @@
       </c>
       <c r="E22" s="1">
         <v>44239.840636574074</v>
+      </c>
+      <c r="F22" s="1">
+        <v>44250.284363425926</v>
+      </c>
+      <c r="G22" s="1">
+        <v>44251.333460648151</v>
       </c>
       <c r="H22" s="9">
         <f t="shared" si="0"/>
@@ -3765,16 +3990,16 @@
       </c>
       <c r="J22" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.0490972222251003</v>
       </c>
       <c r="K22" s="9">
         <f t="shared" si="7"/>
-        <v>1.6206944444493274</v>
+        <v>2.6697916666744277</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B23" s="1">
         <v>44231.351203703707</v>
@@ -3787,6 +4012,12 @@
       </c>
       <c r="E23" s="1">
         <v>44241.123993055553</v>
+      </c>
+      <c r="F23" s="1">
+        <v>44253.638526863426</v>
+      </c>
+      <c r="G23" s="1">
+        <v>44254.627734664355</v>
       </c>
       <c r="H23" s="9">
         <f t="shared" si="0"/>
@@ -3798,15 +4029,15 @@
       </c>
       <c r="J23" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.98920780092885252</v>
       </c>
       <c r="K23" s="9">
         <f t="shared" si="7"/>
-        <v>1.5193287036963739</v>
+        <v>2.5085365046252264</v>
       </c>
       <c r="L23" s="9">
         <f>SUM(K18:K23)</f>
-        <v>4.8990046296239598</v>
+        <v>8.5026684490730986</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -3825,6 +4056,12 @@
       <c r="E24" s="1">
         <v>44236.098437499997</v>
       </c>
+      <c r="F24" s="1">
+        <v>44250.284363425926</v>
+      </c>
+      <c r="G24" s="1">
+        <v>44250.501224479165</v>
+      </c>
       <c r="H24" s="9">
         <f t="shared" si="0"/>
         <v>4.0844907409336884E-2</v>
@@ -3835,11 +4072,11 @@
       </c>
       <c r="J24" s="9">
         <f t="shared" ref="J24" si="9">G24-F24</f>
-        <v>0</v>
+        <v>0.21686105323897209</v>
       </c>
       <c r="K24" s="9">
         <f t="shared" si="7"/>
-        <v>0.21938657407008577</v>
+        <v>0.43624762730905786</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -3858,6 +4095,12 @@
       <c r="E25" s="1">
         <v>44236.100208333337</v>
       </c>
+      <c r="F25" s="1">
+        <v>44250.501224479165</v>
+      </c>
+      <c r="G25" s="1">
+        <v>44250.504872685182</v>
+      </c>
       <c r="H25" s="9">
         <f t="shared" si="0"/>
         <v>8.1018518540076911E-4</v>
@@ -3867,12 +4110,12 @@
         <v>1.7708333398331888E-3</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" ref="J25" si="11">G25-F25</f>
-        <v>0</v>
+        <f t="shared" ref="J25:J39" si="11">G25-F25</f>
+        <v>3.6482060168054886E-3</v>
       </c>
       <c r="K25" s="9">
         <f t="shared" si="7"/>
-        <v>2.5810185252339579E-3</v>
+        <v>6.2292245420394465E-3</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -3891,6 +4134,12 @@
       <c r="E26" s="1">
         <v>44237.53733796296</v>
       </c>
+      <c r="F26" s="1">
+        <v>44252.21806712963</v>
+      </c>
+      <c r="G26" s="1">
+        <v>44252.218354259261</v>
+      </c>
       <c r="H26" s="9">
         <f t="shared" si="0"/>
         <v>9.2592592409346253E-5</v>
@@ -3899,10 +4148,13 @@
         <f t="shared" si="10"/>
         <v>2.1990740788169205E-4</v>
       </c>
-      <c r="J26" s="9"/>
+      <c r="J26" s="9">
+        <f t="shared" si="11"/>
+        <v>2.8712963103316724E-4</v>
+      </c>
       <c r="K26" s="9">
         <f t="shared" si="7"/>
-        <v>3.125000002910383E-4</v>
+        <v>5.9962963132420555E-4</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -3921,6 +4173,12 @@
       <c r="E27" s="1">
         <v>44237.537534722222</v>
       </c>
+      <c r="F27" s="1">
+        <v>44252.232418981483</v>
+      </c>
+      <c r="G27" s="1">
+        <v>44252.232557870368</v>
+      </c>
       <c r="H27" s="9">
         <f t="shared" si="0"/>
         <v>8.1018515629693866E-5</v>
@@ -3929,10 +4187,13 @@
         <f t="shared" si="10"/>
         <v>1.9675926159834489E-4</v>
       </c>
-      <c r="J27" s="9"/>
+      <c r="J27" s="9">
+        <f t="shared" si="11"/>
+        <v>1.3888888497604057E-4</v>
+      </c>
       <c r="K27" s="9">
         <f t="shared" si="7"/>
-        <v>2.7777777722803876E-4</v>
+        <v>4.1666666220407933E-4</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -3951,6 +4212,12 @@
       <c r="E28" s="1">
         <v>44237.53769675926</v>
       </c>
+      <c r="F28" s="1">
+        <v>44252.232557870368</v>
+      </c>
+      <c r="G28" s="1">
+        <v>44252.232754629629</v>
+      </c>
       <c r="H28" s="9">
         <f t="shared" si="0"/>
         <v>6.9444446125999093E-5</v>
@@ -3959,10 +4226,13 @@
         <f t="shared" si="10"/>
         <v>1.6203703853534535E-4</v>
       </c>
-      <c r="J28" s="9"/>
+      <c r="J28" s="9">
+        <f t="shared" si="11"/>
+        <v>1.9675926159834489E-4</v>
+      </c>
       <c r="K28" s="9">
         <f t="shared" si="7"/>
-        <v>2.3148148466134444E-4</v>
+        <v>4.2824074625968933E-4</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -3981,6 +4251,12 @@
       <c r="E29" s="1">
         <v>44237.537766203706</v>
       </c>
+      <c r="F29" s="1">
+        <v>44252.232754629629</v>
+      </c>
+      <c r="G29" s="1">
+        <v>44252.232847222222</v>
+      </c>
       <c r="H29" s="9">
         <f t="shared" si="0"/>
         <v>3.4722223062999547E-5</v>
@@ -3989,10 +4265,13 @@
         <f t="shared" si="10"/>
         <v>6.9444446125999093E-5</v>
       </c>
-      <c r="J29" s="9"/>
+      <c r="J29" s="9">
+        <f t="shared" si="11"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
       <c r="K29" s="9">
         <f t="shared" si="7"/>
-        <v>1.0416666918899864E-4</v>
+        <v>1.9675926159834489E-4</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -4011,6 +4290,12 @@
       <c r="E30" s="1">
         <v>44237.538761574076</v>
       </c>
+      <c r="F30" s="1">
+        <v>44252.232847222222</v>
+      </c>
+      <c r="G30" s="1">
+        <v>44252.234178240738</v>
+      </c>
       <c r="H30" s="9">
         <f t="shared" si="0"/>
         <v>5.0925925461342558E-4</v>
@@ -4019,14 +4304,17 @@
         <f t="shared" si="10"/>
         <v>9.9537037021946162E-4</v>
       </c>
-      <c r="J30" s="9"/>
+      <c r="J30" s="9">
+        <f t="shared" si="11"/>
+        <v>1.3310185167938471E-3</v>
+      </c>
       <c r="K30" s="9">
         <f t="shared" si="7"/>
-        <v>1.5046296248328872E-3</v>
+        <v>2.8356481416267343E-3</v>
       </c>
       <c r="L30" s="9">
         <f>SUM(K24:K30)</f>
-        <v>0.22439814815152204</v>
+        <v>0.44695379629411036</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
@@ -4045,6 +4333,12 @@
       <c r="E31" s="1">
         <v>44238.354687500003</v>
       </c>
+      <c r="F31" s="1">
+        <v>44252.234185601854</v>
+      </c>
+      <c r="G31" s="1">
+        <v>44252.913564814815</v>
+      </c>
       <c r="H31" s="9">
         <f t="shared" si="0"/>
         <v>0.22476851852115942</v>
@@ -4053,10 +4347,13 @@
         <f t="shared" si="10"/>
         <v>0.81592592592642177</v>
       </c>
-      <c r="J31" s="9"/>
+      <c r="J31" s="9">
+        <f t="shared" si="11"/>
+        <v>0.67937921296106651</v>
+      </c>
       <c r="K31" s="9">
         <f t="shared" si="7"/>
-        <v>1.0406944444475812</v>
+        <v>1.7200736574086477</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
@@ -4075,6 +4372,12 @@
       <c r="E32" s="1">
         <v>44238.361666666664</v>
       </c>
+      <c r="F32" s="1">
+        <v>44252.913564814815</v>
+      </c>
+      <c r="G32" s="1">
+        <v>44252.92051084491</v>
+      </c>
       <c r="H32" s="9">
         <f t="shared" si="0"/>
         <v>4.2708333348855376E-3</v>
@@ -4083,10 +4386,13 @@
         <f t="shared" si="10"/>
         <v>6.9791666610399261E-3</v>
       </c>
-      <c r="J32" s="9"/>
+      <c r="J32" s="9">
+        <f t="shared" si="11"/>
+        <v>6.9460300946957432E-3</v>
+      </c>
       <c r="K32" s="9">
         <f t="shared" si="7"/>
-        <v>1.1249999995925464E-2</v>
+        <v>1.8196030090621207E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -4105,6 +4411,12 @@
       <c r="E33" s="1">
         <v>44238.363553240742</v>
       </c>
+      <c r="F33" s="1">
+        <v>44252.92051084491</v>
+      </c>
+      <c r="G33" s="1">
+        <v>44252.92234203704</v>
+      </c>
       <c r="H33" s="9">
         <f t="shared" si="0"/>
         <v>8.1018518540076911E-4</v>
@@ -4113,10 +4425,13 @@
         <f t="shared" si="10"/>
         <v>1.8865740785258822E-3</v>
       </c>
-      <c r="J33" s="9"/>
+      <c r="J33" s="9">
+        <f t="shared" si="11"/>
+        <v>1.8311921303393319E-3</v>
+      </c>
       <c r="K33" s="9">
         <f t="shared" si="7"/>
-        <v>2.6967592639266513E-3</v>
+        <v>4.5279513942659833E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -4135,6 +4450,12 @@
       <c r="E34" s="1">
         <v>44238.380069444444</v>
       </c>
+      <c r="F34" s="1">
+        <v>44252.92234203704</v>
+      </c>
+      <c r="G34" s="1">
+        <v>44252.935813136573</v>
+      </c>
       <c r="H34" s="9">
         <f t="shared" si="0"/>
         <v>8.2407407389837317E-3</v>
@@ -4143,14 +4464,17 @@
         <f t="shared" si="10"/>
         <v>1.6516203701030463E-2</v>
       </c>
-      <c r="J34" s="9"/>
+      <c r="J34" s="9">
+        <f t="shared" si="11"/>
+        <v>1.3471099533489905E-2</v>
+      </c>
       <c r="K34" s="9">
         <f t="shared" si="7"/>
-        <v>2.4756944440014195E-2</v>
+        <v>3.82280439735041E-2</v>
       </c>
       <c r="L34" s="9">
         <f>SUM(K31:K34)</f>
-        <v>1.0793981481474475</v>
+        <v>1.781025682867039</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -4169,6 +4493,12 @@
       <c r="E35" s="1">
         <v>44246.082511574074</v>
       </c>
+      <c r="F35" s="1">
+        <v>44257.182349537034</v>
+      </c>
+      <c r="G35" s="1">
+        <v>44258.004155092596</v>
+      </c>
       <c r="H35" s="9">
         <f t="shared" si="0"/>
         <v>0.40744212963181781</v>
@@ -4177,10 +4507,13 @@
         <f t="shared" si="10"/>
         <v>0.94884259259561077</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="J35" s="9">
+        <f t="shared" si="11"/>
+        <v>0.82180555556260515</v>
+      </c>
       <c r="K35" s="9">
         <f t="shared" si="7"/>
-        <v>1.3562847222274286</v>
+        <v>2.1780902777900337</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -4199,6 +4532,12 @@
       <c r="E36" s="1">
         <v>44246.091238425928</v>
       </c>
+      <c r="F36" s="1">
+        <v>44258.004155092596</v>
+      </c>
+      <c r="G36" s="1">
+        <v>44258.014618055553</v>
+      </c>
       <c r="H36" s="9">
         <f t="shared" si="0"/>
         <v>2.8703703719656914E-3</v>
@@ -4207,10 +4546,13 @@
         <f t="shared" si="10"/>
         <v>8.7268518545897678E-3</v>
       </c>
-      <c r="J36" s="9"/>
+      <c r="J36" s="9">
+        <f t="shared" si="11"/>
+        <v>1.0462962956808042E-2</v>
+      </c>
       <c r="K36" s="9">
         <f t="shared" si="7"/>
-        <v>1.1597222226555459E-2</v>
+        <v>2.2060185183363501E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -4229,6 +4571,12 @@
       <c r="E37" s="1">
         <v>44246.094328703701</v>
       </c>
+      <c r="F37" s="1">
+        <v>44258.014618055553</v>
+      </c>
+      <c r="G37" s="1">
+        <v>44258.01834490741</v>
+      </c>
       <c r="H37" s="9">
         <f t="shared" si="0"/>
         <v>5.7870370073942468E-4</v>
@@ -4237,10 +4585,13 @@
         <f t="shared" si="10"/>
         <v>3.0902777725714259E-3</v>
       </c>
-      <c r="J37" s="9"/>
+      <c r="J37" s="9">
+        <f t="shared" si="11"/>
+        <v>3.7268518572091125E-3</v>
+      </c>
       <c r="K37" s="9">
         <f t="shared" si="7"/>
-        <v>3.6689814733108506E-3</v>
+        <v>7.3958333305199631E-3</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -4259,6 +4610,12 @@
       <c r="E38" s="1">
         <v>44246.096168981479</v>
       </c>
+      <c r="F38" s="1">
+        <v>44258.01834490741</v>
+      </c>
+      <c r="G38" s="1">
+        <v>44258.020150462966</v>
+      </c>
       <c r="H38" s="9">
         <f t="shared" si="0"/>
         <v>3.125000002910383E-4</v>
@@ -4267,10 +4624,13 @@
         <f t="shared" si="10"/>
         <v>1.8402777786832303E-3</v>
       </c>
-      <c r="J38" s="9"/>
+      <c r="J38" s="9">
+        <f t="shared" si="11"/>
+        <v>1.8055555556202307E-3</v>
+      </c>
       <c r="K38" s="9">
         <f t="shared" si="7"/>
-        <v>2.1527777789742686E-3</v>
+        <v>3.9583333345944993E-3</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -4289,6 +4649,12 @@
       <c r="E39" s="1">
         <v>44246.127210648148</v>
       </c>
+      <c r="F39" s="1">
+        <v>44258.020150462966</v>
+      </c>
+      <c r="G39" s="1">
+        <v>44258.05740740741</v>
+      </c>
       <c r="H39" s="9">
         <f t="shared" si="0"/>
         <v>6.2500000058207661E-3</v>
@@ -4297,14 +4663,17 @@
         <f t="shared" si="10"/>
         <v>3.104166666889796E-2</v>
       </c>
-      <c r="J39" s="9"/>
+      <c r="J39" s="9">
+        <f t="shared" si="11"/>
+        <v>3.7256944444379769E-2</v>
+      </c>
       <c r="K39" s="9">
         <f t="shared" si="7"/>
-        <v>3.7291666674718726E-2</v>
+        <v>7.4548611119098496E-2</v>
       </c>
       <c r="L39" s="9">
         <f>SUM(K35:K39)</f>
-        <v>1.4109953703809879</v>
+        <v>2.2860532407576102</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -4323,6 +4692,12 @@
       <c r="E40" s="1">
         <v>44241.184386574074</v>
       </c>
+      <c r="F40" s="1">
+        <v>44254.716562499998</v>
+      </c>
+      <c r="G40" s="1">
+        <v>44254.754108796296</v>
+      </c>
       <c r="H40" s="9">
         <f t="shared" si="0"/>
         <v>1.6345462958270218E-2</v>
@@ -4331,10 +4706,13 @@
         <f t="shared" si="10"/>
         <v>6.0393518520868383E-2</v>
       </c>
-      <c r="J40" s="9"/>
+      <c r="J40" s="9">
+        <f t="shared" ref="J40:J47" si="12">G40-F40</f>
+        <v>3.754629629838746E-2</v>
+      </c>
       <c r="K40" s="9">
         <f t="shared" si="7"/>
-        <v>7.6738981479138602E-2</v>
+        <v>0.11428527777752606</v>
       </c>
       <c r="L40" s="4"/>
     </row>
@@ -4354,6 +4732,12 @@
       <c r="E41" s="1">
         <v>44241.187175925923</v>
       </c>
+      <c r="F41" s="1">
+        <v>44254.716562499998</v>
+      </c>
+      <c r="G41" s="1">
+        <v>44254.750868055555</v>
+      </c>
       <c r="H41" s="9">
         <f t="shared" si="0"/>
         <v>1.1754328705137596E-2</v>
@@ -4362,10 +4746,13 @@
         <f t="shared" si="10"/>
         <v>6.3182870369928423E-2</v>
       </c>
-      <c r="J41" s="9"/>
+      <c r="J41" s="9">
+        <f t="shared" si="12"/>
+        <v>3.4305555556784384E-2</v>
+      </c>
       <c r="K41" s="9">
         <f t="shared" si="7"/>
-        <v>7.4937199075066019E-2</v>
+        <v>0.1092427546318504</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -4384,6 +4771,12 @@
       <c r="E42" s="1">
         <v>44241.135844907411</v>
       </c>
+      <c r="F42" s="1">
+        <v>44254.716562499998</v>
+      </c>
+      <c r="G42" s="1">
+        <v>44254.7265162037</v>
+      </c>
       <c r="H42" s="9">
         <f t="shared" si="0"/>
         <v>6.7126157227903605E-4</v>
@@ -4392,10 +4785,13 @@
         <f t="shared" si="10"/>
         <v>1.1851851857500151E-2</v>
       </c>
-      <c r="J42" s="9"/>
+      <c r="J42" s="9">
+        <f t="shared" si="12"/>
+        <v>9.9537037021946162E-3</v>
+      </c>
       <c r="K42" s="9">
         <f t="shared" si="7"/>
-        <v>1.2523113429779187E-2</v>
+        <v>2.2476817131973803E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -4414,6 +4810,12 @@
       <c r="E43" s="1">
         <v>44241.202187499999</v>
       </c>
+      <c r="F43" s="1">
+        <v>44254.716562499998</v>
+      </c>
+      <c r="G43" s="1">
+        <v>44254.777060185188</v>
+      </c>
       <c r="H43" s="9">
         <f t="shared" si="0"/>
         <v>1.3356354167626705E-2</v>
@@ -4422,14 +4824,17 @@
         <f t="shared" si="10"/>
         <v>7.8194444446125999E-2</v>
       </c>
-      <c r="J43" s="9"/>
+      <c r="J43" s="9">
+        <f t="shared" si="12"/>
+        <v>6.0497685190057382E-2</v>
+      </c>
       <c r="K43" s="9">
         <f t="shared" si="7"/>
-        <v>9.1550798613752704E-2</v>
+        <v>0.15204848380381009</v>
       </c>
       <c r="L43" s="9">
         <f>SUM(K40:K43)</f>
-        <v>0.25575009259773651</v>
+        <v>0.39805333334516035</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -4448,6 +4853,12 @@
       <c r="E44" s="1">
         <v>44241.474895833337</v>
       </c>
+      <c r="F44" s="1">
+        <v>44254.777060185188</v>
+      </c>
+      <c r="G44" s="1">
+        <v>44255.051388888889</v>
+      </c>
       <c r="H44" s="9">
         <f t="shared" si="0"/>
         <v>5.6371608799963724E-2</v>
@@ -4456,10 +4867,13 @@
         <f t="shared" si="10"/>
         <v>0.27270833333750488</v>
       </c>
-      <c r="J44" s="9"/>
+      <c r="J44" s="9">
+        <f t="shared" si="12"/>
+        <v>0.27432870370103046</v>
+      </c>
       <c r="K44" s="9">
         <f t="shared" si="7"/>
-        <v>0.32907994213746861</v>
+        <v>0.60340864583849907</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -4478,6 +4892,12 @@
       <c r="E45" s="1">
         <v>44241.767488425925</v>
       </c>
+      <c r="F45" s="1">
+        <v>44255.051388888889</v>
+      </c>
+      <c r="G45" s="1">
+        <v>44255.307615740741</v>
+      </c>
       <c r="H45" s="9">
         <f t="shared" si="0"/>
         <v>5.7443761572358198E-2</v>
@@ -4486,10 +4906,13 @@
         <f t="shared" si="10"/>
         <v>0.29259259258833481</v>
       </c>
-      <c r="J45" s="9"/>
+      <c r="J45" s="9">
+        <f t="shared" si="12"/>
+        <v>0.25622685185226146</v>
+      </c>
       <c r="K45" s="9">
         <f t="shared" si="7"/>
-        <v>0.35003635416069301</v>
+        <v>0.60626320601295447</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -4508,18 +4931,27 @@
       <c r="E46" s="1">
         <v>44244.765196759261</v>
       </c>
+      <c r="F46" s="1">
+        <v>44255.307627314818</v>
+      </c>
+      <c r="G46" s="1">
+        <v>44256.885092592594</v>
+      </c>
       <c r="H46" s="9">
-        <f t="shared" si="0"/>
+        <f>C46-B46</f>
         <v>0.2138667592589627</v>
       </c>
       <c r="I46" s="9">
         <f t="shared" si="10"/>
         <v>1.4495717592581059</v>
       </c>
-      <c r="J46" s="9"/>
+      <c r="J46" s="9">
+        <f t="shared" si="12"/>
+        <v>1.5774652777763549</v>
+      </c>
       <c r="K46" s="9">
         <f t="shared" si="7"/>
-        <v>1.6634385185170686</v>
+        <v>3.2409037962934235</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -4538,6 +4970,12 @@
       <c r="E47" s="1">
         <v>44245.133668981478</v>
       </c>
+      <c r="F47" s="1">
+        <v>44256.885092592594</v>
+      </c>
+      <c r="G47" s="1">
+        <v>44257.182349537034</v>
+      </c>
       <c r="H47" s="9">
         <f t="shared" si="0"/>
         <v>7.1721886575687677E-2</v>
@@ -4546,14 +4984,17 @@
         <f t="shared" si="10"/>
         <v>0.3684722222169512</v>
       </c>
-      <c r="J47" s="9"/>
+      <c r="J47" s="9">
+        <f t="shared" si="12"/>
+        <v>0.29725694443914108</v>
+      </c>
       <c r="K47" s="9">
         <f t="shared" si="7"/>
-        <v>0.44019410879263887</v>
+        <v>0.73745105323177995</v>
       </c>
       <c r="L47" s="9">
         <f>SUM(K44:K47)</f>
-        <v>2.7827489236078691</v>
+        <v>5.188026701376657</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -4562,16 +5003,16 @@
         <v>2.0530823495428194</v>
       </c>
       <c r="I48" s="9">
-        <f t="shared" ref="I48:J48" si="12">SUM(I2:I47)</f>
+        <f t="shared" ref="I48:J48" si="13">SUM(I2:I47)</f>
         <v>9.48988425925927</v>
       </c>
       <c r="J48" s="9">
-        <f t="shared" si="12"/>
-        <v>0.45200231481430819</v>
+        <f t="shared" si="13"/>
+        <v>8.4024882060184609</v>
       </c>
       <c r="K48" s="9">
         <f>SUM(K2:K47)</f>
-        <v>11.994968923616398</v>
+        <v>19.94545481482055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final basic episode production
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD68941-6E1E-4D48-8D68-80FD8DA95007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50169379-AFA2-4E2C-9588-563423B9390C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="New Algorithm" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
   <si>
     <t>readindividuals</t>
   </si>
@@ -308,6 +309,9 @@
   </si>
   <si>
     <t>create basic episodes</t>
+  </si>
+  <si>
+    <t>basic episode QA</t>
   </si>
 </sst>
 </file>
@@ -697,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -709,7 +713,7 @@
     <col min="2" max="7" width="16.59765625" customWidth="1"/>
     <col min="8" max="10" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="14" max="14" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -750,29 +754,38 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44213.747048611112</v>
+        <v>44265.512569444443</v>
       </c>
       <c r="C2" s="1">
-        <v>44213.747488425928</v>
+        <v>44265.512754629628</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44266.516689814816</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44266.516956018517</v>
       </c>
       <c r="F2" s="1">
-        <v>44248.27752314815</v>
+        <v>44266.516956018517</v>
       </c>
       <c r="G2" s="1">
-        <v>44248.27789351852</v>
+        <v>44266.517141203702</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H11" si="0">C2-B2</f>
-        <v>4.398148157633841E-4</v>
-      </c>
-      <c r="I2" s="2"/>
+        <v>1.8518518481869251E-4</v>
+      </c>
+      <c r="I2" s="2">
+        <f>E2-D2</f>
+        <v>2.6620370044838637E-4</v>
+      </c>
       <c r="J2" s="2">
         <f>G2-F2</f>
-        <v>3.7037036963738501E-4</v>
+        <v>1.8518518481869251E-4</v>
       </c>
       <c r="K2" s="2">
         <f>SUM(H2:J2)</f>
-        <v>8.1018518540076911E-4</v>
+        <v>6.3657407008577138E-4</v>
       </c>
       <c r="M2" s="2">
         <v>4.398148157633841E-4</v>
@@ -790,28 +803,38 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>44213.747488425928</v>
+        <v>44265.512754629628</v>
       </c>
       <c r="C3" s="1">
-        <v>44213.747523148151</v>
+        <v>44265.512777777774</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44266.517141203702</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44266.517175925925</v>
       </c>
       <c r="F3" s="1">
-        <v>44248.27789351852</v>
+        <v>44266.517175925925</v>
       </c>
       <c r="G3" s="1">
-        <v>44248.277928240743</v>
+        <v>44266.517175925925</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" si="0"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I19" si="1">E3-D3</f>
         <v>3.4722223062999547E-5</v>
       </c>
       <c r="J3" s="2">
         <f>G3-F3</f>
-        <v>3.4722223062999547E-5</v>
+        <v>0</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K11" si="1">SUM(H3:J3)</f>
-        <v>6.9444446125999093E-5</v>
+        <f t="shared" ref="K3:K11" si="2">SUM(H3:J3)</f>
+        <v>5.7870369346346706E-5</v>
       </c>
       <c r="M3" s="2">
         <v>3.4722223062999547E-5</v>
@@ -829,36 +852,38 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>44213.747523148151</v>
+        <v>44265.512777777774</v>
       </c>
       <c r="C4" s="1">
-        <v>44213.752395833333</v>
+        <v>44265.517592592594</v>
       </c>
       <c r="D4" s="1">
-        <v>44213.753182870372</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>44266.517175925925</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44266.518159722225</v>
+      </c>
       <c r="F4" s="1">
-        <v>44248.277928240743</v>
+        <v>44266.518159722225</v>
       </c>
       <c r="G4" s="1">
-        <v>44248.278148148151</v>
+        <v>44266.518252314818</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8726851819083095E-3</v>
+        <v>4.8148148198379204E-3</v>
       </c>
       <c r="I4" s="2">
-        <f>D4-C4</f>
-        <v>7.8703703911742195E-4</v>
+        <f t="shared" si="1"/>
+        <v>9.8379630071576685E-4</v>
       </c>
       <c r="J4" s="2">
         <f>G4-F4</f>
-        <v>2.1990740788169205E-4</v>
+        <v>9.2592592409346253E-5</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="1"/>
-        <v>5.8796296289074235E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.8912037129630335E-3</v>
       </c>
       <c r="M4" s="2">
         <v>4.8726851819083095E-3</v>
@@ -878,28 +903,38 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>44213.753449074073</v>
+        <v>44265.517592592594</v>
       </c>
       <c r="C5" s="1">
-        <v>44213.753645833334</v>
+        <v>44265.517685185187</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44266.518252314818</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44266.518333333333</v>
       </c>
       <c r="F5" s="1">
-        <v>44248.278148148151</v>
+        <v>44266.518333333333</v>
       </c>
       <c r="G5" s="1">
-        <v>44248.278275462966</v>
+        <v>44266.518391203703</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>1.9675926159834489E-4</v>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>8.1018515629693866E-5</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" ref="J5:J17" si="2">G5-F5</f>
-        <v>1.273148154723458E-4</v>
+        <f t="shared" ref="J5:J17" si="3">G5-F5</f>
+        <v>5.7870369346346706E-5</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="1"/>
-        <v>3.2407407707069069E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.3148147738538682E-4</v>
       </c>
       <c r="M5" s="2">
         <v>1.9675926159834489E-4</v>
@@ -917,28 +952,38 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>44213.753645833334</v>
+        <v>44265.517685185187</v>
       </c>
       <c r="C6" s="1">
-        <v>44213.753912037035</v>
+        <v>44265.517789351848</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44266.518391203703</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44266.518449074072</v>
       </c>
       <c r="F6" s="1">
-        <v>44248.278275462966</v>
+        <v>44266.518449074072</v>
       </c>
       <c r="G6" s="1">
-        <v>44248.278402777774</v>
+        <v>44266.518553240741</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="0"/>
+        <v>1.0416666191304103E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0416666918899864E-4</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="2"/>
         <v>2.6620370044838637E-4</v>
-      </c>
-      <c r="J6" s="2">
-        <f t="shared" si="2"/>
-        <v>1.2731480819638819E-4</v>
-      </c>
-      <c r="K6" s="2">
-        <f t="shared" si="1"/>
-        <v>3.9351850864477456E-4</v>
       </c>
       <c r="M6" s="2">
         <v>2.6620370044838637E-4</v>
@@ -956,36 +1001,38 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>44213.753912037035</v>
+        <v>44265.517789351848</v>
       </c>
       <c r="C7" s="1">
-        <v>44213.775034722225</v>
+        <v>44265.538356481484</v>
       </c>
       <c r="D7" s="1">
-        <v>44213.780173611114</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>44266.518553240741</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44266.52270833333</v>
+      </c>
       <c r="F7" s="1">
-        <v>44248.278402777774</v>
+        <v>44266.52270833333</v>
       </c>
       <c r="G7" s="1">
-        <v>44248.301840277774</v>
+        <v>44266.545011574075</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>2.1122685189766344E-2</v>
+        <v>2.0567129635310266E-2</v>
       </c>
       <c r="I7" s="2">
-        <f>D7-C7</f>
-        <v>5.1388888896326534E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.1550925889168866E-3</v>
       </c>
       <c r="J7" s="2">
+        <f t="shared" si="3"/>
+        <v>2.2303240744804498E-2</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="2"/>
-        <v>2.34375E-2</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="1"/>
-        <v>4.9699074079398997E-2</v>
+        <v>4.7025462969031651E-2</v>
       </c>
       <c r="M7" s="2">
         <v>2.1122685189766344E-2</v>
@@ -1010,9 +1057,7 @@
       <c r="C8" s="1">
         <v>44213.803738425922</v>
       </c>
-      <c r="D8" s="1">
-        <v>44213.803773148145</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>44248.301840277774</v>
@@ -1025,16 +1070,16 @@
         <v>1.2731480819638819E-4</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" ref="I8" si="3">D8-C8</f>
-        <v>3.4722223062999547E-5</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J8" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0092593078734353E-4</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="2"/>
-        <v>3.0092593078734353E-4</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="1"/>
-        <v>4.6296296204673126E-4</v>
+        <v>4.2824073898373172E-4</v>
       </c>
       <c r="M8" s="2">
         <v>1.2731480819638819E-4</v>
@@ -1059,9 +1104,7 @@
       <c r="C9" s="1">
         <v>44213.804328703707</v>
       </c>
-      <c r="D9" s="1">
-        <v>44213.804340277777</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
         <v>44248.302141203705</v>
@@ -1074,16 +1117,16 @@
         <v>2.4305556144099683E-4</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" ref="I9" si="4">D9-C9</f>
-        <v>1.1574069503694773E-5</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J9" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0833333110203966E-4</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="2"/>
-        <v>2.0833333110203966E-4</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="1"/>
-        <v>4.6296296204673126E-4</v>
+        <v>4.5138889254303649E-4</v>
       </c>
       <c r="M9" s="2">
         <v>2.4305556144099683E-4</v>
@@ -1108,9 +1151,7 @@
       <c r="C10" s="1">
         <v>44213.804490740738</v>
       </c>
-      <c r="D10" s="1">
-        <v>44213.804513888892</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
         <v>44248.302349537036</v>
@@ -1123,16 +1164,16 @@
         <v>1.0416666191304103E-4</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" ref="I10:I11" si="5">D10-C10</f>
-        <v>2.3148153559304774E-5</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J10" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5046296175569296E-4</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>1.5046296175569296E-4</v>
-      </c>
-      <c r="K10" s="2">
-        <f t="shared" si="1"/>
-        <v>2.7777777722803876E-4</v>
+        <v>2.5462962366873398E-4</v>
       </c>
       <c r="M10" s="2">
         <v>1.0416666191304103E-4</v>
@@ -1157,9 +1198,7 @@
       <c r="C11" s="1">
         <v>44213.804837962962</v>
       </c>
-      <c r="D11" s="1">
-        <v>44213.804884259262</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
         <v>44248.302499999998</v>
@@ -1172,20 +1211,20 @@
         <v>1.7361110803904012E-4</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="5"/>
-        <v>4.6296299842651933E-5</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J11" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0509259270038456E-4</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="2"/>
-        <v>4.0509259270038456E-4</v>
-      </c>
-      <c r="K11" s="2">
-        <f t="shared" si="1"/>
-        <v>6.2500000058207661E-4</v>
+        <v>5.7870370073942468E-4</v>
       </c>
       <c r="L11" s="2">
         <f>SUM(K2:K11)</f>
-        <v>5.9004629627452232E-2</v>
+        <v>5.5821759255195502E-2</v>
       </c>
       <c r="M11" s="2">
         <v>1.7361110803904012E-4</v>
@@ -1205,36 +1244,38 @@
         <v>40</v>
       </c>
       <c r="B12" s="1">
-        <v>44213.805347222224</v>
+        <v>44265.538356481484</v>
       </c>
       <c r="C12" s="1">
-        <v>44213.807071759256</v>
+        <v>44265.547210648147</v>
       </c>
       <c r="D12" s="1">
-        <v>44213.807557870372</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>44266.545011574075</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44266.546307870369</v>
+      </c>
       <c r="F12" s="1">
-        <v>44248.302905092591</v>
+        <v>44266.546307870369</v>
       </c>
       <c r="G12" s="1">
-        <v>44248.308738425927</v>
+        <v>44266.552370115744</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H12:H16" si="6">C12-B12</f>
-        <v>1.7245370327145793E-3</v>
+        <f t="shared" ref="H12:H16" si="4">C12-B12</f>
+        <v>8.8541666627861559E-3</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" ref="I12:I14" si="7">D12-C12</f>
-        <v>4.8611111560603604E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.2962962937308475E-3</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="2"/>
-        <v>5.8333333363407291E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.0622453747782856E-3</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" ref="K12:K16" si="8">SUM(H12:J12)</f>
-        <v>8.0439814846613444E-3</v>
+        <f t="shared" ref="K12:K16" si="5">SUM(H12:J12)</f>
+        <v>1.6212708331295289E-2</v>
       </c>
       <c r="M12" s="2">
         <v>1.7245370327145793E-3</v>
@@ -1254,36 +1295,38 @@
         <v>41</v>
       </c>
       <c r="B13" s="1">
-        <v>44215.502141203702</v>
+        <v>44265.547210648147</v>
       </c>
       <c r="C13" s="1">
-        <v>44215.502766203703</v>
+        <v>44265.547731481478</v>
       </c>
       <c r="D13" s="1">
-        <v>44215.502881944441</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>44266.552361111113</v>
+      </c>
+      <c r="E13" s="1">
+        <v>44266.552499999998</v>
+      </c>
       <c r="F13" s="1">
-        <v>44248.308738425927</v>
+        <v>44266.552499999998</v>
       </c>
       <c r="G13" s="1">
-        <v>44248.30909722222</v>
+        <v>44266.552835648145</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="6"/>
-        <v>6.2500000058207661E-4</v>
+        <f t="shared" si="4"/>
+        <v>5.2083333139307797E-4</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="7"/>
-        <v>1.1574073869269341E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.3888888497604057E-4</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="2"/>
-        <v>3.5879629285773262E-4</v>
+        <f t="shared" si="3"/>
+        <v>3.3564814657438546E-4</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="8"/>
-        <v>1.0995370321325026E-3</v>
+        <f t="shared" si="5"/>
+        <v>9.9537036294350401E-4</v>
       </c>
       <c r="M13" s="2">
         <v>6.2500000058207661E-4</v>
@@ -1303,40 +1346,42 @@
         <v>42</v>
       </c>
       <c r="B14" s="1">
-        <v>44213.809675925928</v>
+        <v>44265.547731481478</v>
       </c>
       <c r="C14" s="1">
-        <v>44213.812106481484</v>
+        <v>44265.563562604169</v>
       </c>
       <c r="D14" s="1">
-        <v>44213.812604166669</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>44266.552835648145</v>
+      </c>
+      <c r="E14" s="1">
+        <v>44266.555677939818</v>
+      </c>
       <c r="F14" s="1">
-        <v>44248.30909722222</v>
+        <v>44266.555671296293</v>
       </c>
       <c r="G14" s="1">
-        <v>44248.322638333331</v>
+        <v>44266.569363425922</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="6"/>
-        <v>2.4305555562023073E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.5831122691452038E-2</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="7"/>
-        <v>4.9768518510973081E-4</v>
+        <f t="shared" si="1"/>
+        <v>2.8422916730050929E-3</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="2"/>
-        <v>1.35411111114081E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.3692129628907423E-2</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="8"/>
-        <v>1.6469351852720138E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.2365543993364554E-2</v>
       </c>
       <c r="L14" s="2">
         <f>SUM(K12:K14)</f>
-        <v>2.5612870369513985E-2</v>
+        <v>4.9573622687603347E-2</v>
       </c>
       <c r="M14" s="2">
         <v>2.4305555562023073E-3</v>
@@ -1356,38 +1401,38 @@
         <v>45</v>
       </c>
       <c r="B15" s="1">
-        <v>44231.329687500001</v>
+        <v>44265.56355324074</v>
       </c>
       <c r="C15" s="1">
-        <v>44231.464456018519</v>
+        <v>44265.75880787037</v>
       </c>
       <c r="D15" s="1">
-        <v>44231.464456018519</v>
+        <v>44266.569363425922</v>
       </c>
       <c r="E15" s="1">
-        <v>44231.486522939813</v>
+        <v>44266.601527777777</v>
       </c>
       <c r="F15" s="1">
-        <v>44248.322638333331</v>
+        <v>44266.601527777777</v>
       </c>
       <c r="G15" s="1">
-        <v>44248.464386574073</v>
+        <v>44266.767002314817</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="6"/>
-        <v>0.13476851851737592</v>
+        <f t="shared" si="4"/>
+        <v>0.19525462963065365</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" ref="I15:I16" si="9">E15-D15</f>
-        <v>2.2066921294026542E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.2164351854589768E-2</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="2"/>
-        <v>0.14174824074143544</v>
+        <f t="shared" si="3"/>
+        <v>0.1654745370396995</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="8"/>
-        <v>0.2985836805528379</v>
+        <f t="shared" si="5"/>
+        <v>0.39289351852494292</v>
       </c>
       <c r="M15" s="2">
         <v>0.13476851851737592</v>
@@ -1407,38 +1452,38 @@
         <v>86</v>
       </c>
       <c r="B16" s="1">
-        <v>44263.666504629633</v>
+        <v>44265.75880787037</v>
       </c>
       <c r="C16" s="1">
-        <v>44263.881840277776</v>
+        <v>44265.974907407406</v>
       </c>
       <c r="D16" s="1">
-        <v>44263.881840277776</v>
+        <v>44266.767002314817</v>
       </c>
       <c r="E16" s="1">
-        <v>44263.921747685185</v>
+        <v>44266.807393750001</v>
       </c>
       <c r="F16" s="1">
-        <v>44263.921747685185</v>
+        <v>44266.807384259257</v>
       </c>
       <c r="G16" s="1">
-        <v>44264.094143518516</v>
+        <v>44266.97210648148</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="6"/>
-        <v>0.21533564814308193</v>
+        <f t="shared" si="4"/>
+        <v>0.216099537035916</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="9"/>
-        <v>3.9907407408463769E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.039143518457422E-2</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="2"/>
-        <v>0.17239583333139308</v>
+        <f t="shared" si="3"/>
+        <v>0.16472222222364508</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="8"/>
-        <v>0.42763888888293877</v>
+        <f t="shared" si="5"/>
+        <v>0.4212131944441353</v>
       </c>
       <c r="M16" s="2">
         <v>0.19711535879469011</v>
@@ -1458,41 +1503,41 @@
         <v>85</v>
       </c>
       <c r="B17" s="1">
-        <v>44264.110439814816</v>
+        <v>44266.332280092596</v>
       </c>
       <c r="C17" s="1">
-        <v>44264.192407407405</v>
+        <v>44266.418611111112</v>
       </c>
       <c r="D17" s="1">
-        <v>44264.094143518516</v>
+        <v>44266.97210648148</v>
       </c>
       <c r="E17" s="1">
-        <v>44264.110439814816</v>
+        <v>44266.988981481481</v>
       </c>
       <c r="F17" s="1">
-        <v>44250.034444444442</v>
+        <v>44266.988981481481</v>
       </c>
       <c r="G17" s="1">
-        <v>44250.092939814815</v>
+        <v>44267.047349537039</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17" si="10">C17-B17</f>
-        <v>8.1967592588625848E-2</v>
+        <f t="shared" ref="H17" si="6">C17-B17</f>
+        <v>8.6331018515920732E-2</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" ref="I17" si="11">E17-D17</f>
-        <v>1.6296296300424729E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6875000001164153E-2</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="2"/>
-        <v>5.8495370372838806E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.8368055557366461E-2</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ref="K17" si="12">SUM(H17:J17)</f>
-        <v>0.15675925926188938</v>
+        <f t="shared" ref="K17" si="7">SUM(H17:J17)</f>
+        <v>0.16157407407445135</v>
       </c>
       <c r="M17" s="2">
-        <v>8.6979166662786156E-2</v>
+        <v>8.2291666665696539E-2</v>
       </c>
       <c r="N17" s="2">
         <v>1.7129629632108845E-2</v>
@@ -1509,41 +1554,41 @@
         <v>89</v>
       </c>
       <c r="B18" s="1">
-        <v>44259.901886574073</v>
+        <v>44266.418611111112</v>
       </c>
       <c r="C18" s="1">
-        <v>44259.944791666669</v>
+        <v>44266.46298611111</v>
       </c>
       <c r="D18" s="1">
-        <v>44256.625335648147</v>
+        <v>44267.047349537039</v>
       </c>
       <c r="E18" s="1">
-        <v>44256.635081018518</v>
+        <v>44267.056574074071</v>
       </c>
       <c r="F18" s="1">
-        <v>44263.50886574074</v>
+        <v>44267.056574074071</v>
       </c>
       <c r="G18" s="1">
-        <v>44263.538287037038</v>
+        <v>44267.085613425923</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" ref="H18" si="13">C18-B18</f>
-        <v>4.2905092595901806E-2</v>
+        <f t="shared" ref="H18" si="8">C18-B18</f>
+        <v>4.4374999997671694E-2</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" ref="I18" si="14">E18-D18</f>
-        <v>9.7453703710925765E-3</v>
+        <f t="shared" si="1"/>
+        <v>9.2245370324235409E-3</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" ref="J18" si="15">G18-F18</f>
-        <v>2.9421296298096422E-2</v>
+        <f t="shared" ref="J18" si="9">G18-F18</f>
+        <v>2.9039351851679385E-2</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" ref="K18" si="16">SUM(H18:J18)</f>
-        <v>8.2071759265090805E-2</v>
+        <f t="shared" ref="K18" si="10">SUM(H18:J18)</f>
+        <v>8.2638888881774619E-2</v>
       </c>
       <c r="M18" s="2">
-        <v>4.2905092595901806E-2</v>
+        <v>4.3865740743058268E-2</v>
       </c>
       <c r="N18" s="2">
         <v>9.7453703710925765E-3</v>
@@ -1556,21 +1601,63 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H19" s="9">
-        <f>SUM(H2:H18)</f>
-        <v>0.5073379629466217</v>
-      </c>
-      <c r="I19" s="9">
-        <f t="shared" ref="I19:J19" si="17">SUM(I2:I18)</f>
-        <v>9.5157199088134803E-2</v>
-      </c>
-      <c r="J19" s="9">
-        <f t="shared" si="17"/>
-        <v>0.44717592592496658</v>
-      </c>
-      <c r="K19" s="9">
-        <f>SUM(K2:K17)</f>
-        <v>0.96759932869463228</v>
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44266.46298611111</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44266.463055555556</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44267.085613425923</v>
+      </c>
+      <c r="E19" s="1">
+        <v>44267.085729166669</v>
+      </c>
+      <c r="F19" s="1">
+        <v>44267.085729166669</v>
+      </c>
+      <c r="G19" s="1">
+        <v>44267.085787037038</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" ref="H19" si="11">C19-B19</f>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1574074596865103E-4</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" ref="J19" si="12">G19-F19</f>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" ref="K19:K20" si="13">SUM(H19:J19)</f>
+        <v>2.4305556144099683E-4</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1.0416666918899864E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H20" s="2">
+        <f>SUM(H2:H19)</f>
+        <v>0.59377093749208143</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" ref="I20:J20" si="14">SUM(I2:I19)</f>
+        <v>0.10862724536855239</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="14"/>
+        <v>0.4615599305689102</v>
+      </c>
+      <c r="K20" s="9">
+        <f t="shared" si="13"/>
+        <v>1.163958113429544</v>
       </c>
     </row>
   </sheetData>
@@ -3114,7 +3201,7 @@
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H36" s="11">
         <f>H35/Performance_SNOW!I19</f>
-        <v>8.0176255604894724</v>
+        <v>6591.7563023160392</v>
       </c>
       <c r="I36" s="11">
         <f>Pentaho_CHPC!I48/Pentaho_SNOW!I35</f>
@@ -3148,7 +3235,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Completed YrAge Episode Extraction
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50169379-AFA2-4E2C-9588-563423B9390C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64D3A9-4DB5-4C50-9CFD-7F9FC8C6A740}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15855" windowWidth="29040" windowHeight="15840" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="New Algorithm" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>readindividuals</t>
   </si>
@@ -312,6 +311,30 @@
   </si>
   <si>
     <t>basic episode QA</t>
+  </si>
+  <si>
+    <t>Performance 1</t>
+  </si>
+  <si>
+    <t>DataFrames &lt; 1.0</t>
+  </si>
+  <si>
+    <t>Faster</t>
+  </si>
+  <si>
+    <t>Slower</t>
+  </si>
+  <si>
+    <t>create yr-age episodes</t>
+  </si>
+  <si>
+    <t>create yr-age episodes QA</t>
+  </si>
+  <si>
+    <t>ArrowToStata Basic episodes</t>
+  </si>
+  <si>
+    <t>ArrowToStata YrAge episodes</t>
   </si>
 </sst>
 </file>
@@ -365,7 +388,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -382,6 +405,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -701,973 +727,1503 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EA2E6-0F1D-431C-953D-8960A0E710E7}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="16.59765625" customWidth="1"/>
     <col min="8" max="10" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
     <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="9.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N2" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="Q2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>44265.512569444443</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44265.512754629628</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44266.516689814816</v>
-      </c>
-      <c r="E2" s="1">
-        <v>44266.516956018517</v>
-      </c>
-      <c r="F2" s="1">
-        <v>44266.516956018517</v>
-      </c>
-      <c r="G2" s="1">
-        <v>44266.517141203702</v>
-      </c>
-      <c r="H2" s="2">
-        <f t="shared" ref="H2:H11" si="0">C2-B2</f>
-        <v>1.8518518481869251E-4</v>
-      </c>
-      <c r="I2" s="2">
-        <f>E2-D2</f>
-        <v>2.6620370044838637E-4</v>
-      </c>
-      <c r="J2" s="2">
-        <f>G2-F2</f>
-        <v>1.8518518481869251E-4</v>
-      </c>
-      <c r="K2" s="2">
-        <f>SUM(H2:J2)</f>
-        <v>6.3657407008577138E-4</v>
-      </c>
-      <c r="M2" s="2">
-        <v>4.398148157633841E-4</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2">
-        <v>3.7037036963738501E-4</v>
-      </c>
-      <c r="P2" s="2">
-        <v>8.1018518540076911E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" s="1">
-        <v>44265.512754629628</v>
+        <v>44308.610358796293</v>
       </c>
       <c r="C3" s="1">
-        <v>44265.512777777774</v>
+        <v>44308.610752314817</v>
       </c>
       <c r="D3" s="1">
-        <v>44266.517141203702</v>
+        <v>44308.610752314817</v>
       </c>
       <c r="E3" s="1">
-        <v>44266.517175925925</v>
+        <v>44308.61078703704</v>
       </c>
       <c r="F3" s="1">
-        <v>44266.517175925925</v>
+        <v>44308.61078703704</v>
       </c>
       <c r="G3" s="1">
-        <v>44266.517175925925</v>
+        <v>44308.610960648148</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" si="0"/>
-        <v>2.314814628334716E-5</v>
+        <f t="shared" ref="H3:H12" si="0">C3-B3</f>
+        <v>3.9351852319668978E-4</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I19" si="1">E3-D3</f>
+        <f>E3-D3</f>
         <v>3.4722223062999547E-5</v>
       </c>
       <c r="J3" s="2">
         <f>G3-F3</f>
-        <v>0</v>
+        <v>1.7361110803904012E-4</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K11" si="2">SUM(H3:J3)</f>
-        <v>5.7870369346346706E-5</v>
+        <f>SUM(H3:J3)</f>
+        <v>6.0185185429872945E-4</v>
       </c>
       <c r="M3" s="2">
-        <v>3.4722223062999547E-5</v>
+        <v>4.398148157633841E-4</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2">
-        <v>3.4722223062999547E-5</v>
+        <v>3.7037036963738501E-4</v>
       </c>
       <c r="P3" s="2">
-        <v>6.9444446125999093E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.1018518540076911E-4</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1.8518518481869251E-4</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2.6620370044838637E-4</v>
+      </c>
+      <c r="S3" s="2">
+        <v>1.8518518481869251E-4</v>
+      </c>
+      <c r="T3" s="2">
+        <f t="shared" ref="T3:T12" si="1">SUM(Q3:S3)-K3</f>
+        <v>3.4722215787041932E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>44265.512777777774</v>
+        <v>44308.610960648148</v>
       </c>
       <c r="C4" s="1">
-        <v>44265.517592592594</v>
+        <v>44308.611006944448</v>
       </c>
       <c r="D4" s="1">
-        <v>44266.517175925925</v>
+        <v>44308.611006944448</v>
       </c>
       <c r="E4" s="1">
-        <v>44266.518159722225</v>
+        <v>44308.611006944448</v>
       </c>
       <c r="F4" s="1">
-        <v>44266.518159722225</v>
+        <v>44308.611006944448</v>
       </c>
       <c r="G4" s="1">
-        <v>44266.518252314818</v>
+        <v>44308.611006944448</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8148148198379204E-3</v>
+        <v>4.6296299842651933E-5</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="1"/>
-        <v>9.8379630071576685E-4</v>
+        <f t="shared" ref="I4:I24" si="2">E4-D4</f>
+        <v>0</v>
       </c>
       <c r="J4" s="2">
         <f>G4-F4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K12" si="3">SUM(H4:J4)</f>
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="P4" s="2">
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="R4" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1574069503694773E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44310.630185185182</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44310.634432870371</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44310.634432870371</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44310.635150462964</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44310.635150462964</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44310.63521990741</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2476851886021905E-3</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="2"/>
+        <v>7.1759259299142286E-4</v>
+      </c>
+      <c r="J5" s="2">
+        <f>G5-F5</f>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>5.0347222277196124E-3</v>
+      </c>
+      <c r="M5" s="2">
+        <v>4.8726851819083095E-3</v>
+      </c>
+      <c r="N5" s="2">
+        <v>7.8703703911742195E-4</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2.1990740788169205E-4</v>
+      </c>
+      <c r="P5" s="2">
+        <v>5.8796296289074235E-3</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>4.8148148198379204E-3</v>
+      </c>
+      <c r="R5" s="2">
+        <v>9.8379630071576685E-4</v>
+      </c>
+      <c r="S5" s="2">
         <v>9.2592592409346253E-5</v>
       </c>
-      <c r="K4" s="2">
+      <c r="T5" s="2">
+        <f t="shared" si="1"/>
+        <v>8.5648148524342105E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44308.616006944445</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44308.616111111114</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44308.616111111114</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44308.61613425926</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44308.61613425926</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44308.616180555553</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0416666918899864E-4</v>
+      </c>
+      <c r="I6" s="2">
         <f t="shared" si="2"/>
-        <v>5.8912037129630335E-3</v>
-      </c>
-      <c r="M4" s="2">
-        <v>4.8726851819083095E-3</v>
-      </c>
-      <c r="N4" s="2">
-        <v>7.8703703911742195E-4</v>
-      </c>
-      <c r="O4" s="2">
-        <v>2.1990740788169205E-4</v>
-      </c>
-      <c r="P4" s="2">
-        <v>5.8796296289074235E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44265.517592592594</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44265.517685185187</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44266.518252314818</v>
-      </c>
-      <c r="E5" s="1">
-        <v>44266.518333333333</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44266.518333333333</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44266.518391203703</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" ref="J6:J18" si="4">G6-F6</f>
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7361110803904012E-4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1.9675926159834489E-4</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
+        <v>1.273148154723458E-4</v>
+      </c>
+      <c r="P6" s="2">
+        <v>3.2407407707069069E-4</v>
+      </c>
+      <c r="Q6" s="2">
         <v>9.2592592409346253E-5</v>
       </c>
-      <c r="I5" s="2">
-        <f t="shared" si="1"/>
+      <c r="R6" s="2">
         <v>8.1018515629693866E-5</v>
       </c>
-      <c r="J5" s="2">
-        <f t="shared" ref="J5:J17" si="3">G5-F5</f>
+      <c r="S6" s="2">
         <v>5.7870369346346706E-5</v>
       </c>
-      <c r="K5" s="2">
-        <f t="shared" si="2"/>
-        <v>2.3148147738538682E-4</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1.9675926159834489E-4</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2">
-        <v>1.273148154723458E-4</v>
-      </c>
-      <c r="P5" s="2">
-        <v>3.2407407707069069E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44265.517685185187</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44265.517789351848</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44266.518391203703</v>
-      </c>
-      <c r="E6" s="1">
-        <v>44266.518449074072</v>
-      </c>
-      <c r="F6" s="1">
-        <v>44266.518449074072</v>
-      </c>
-      <c r="G6" s="1">
-        <v>44266.518553240741</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0416666191304103E-4</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="T6" s="2">
         <f t="shared" si="1"/>
         <v>5.7870369346346706E-5</v>
       </c>
-      <c r="J6" s="2">
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44308.616180555553</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44308.616296296299</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44308.616296296299</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44308.616319444445</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44308.616319444445</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44308.616412037038</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1574074596865103E-4</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="4"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
+        <v>2.3148148466134444E-4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2.6620370044838637E-4</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
+        <v>1.2731480819638819E-4</v>
+      </c>
+      <c r="P7" s="2">
+        <v>3.9351850864477456E-4</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1.0416666191304103E-4</v>
+      </c>
+      <c r="R7" s="2">
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="S7" s="2">
         <v>1.0416666918899864E-4</v>
       </c>
-      <c r="K6" s="2">
+      <c r="T7" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4722215787041932E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44308.616412037038</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44308.631828703707</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44308.631828703707</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44308.634687500002</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44308.634687500002</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44308.646701388891</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.541666666889796E-2</v>
+      </c>
+      <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>2.6620370044838637E-4</v>
-      </c>
-      <c r="M6" s="2">
-        <v>2.6620370044838637E-4</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2">
+        <v>2.8587962951860391E-3</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2013888888759539E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0289351852843538E-2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2.1122685189766344E-2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>5.1388888896326534E-3</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2.34375E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <v>4.9699074079398997E-2</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>2.0567129635310266E-2</v>
+      </c>
+      <c r="R8" s="2">
+        <v>4.1550925889168866E-3</v>
+      </c>
+      <c r="S8" s="2">
+        <v>2.2303240744804498E-2</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6736111116188113E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44308.646701388891</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44308.646828703706</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44308.646828703706</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44308.646863425929</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44308.646863425929</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44308.647083333337</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>1.273148154723458E-4</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="4"/>
+        <v>2.1990740788169205E-4</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>3.819444464170374E-4</v>
+      </c>
+      <c r="M9" s="2">
         <v>1.2731480819638819E-4</v>
       </c>
-      <c r="P6" s="2">
-        <v>3.9351850864477456E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44265.517789351848</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44265.538356481484</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44266.518553240741</v>
-      </c>
-      <c r="E7" s="1">
-        <v>44266.52270833333</v>
-      </c>
-      <c r="F7" s="1">
-        <v>44266.52270833333</v>
-      </c>
-      <c r="G7" s="1">
-        <v>44266.545011574075</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>2.0567129635310266E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>4.1550925889168866E-3</v>
-      </c>
-      <c r="J7" s="2">
-        <f t="shared" si="3"/>
-        <v>2.2303240744804498E-2</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="2"/>
-        <v>4.7025462969031651E-2</v>
-      </c>
-      <c r="M7" s="2">
-        <v>2.1122685189766344E-2</v>
-      </c>
-      <c r="N7" s="2">
-        <v>5.1388888896326534E-3</v>
-      </c>
-      <c r="O7" s="2">
-        <v>2.34375E-2</v>
-      </c>
-      <c r="P7" s="2">
-        <v>4.9699074079398997E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44213.803611111114</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44213.803738425922</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1">
-        <v>44248.301840277774</v>
-      </c>
-      <c r="G8" s="1">
-        <v>44248.302141203705</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2731480819638819E-4</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" si="3"/>
+      <c r="N9" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="O9" s="2">
         <v>3.0092593078734353E-4</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="2"/>
-        <v>4.2824073898373172E-4</v>
-      </c>
-      <c r="M8" s="2">
-        <v>1.2731480819638819E-4</v>
-      </c>
-      <c r="N8" s="2">
-        <v>3.4722223062999547E-5</v>
-      </c>
-      <c r="O8" s="2">
-        <v>3.0092593078734353E-4</v>
-      </c>
-      <c r="P8" s="2">
-        <v>4.6296296204673126E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44213.804085648146</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44213.804328703707</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1">
-        <v>44248.302141203705</v>
-      </c>
-      <c r="G9" s="1">
-        <v>44248.302349537036</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>2.4305556144099683E-4</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <f t="shared" si="3"/>
-        <v>2.0833333110203966E-4</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="2"/>
-        <v>4.5138889254303649E-4</v>
-      </c>
-      <c r="M9" s="2">
-        <v>2.4305556144099683E-4</v>
-      </c>
-      <c r="N9" s="2">
-        <v>1.1574069503694773E-5</v>
-      </c>
-      <c r="O9" s="2">
-        <v>2.0833333110203966E-4</v>
       </c>
       <c r="P9" s="2">
         <v>4.6296296204673126E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q9" s="2">
+        <v>1.2731480819638819E-4</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>3.0092593078734353E-4</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="1"/>
+        <v>4.6296292566694319E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44308.647083333337</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44308.647337962961</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44308.647337962961</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44308.647349537037</v>
+      </c>
+      <c r="F10" s="1">
+        <v>44308.647349537037</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44308.647430555553</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5462962366873398E-4</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="4"/>
+        <v>8.1018515629693866E-5</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>3.4722221607808024E-4</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2.4305556144099683E-4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2.0833333110203966E-4</v>
+      </c>
+      <c r="P10" s="2">
+        <v>4.6296296204673126E-4</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>2.4305556144099683E-4</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>2.0833333110203966E-4</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0416667646495625E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
-        <v>44213.804386574076</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44213.804490740738</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
-        <v>44248.302349537036</v>
-      </c>
-      <c r="G10" s="1">
-        <v>44248.302499999998</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
+      <c r="B11" s="1">
+        <v>44308.647430555553</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44308.647523148145</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44308.647523148145</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44308.647534722222</v>
+      </c>
+      <c r="F11" s="1">
+        <v>44308.647534722222</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44308.647662037038</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="4"/>
+        <v>1.273148154723458E-4</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>2.3148148466134444E-4</v>
+      </c>
+      <c r="M11" s="2">
         <v>1.0416666191304103E-4</v>
       </c>
-      <c r="I10" s="2">
+      <c r="N11" s="2">
+        <v>2.3148153559304774E-5</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1.5046296175569296E-4</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2.7777777722803876E-4</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>1.0416666191304103E-4</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>1.5046296175569296E-4</v>
+      </c>
+      <c r="T11" s="2">
         <f t="shared" si="1"/>
+        <v>2.3148139007389545E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44308.647662037038</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44308.647789351853</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44308.647789351853</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44308.647824074076</v>
+      </c>
+      <c r="F12" s="1">
+        <v>44308.647824074076</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44308.648090277777</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.273148154723458E-4</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="4"/>
+        <v>2.6620370044838637E-4</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>4.2824073898373172E-4</v>
+      </c>
+      <c r="L12" s="2">
+        <f>SUM(K3:K12)</f>
+        <v>3.776620371354511E-2</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1.7361110803904012E-4</v>
+      </c>
+      <c r="N12" s="2">
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="O12" s="2">
+        <v>4.0509259270038456E-4</v>
+      </c>
+      <c r="P12" s="2">
+        <v>6.2500000058207661E-4</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1.7361110803904012E-4</v>
+      </c>
+      <c r="R12" s="2">
         <v>0</v>
       </c>
-      <c r="J10" s="2">
-        <f t="shared" si="3"/>
+      <c r="S12" s="2">
+        <v>4.0509259270038456E-4</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="1"/>
         <v>1.5046296175569296E-4</v>
       </c>
-      <c r="K10" s="2">
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44310.63521990741</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44310.644571759258</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44310.644571759258</v>
+      </c>
+      <c r="E13" s="1">
+        <v>44310.646018518521</v>
+      </c>
+      <c r="F13" s="1">
+        <v>44310.646018518521</v>
+      </c>
+      <c r="G13" s="1">
+        <v>44310.652592592596</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" ref="H13:H17" si="5">C13-B13</f>
+        <v>9.3518518478958867E-3</v>
+      </c>
+      <c r="I13" s="2">
         <f t="shared" si="2"/>
-        <v>2.5462962366873398E-4</v>
-      </c>
-      <c r="M10" s="2">
-        <v>1.0416666191304103E-4</v>
-      </c>
-      <c r="N10" s="2">
-        <v>2.3148153559304774E-5</v>
-      </c>
-      <c r="O10" s="2">
-        <v>1.5046296175569296E-4</v>
-      </c>
-      <c r="P10" s="2">
-        <v>2.7777777722803876E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44213.804664351854</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44213.804837962962</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
-        <v>44248.302499999998</v>
-      </c>
-      <c r="G11" s="1">
-        <v>44248.302905092591</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7361110803904012E-4</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <f t="shared" si="3"/>
-        <v>4.0509259270038456E-4</v>
-      </c>
-      <c r="K11" s="2">
+        <v>1.4467592627624981E-3</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="4"/>
+        <v>6.5740740756154992E-3</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" ref="K13:K17" si="6">SUM(H13:J13)</f>
+        <v>1.7372685186273884E-2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1.7245370327145793E-3</v>
+      </c>
+      <c r="N13" s="2">
+        <v>4.8611111560603604E-4</v>
+      </c>
+      <c r="O13" s="2">
+        <v>5.8333333363407291E-3</v>
+      </c>
+      <c r="P13" s="2">
+        <v>8.0439814846613444E-3</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>8.8541666627861559E-3</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1.2962962937308475E-3</v>
+      </c>
+      <c r="S13" s="2">
+        <v>6.0622453747782856E-3</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" ref="T13:T20" si="7">SUM(Q13:S13)-K13</f>
+        <v>-1.1599768549785949E-3</v>
+      </c>
+      <c r="U13" s="2">
+        <f>ABS(T13)</f>
+        <v>1.1599768549785949E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44310.652592592596</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44310.653124999997</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44310.653124999997</v>
+      </c>
+      <c r="E14" s="1">
+        <v>44310.653252314813</v>
+      </c>
+      <c r="F14" s="1">
+        <v>44310.653252314813</v>
+      </c>
+      <c r="G14" s="1">
+        <v>44310.653634259259</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="5"/>
+        <v>5.3240740089677274E-4</v>
+      </c>
+      <c r="I14" s="2">
         <f t="shared" si="2"/>
-        <v>5.7870370073942468E-4</v>
-      </c>
-      <c r="L11" s="2">
-        <f>SUM(K2:K11)</f>
-        <v>5.5821759255195502E-2</v>
-      </c>
-      <c r="M11" s="2">
-        <v>1.7361110803904012E-4</v>
-      </c>
-      <c r="N11" s="2">
+        <v>1.273148154723458E-4</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="4"/>
+        <v>3.819444464170374E-4</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="6"/>
+        <v>1.0416666627861559E-3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>6.2500000058207661E-4</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1.1574073869269341E-4</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3.5879629285773262E-4</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1.0995370321325026E-3</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>5.2083333139307797E-4</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1.3888888497604057E-4</v>
+      </c>
+      <c r="S14" s="2">
+        <v>3.3564814657438546E-4</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="7"/>
+        <v>-4.6296299842651933E-5</v>
+      </c>
+      <c r="U14" s="2">
+        <f>ABS(T14)</f>
         <v>4.6296299842651933E-5</v>
       </c>
-      <c r="O11" s="2">
-        <v>4.0509259270038456E-4</v>
-      </c>
-      <c r="P11" s="2">
-        <v>6.2500000058207661E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1">
-        <v>44265.538356481484</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44265.547210648147</v>
-      </c>
-      <c r="D12" s="1">
-        <v>44266.545011574075</v>
-      </c>
-      <c r="E12" s="1">
-        <v>44266.546307870369</v>
-      </c>
-      <c r="F12" s="1">
-        <v>44266.546307870369</v>
-      </c>
-      <c r="G12" s="1">
-        <v>44266.552370115744</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" ref="H12:H16" si="4">C12-B12</f>
-        <v>8.8541666627861559E-3</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>1.2962962937308475E-3</v>
-      </c>
-      <c r="J12" s="2">
-        <f t="shared" si="3"/>
-        <v>6.0622453747782856E-3</v>
-      </c>
-      <c r="K12" s="2">
-        <f t="shared" ref="K12:K16" si="5">SUM(H12:J12)</f>
-        <v>1.6212708331295289E-2</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1.7245370327145793E-3</v>
-      </c>
-      <c r="N12" s="2">
-        <v>4.8611111560603604E-4</v>
-      </c>
-      <c r="O12" s="2">
-        <v>5.8333333363407291E-3</v>
-      </c>
-      <c r="P12" s="2">
-        <v>8.0439814846613444E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="1">
-        <v>44265.547210648147</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44265.547731481478</v>
-      </c>
-      <c r="D13" s="1">
-        <v>44266.552361111113</v>
-      </c>
-      <c r="E13" s="1">
-        <v>44266.552499999998</v>
-      </c>
-      <c r="F13" s="1">
-        <v>44266.552499999998</v>
-      </c>
-      <c r="G13" s="1">
-        <v>44266.552835648145</v>
-      </c>
-      <c r="H13" s="2">
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44310.653634259259</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44310.668981481482</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44310.668981481482</v>
+      </c>
+      <c r="E15" s="1">
+        <v>44310.671712962961</v>
+      </c>
+      <c r="F15" s="1">
+        <v>44310.671712962961</v>
+      </c>
+      <c r="G15" s="1">
+        <v>44310.685150462959</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5347222222771961E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="2"/>
+        <v>2.7314814797136933E-3</v>
+      </c>
+      <c r="J15" s="2">
         <f t="shared" si="4"/>
-        <v>5.2083333139307797E-4</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3888888497604057E-4</v>
-      </c>
-      <c r="J13" s="2">
-        <f t="shared" si="3"/>
-        <v>3.3564814657438546E-4</v>
-      </c>
-      <c r="K13" s="2">
+        <v>1.3437499997962732E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="6"/>
+        <v>3.1516203700448386E-2</v>
+      </c>
+      <c r="L15" s="2">
+        <f>SUM(K13:K15)</f>
+        <v>4.9930555549508426E-2</v>
+      </c>
+      <c r="M15" s="2">
+        <v>2.4305555562023073E-3</v>
+      </c>
+      <c r="N15" s="2">
+        <v>4.9768518510973081E-4</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.35411111114081E-2</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1.6469351852720138E-2</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.5831122691452038E-2</v>
+      </c>
+      <c r="R15" s="2">
+        <v>2.8422916730050929E-3</v>
+      </c>
+      <c r="S15" s="2">
+        <v>1.3692129628907423E-2</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="7"/>
+        <v>8.4934029291616753E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44310.685150462959</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44310.900891203702</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44310.900891203702</v>
+      </c>
+      <c r="E16" s="1">
+        <v>44310.931990740741</v>
+      </c>
+      <c r="F16" s="1">
+        <v>44310.931990740741</v>
+      </c>
+      <c r="G16" s="1">
+        <v>44311.089965277781</v>
+      </c>
+      <c r="H16" s="2">
         <f t="shared" si="5"/>
-        <v>9.9537036294350401E-4</v>
-      </c>
-      <c r="M13" s="2">
-        <v>6.2500000058207661E-4</v>
-      </c>
-      <c r="N13" s="2">
-        <v>1.1574073869269341E-4</v>
-      </c>
-      <c r="O13" s="2">
-        <v>3.5879629285773262E-4</v>
-      </c>
-      <c r="P13" s="2">
-        <v>1.0995370321325026E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44265.547731481478</v>
-      </c>
-      <c r="C14" s="1">
-        <v>44265.563562604169</v>
-      </c>
-      <c r="D14" s="1">
-        <v>44266.552835648145</v>
-      </c>
-      <c r="E14" s="1">
-        <v>44266.555677939818</v>
-      </c>
-      <c r="F14" s="1">
-        <v>44266.555671296293</v>
-      </c>
-      <c r="G14" s="1">
-        <v>44266.569363425922</v>
-      </c>
-      <c r="H14" s="2">
+        <v>0.21574074074305827</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="2"/>
+        <v>3.1099537038244307E-2</v>
+      </c>
+      <c r="J16" s="2">
         <f t="shared" si="4"/>
-        <v>1.5831122691452038E-2</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
-        <v>2.8422916730050929E-3</v>
-      </c>
-      <c r="J14" s="2">
-        <f t="shared" si="3"/>
-        <v>1.3692129628907423E-2</v>
-      </c>
-      <c r="K14" s="2">
+        <v>0.15797453703999054</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="6"/>
+        <v>0.40481481482129311</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.13476851851737592</v>
+      </c>
+      <c r="N16" s="2">
+        <v>2.2066921294026542E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.14174824074143544</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.2985836805528379</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0.19525462963065365</v>
+      </c>
+      <c r="R16" s="2">
+        <v>3.2164351854589768E-2</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.1654745370396995</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.1921296296350192E-2</v>
+      </c>
+      <c r="U16" s="2">
+        <f>ABS(T16)</f>
+        <v>1.1921296296350192E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44327.666898148149</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44327.842604166668</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44326.198842592596</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44326.232002314813</v>
+      </c>
+      <c r="F17" s="1">
+        <v>44327.842604166668</v>
+      </c>
+      <c r="G17" s="1">
+        <v>44327.97892361111</v>
+      </c>
+      <c r="H17" s="2">
         <f t="shared" si="5"/>
-        <v>3.2365543993364554E-2</v>
-      </c>
-      <c r="L14" s="2">
-        <f>SUM(K12:K14)</f>
-        <v>4.9573622687603347E-2</v>
-      </c>
-      <c r="M14" s="2">
-        <v>2.4305555562023073E-3</v>
-      </c>
-      <c r="N14" s="2">
-        <v>4.9768518510973081E-4</v>
-      </c>
-      <c r="O14" s="2">
-        <v>1.35411111114081E-2</v>
-      </c>
-      <c r="P14" s="2">
-        <v>1.6469351852720138E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="1">
-        <v>44265.56355324074</v>
-      </c>
-      <c r="C15" s="1">
-        <v>44265.75880787037</v>
-      </c>
-      <c r="D15" s="1">
-        <v>44266.569363425922</v>
-      </c>
-      <c r="E15" s="1">
-        <v>44266.601527777777</v>
-      </c>
-      <c r="F15" s="1">
-        <v>44266.601527777777</v>
-      </c>
-      <c r="G15" s="1">
-        <v>44266.767002314817</v>
-      </c>
-      <c r="H15" s="2">
+        <v>0.17570601851912215</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="2"/>
+        <v>3.3159722217533272E-2</v>
+      </c>
+      <c r="J17" s="2">
         <f t="shared" si="4"/>
-        <v>0.19525462963065365</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="1"/>
-        <v>3.2164351854589768E-2</v>
-      </c>
-      <c r="J15" s="2">
-        <f t="shared" si="3"/>
-        <v>0.1654745370396995</v>
-      </c>
-      <c r="K15" s="2">
-        <f t="shared" si="5"/>
-        <v>0.39289351852494292</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0.13476851851737592</v>
-      </c>
-      <c r="N15" s="2">
-        <v>2.2066921294026542E-2</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0.14174824074143544</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0.2985836805528379</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44265.75880787037</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44265.974907407406</v>
-      </c>
-      <c r="D16" s="1">
-        <v>44266.767002314817</v>
-      </c>
-      <c r="E16" s="1">
-        <v>44266.807393750001</v>
-      </c>
-      <c r="F16" s="1">
-        <v>44266.807384259257</v>
-      </c>
-      <c r="G16" s="1">
-        <v>44266.97210648148</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" si="4"/>
+        <v>0.13631944444205146</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="6"/>
+        <v>0.34518518517870689</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.19711535879469011</v>
+      </c>
+      <c r="N17" s="2">
+        <v>3.8494988431921229E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.16383101852261461</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.39944136574922595</v>
+      </c>
+      <c r="Q17" s="2">
         <v>0.216099537035916</v>
       </c>
-      <c r="I16" s="2">
-        <f t="shared" si="1"/>
+      <c r="R17" s="2">
         <v>4.039143518457422E-2</v>
       </c>
-      <c r="J16" s="2">
-        <f t="shared" si="3"/>
+      <c r="S17" s="2">
         <v>0.16472222222364508</v>
       </c>
-      <c r="K16" s="2">
-        <f t="shared" si="5"/>
-        <v>0.4212131944441353</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0.19711535879469011</v>
-      </c>
-      <c r="N16" s="2">
-        <v>3.8494988431921229E-2</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0.16383101852261461</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0.39944136574922595</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="T17" s="2">
+        <f t="shared" si="7"/>
+        <v>7.6028009265428409E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="1">
-        <v>44266.332280092596</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44266.418611111112</v>
-      </c>
-      <c r="D17" s="1">
-        <v>44266.97210648148</v>
-      </c>
-      <c r="E17" s="1">
-        <v>44266.988981481481</v>
-      </c>
-      <c r="F17" s="1">
-        <v>44266.988981481481</v>
-      </c>
-      <c r="G17" s="1">
-        <v>44267.047349537039</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" ref="H17" si="6">C17-B17</f>
-        <v>8.6331018515920732E-2</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6875000001164153E-2</v>
-      </c>
-      <c r="J17" s="2">
-        <f t="shared" si="3"/>
-        <v>5.8368055557366461E-2</v>
-      </c>
-      <c r="K17" s="2">
-        <f t="shared" ref="K17" si="7">SUM(H17:J17)</f>
-        <v>0.16157407407445135</v>
-      </c>
-      <c r="M17" s="2">
-        <v>8.2291666665696539E-2</v>
-      </c>
-      <c r="N17" s="2">
-        <v>1.7129629632108845E-2</v>
-      </c>
-      <c r="O17" s="2">
-        <v>5.8495370372838806E-2</v>
-      </c>
-      <c r="P17" s="2">
-        <v>0.16260416666773381</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>89</v>
-      </c>
       <c r="B18" s="1">
-        <v>44266.418611111112</v>
+        <v>44327.97892361111</v>
       </c>
       <c r="C18" s="1">
-        <v>44266.46298611111</v>
+        <v>44328.065150462964</v>
       </c>
       <c r="D18" s="1">
-        <v>44267.047349537039</v>
+        <v>44326.232002314813</v>
       </c>
       <c r="E18" s="1">
-        <v>44267.056574074071</v>
+        <v>44326.24894675926</v>
       </c>
       <c r="F18" s="1">
-        <v>44267.056574074071</v>
+        <v>44328.065150462964</v>
       </c>
       <c r="G18" s="1">
-        <v>44267.085613425923</v>
+        <v>44328.123761574076</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" ref="H18" si="8">C18-B18</f>
+        <v>8.6226851854007691E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6944444447290152E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="4"/>
+        <v>5.86111111115315E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" ref="K18" si="9">SUM(H18:J18)</f>
+        <v>0.16178240741282934</v>
+      </c>
+      <c r="M18" s="2">
+        <v>8.2291666665696539E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1.7129629632108845E-2</v>
+      </c>
+      <c r="O18" s="2">
+        <v>5.8495370372838806E-2</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.16260416666773381</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>8.6331018515920732E-2</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1.6875000001164153E-2</v>
+      </c>
+      <c r="S18" s="2">
+        <v>5.8368055557366461E-2</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="7"/>
+        <v>-2.0833333837799728E-4</v>
+      </c>
+      <c r="U18" s="2">
+        <f>ABS(T18)</f>
+        <v>2.0833333837799728E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44328.123761574076</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44328.167824074073</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44326.24894675926</v>
+      </c>
+      <c r="E19" s="1">
+        <v>44326.258298611108</v>
+      </c>
+      <c r="F19" s="1">
+        <v>44328.167824074073</v>
+      </c>
+      <c r="G19" s="1">
+        <v>44328.198136574072</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" ref="H19" si="10">C19-B19</f>
+        <v>4.4062499997380655E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="2"/>
+        <v>9.3518518478958867E-3</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" ref="J19" si="11">G19-F19</f>
+        <v>3.0312499999126885E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" ref="K19" si="12">SUM(H19:J19)</f>
+        <v>8.3726851844403427E-2</v>
+      </c>
+      <c r="M19" s="2">
+        <v>4.3865740743058268E-2</v>
+      </c>
+      <c r="N19" s="2">
+        <v>9.7453703710925765E-3</v>
+      </c>
+      <c r="O19" s="2">
+        <v>2.9421296298096422E-2</v>
+      </c>
+      <c r="P19" s="2">
+        <v>8.2071759265090805E-2</v>
+      </c>
+      <c r="Q19" s="2">
         <v>4.4374999997671694E-2</v>
       </c>
-      <c r="I18" s="2">
-        <f t="shared" si="1"/>
+      <c r="R19" s="2">
         <v>9.2245370324235409E-3</v>
       </c>
-      <c r="J18" s="2">
-        <f t="shared" ref="J18" si="9">G18-F18</f>
+      <c r="S19" s="2">
         <v>2.9039351851679385E-2</v>
       </c>
-      <c r="K18" s="2">
-        <f t="shared" ref="K18" si="10">SUM(H18:J18)</f>
-        <v>8.2638888881774619E-2</v>
-      </c>
-      <c r="M18" s="2">
-        <v>4.3865740743058268E-2</v>
-      </c>
-      <c r="N18" s="2">
-        <v>9.7453703710925765E-3</v>
-      </c>
-      <c r="O18" s="2">
-        <v>2.9421296298096422E-2</v>
-      </c>
-      <c r="P18" s="2">
-        <v>8.2071759265090805E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="T19" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.0879629626288079E-3</v>
+      </c>
+      <c r="U19" s="2">
+        <f>ABS(T19)</f>
+        <v>1.0879629626288079E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="1">
-        <v>44266.46298611111</v>
-      </c>
-      <c r="C19" s="1">
-        <v>44266.463055555556</v>
-      </c>
-      <c r="D19" s="1">
-        <v>44267.085613425923</v>
-      </c>
-      <c r="E19" s="1">
-        <v>44267.085729166669</v>
-      </c>
-      <c r="F19" s="1">
-        <v>44267.085729166669</v>
-      </c>
-      <c r="G19" s="1">
-        <v>44267.085787037038</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" ref="H19" si="11">C19-B19</f>
+      <c r="B20" s="1">
+        <v>44328.198136574072</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44328.198229166665</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44326.258298611108</v>
+      </c>
+      <c r="E20" s="1">
+        <v>44326.258449074077</v>
+      </c>
+      <c r="F20" s="1">
+        <v>44328.198229166665</v>
+      </c>
+      <c r="G20" s="1">
+        <v>44328.198287037034</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" ref="H20:H24" si="13">C20-B20</f>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5046296903165057E-4</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" ref="J20:J24" si="14">G20-F20</f>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" ref="K20:K24" si="15">SUM(H20:J20)</f>
+        <v>3.0092593078734353E-4</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1.0416666918899864E-4</v>
+      </c>
+      <c r="Q20" s="2">
         <v>6.9444446125999093E-5</v>
       </c>
-      <c r="I19" s="2">
-        <f t="shared" si="1"/>
+      <c r="R20" s="2">
         <v>1.1574074596865103E-4</v>
       </c>
-      <c r="J19" s="2">
-        <f t="shared" ref="J19" si="12">G19-F19</f>
+      <c r="S20" s="2">
         <v>5.7870369346346706E-5</v>
       </c>
-      <c r="K19" s="2">
-        <f t="shared" ref="K19:K20" si="13">SUM(H19:J19)</f>
-        <v>2.4305556144099683E-4</v>
-      </c>
-      <c r="M19" s="2">
-        <v>1.0416666918899864E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H20" s="2">
-        <f>SUM(H2:H19)</f>
+      <c r="T20" s="2">
+        <f t="shared" si="7"/>
+        <v>-5.7870369346346706E-5</v>
+      </c>
+      <c r="U20" s="2">
+        <f>ABS(T20)</f>
+        <v>5.7870369346346706E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44328.198287037034</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44328.244062500002</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44326.258449074077</v>
+      </c>
+      <c r="E21" s="1">
+        <v>44326.267881944441</v>
+      </c>
+      <c r="F21" s="1">
+        <v>44328.244317129633</v>
+      </c>
+      <c r="G21" s="1">
+        <v>44328.275937500002</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="13"/>
+        <v>4.5775462967867497E-2</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="2"/>
+        <v>9.4328703635255806E-3</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="14"/>
+        <v>3.1620370369637385E-2</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="15"/>
+        <v>8.6828703701030463E-2</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44328.244062500002</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44328.244317129633</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44326.267881944441</v>
+      </c>
+      <c r="E22" s="1">
+        <v>44326.268020833333</v>
+      </c>
+      <c r="F22" s="1">
+        <v>44328.275937500002</v>
+      </c>
+      <c r="G22" s="1">
+        <v>44328.27616898148</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="13"/>
+        <v>2.546296309446916E-4</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3888889225199819E-4</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="14"/>
+        <v>2.3148147738538682E-4</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="15"/>
+        <v>6.2500000058207661E-4</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44328.451863425929</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44328.451932870368</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44328.451932870368</v>
+      </c>
+      <c r="E23" s="1">
+        <v>44328.451932870368</v>
+      </c>
+      <c r="F23" s="1">
+        <v>44328.451932870368</v>
+      </c>
+      <c r="G23" s="1">
+        <v>44328.451956018522</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="13"/>
+        <v>6.9444438850041479E-5</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="14"/>
+        <v>2.3148153559304774E-5</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="15"/>
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44328.451956018522</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44328.452141203707</v>
+      </c>
+      <c r="D24" s="1">
+        <v>44328.452141203707</v>
+      </c>
+      <c r="E24" s="1">
+        <v>44328.452175925922</v>
+      </c>
+      <c r="F24" s="1">
+        <v>44328.452175925922</v>
+      </c>
+      <c r="G24" s="1">
+        <v>44328.452314814815</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="13"/>
+        <v>1.8518518481869251E-4</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="2"/>
+        <v>3.4722215787041932E-5</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="14"/>
+        <v>1.3888889225199819E-4</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="15"/>
+        <v>3.5879629285773262E-4</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H25" s="2">
+        <f>SUM(H3:H24)</f>
+        <v>0.61427083334274357</v>
+      </c>
+      <c r="I25" s="2">
+        <f>SUM(I3:I24)</f>
+        <v>0.10836805555300089</v>
+      </c>
+      <c r="J25" s="2">
+        <f>SUM(J3:J24)</f>
+        <v>0.44877314814220881</v>
+      </c>
+      <c r="K25" s="9">
+        <f>SUM(K3:K24)</f>
+        <v>1.1714120370379533</v>
+      </c>
+      <c r="Q25" s="2">
+        <f>SUM(Q3:Q20)</f>
         <v>0.59377093749208143</v>
       </c>
-      <c r="I20" s="2">
-        <f t="shared" ref="I20:J20" si="14">SUM(I2:I19)</f>
+      <c r="R25" s="2">
+        <f t="shared" ref="R25:S25" si="16">SUM(R3:R20)</f>
         <v>0.10862724536855239</v>
       </c>
-      <c r="J20" s="2">
-        <f t="shared" si="14"/>
+      <c r="S25" s="2">
+        <f t="shared" si="16"/>
         <v>0.4615599305689102</v>
       </c>
-      <c r="K20" s="9">
-        <f t="shared" si="13"/>
-        <v>1.163958113429544</v>
-      </c>
+      <c r="T25" s="9">
+        <f>SUM(T3:T20)</f>
+        <v>8.0451168978470378E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="5">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="T11:T12 T3:T10" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2235,18 +2791,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="13"/>
       <c r="H1" t="s">
         <v>6</v>
       </c>
@@ -3200,8 +3756,8 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H36" s="11">
-        <f>H35/Performance_SNOW!I19</f>
-        <v>6591.7563023160392</v>
+        <f>H35/Performance_SNOW!I20</f>
+        <v>5070.5817955322173</v>
       </c>
       <c r="I36" s="11">
         <f>Pentaho_CHPC!I48/Pentaho_SNOW!I35</f>
@@ -3251,18 +3807,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="10" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Final source for 2022 Dataset Production
</commit_message>
<xml_diff>
--- a/src/Performance.xlsx
+++ b/src/Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ahriorg-my.sharepoint.com/personal/kobus_herbst_ahri_org/Documents/Documents/GitHub/SaprinJulia/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3342584-36F2-4168-B0CB-CF5674D91F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{D3342584-36F2-4168-B0CB-CF5674D91F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAB59406-E2F7-42FB-B04F-6D4D2DA64325}"/>
   <bookViews>
-    <workbookView xWindow="4550" yWindow="3390" windowWidth="28800" windowHeight="15230" activeTab="3" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{ADA19AFF-9B1D-47A9-946C-AEEEF5365620}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_SNOW" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="105">
   <si>
     <t>readindividuals</t>
   </si>
@@ -347,6 +348,12 @@
   </si>
   <si>
     <t>father coresidency</t>
+  </si>
+  <si>
+    <t>2020 Performance</t>
+  </si>
+  <si>
+    <t>Difference compared to 2020</t>
   </si>
 </sst>
 </file>
@@ -400,7 +407,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -424,13 +431,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -760,32 +792,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14" t="s">
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="16"/>
       <c r="H2" t="s">
         <v>5</v>
       </c>
@@ -2377,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751965E-4A3A-442F-9C21-79FCCBFBF505}">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2389,33 +2421,42 @@
     <col min="2" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.19921875" customWidth="1"/>
     <col min="5" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.796875" customWidth="1"/>
+    <col min="15" max="17" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3" customWidth="1"/>
+    <col min="21" max="21" width="9.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="M1" s="15"/>
+      <c r="N1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="12" t="s">
         <v>5</v>
       </c>
@@ -2428,76 +2469,124 @@
       <c r="K2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="11"/>
+      <c r="N2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>83</v>
+      </c>
       <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>44358.871400462966</v>
+        <v>44736.518518518518</v>
       </c>
       <c r="C3" s="1">
-        <v>44358.872060185182</v>
+        <v>44736.519131944442</v>
       </c>
       <c r="D3" s="1">
-        <v>44358.872060185182</v>
+        <v>44736.519131944442</v>
       </c>
       <c r="E3" s="1">
-        <v>44358.872118055559</v>
+        <v>44736.519189814811</v>
       </c>
       <c r="F3" s="1">
-        <v>44358.872118055559</v>
+        <v>44736.519189814811</v>
       </c>
       <c r="G3" s="1">
-        <v>44358.872523148151</v>
+        <v>44736.519606481481</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ref="H3" si="0">C3-B3</f>
-        <v>6.5972221636911854E-4</v>
+        <v>6.1342592380242422E-4</v>
       </c>
       <c r="I3" s="2">
         <f>E3-D3</f>
-        <v>5.787037662230432E-5</v>
+        <v>5.7870369346346706E-5</v>
       </c>
       <c r="J3" s="2">
         <f>G3-F3</f>
-        <v>4.0509259270038456E-4</v>
+        <v>4.1666666948003694E-4</v>
       </c>
       <c r="K3" s="2">
         <f>SUM(H3:J3)</f>
+        <v>1.0879629626288079E-3</v>
+      </c>
+      <c r="N3" s="2">
+        <v>6.5972221636911854E-4</v>
+      </c>
+      <c r="O3" s="2">
+        <v>5.787037662230432E-5</v>
+      </c>
+      <c r="P3" s="2">
+        <v>4.0509259270038456E-4</v>
+      </c>
+      <c r="Q3" s="2">
         <v>1.1226851856918074E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S3" s="2">
+        <f>ABS(N3-H3)</f>
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="T3" s="2">
+        <f>ABS(O3-I3)</f>
+        <v>7.2759576141834259E-12</v>
+      </c>
+      <c r="U3" s="2">
+        <f>ABS(P3-J3)</f>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="V3" s="2">
+        <f>ABS(SUM(N3-H3,O3-I3,P3-J3))</f>
+        <v>3.4722223062999547E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>44358.872523148151</v>
+        <v>44736.519606481481</v>
       </c>
       <c r="C4" s="1">
-        <v>44358.872604166667</v>
+        <v>44736.519675925927</v>
       </c>
       <c r="D4" s="1">
-        <v>44358.872604166667</v>
+        <v>44736.519675925927</v>
       </c>
       <c r="E4" s="1">
-        <v>44358.872604166667</v>
+        <v>44736.519675925927</v>
       </c>
       <c r="F4" s="1">
-        <v>44358.872604166667</v>
+        <v>44736.519675925927</v>
       </c>
       <c r="G4" s="1">
-        <v>44358.872604166667</v>
+        <v>44736.519675925927</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ref="H4:H29" si="1">C4-B4</f>
-        <v>8.1018515629693866E-5</v>
+        <v>6.9444446125999093E-5</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ref="I4:I29" si="2">E4-D4</f>
@@ -2509,70 +2598,126 @@
       </c>
       <c r="K4" s="2">
         <f t="shared" ref="K4:K27" si="4">SUM(H4:J4)</f>
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="N4" s="2">
         <v>8.1018515629693866E-5</v>
       </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>8.1018515629693866E-5</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" ref="S4:S30" si="5">ABS(N4-H4)</f>
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" ref="T4:T30" si="6">ABS(O4-I4)</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" ref="U4:U30" si="7">ABS(P4-J4)</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" ref="V4:V30" si="8">ABS(SUM(N4-H4,O4-I4,P4-J4))</f>
+        <v>1.1574069503694773E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>44359.215763888889</v>
+        <v>44736.519675925927</v>
       </c>
       <c r="C5" s="1">
-        <v>44359.217893518522</v>
+        <v>44736.52270833333</v>
       </c>
       <c r="D5" s="1">
-        <v>44359.217893518522</v>
+        <v>44736.52270833333</v>
       </c>
       <c r="E5" s="1">
-        <v>44359.2184837963</v>
+        <v>44736.523668981485</v>
       </c>
       <c r="F5" s="1">
-        <v>44359.2184837963</v>
+        <v>44736.523668981485</v>
       </c>
       <c r="G5" s="1">
-        <v>44359.218622685185</v>
+        <v>44736.523819444446</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="1"/>
-        <v>2.1296296326909214E-3</v>
+        <v>3.0324074032250792E-3</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="2"/>
-        <v>5.9027777751907706E-4</v>
+        <v>9.6064815443241969E-4</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="3"/>
-        <v>1.3888888497604057E-4</v>
+        <v>1.5046296175569296E-4</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="4"/>
+        <v>4.1435185194131918E-3</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2.1296296326909214E-3</v>
+      </c>
+      <c r="O5" s="2">
+        <v>5.9027777751907706E-4</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1.3888888497604057E-4</v>
+      </c>
+      <c r="Q5" s="2">
         <v>2.8587962951860391E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S5" s="2">
+        <f t="shared" si="5"/>
+        <v>9.0277777053415775E-4</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" si="6"/>
+        <v>3.7037037691334262E-4</v>
+      </c>
+      <c r="U5" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="V5" s="2">
+        <f t="shared" si="8"/>
+        <v>1.2847222242271528E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>44359.218622685185</v>
+        <v>44736.523819444446</v>
       </c>
       <c r="C6" s="1">
-        <v>44359.218784722223</v>
+        <v>44736.523981481485</v>
       </c>
       <c r="D6" s="1">
-        <v>44359.218784722223</v>
+        <v>44736.523981481485</v>
       </c>
       <c r="E6" s="1">
-        <v>44359.218877314815</v>
+        <v>44736.524027777778</v>
       </c>
       <c r="F6" s="1">
-        <v>44359.218877314815</v>
+        <v>44736.524027777778</v>
       </c>
       <c r="G6" s="1">
-        <v>44359.219039351854</v>
+        <v>44736.524178240739</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="1"/>
@@ -2580,494 +2725,858 @@
       </c>
       <c r="I6" s="2">
         <f t="shared" si="2"/>
-        <v>9.2592592409346253E-5</v>
+        <v>4.6296292566694319E-5</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="3"/>
-        <v>1.6203703853534535E-4</v>
+        <v>1.5046296175569296E-4</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="4"/>
+        <v>3.5879629285773262E-4</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1.6203703853534535E-4</v>
+      </c>
+      <c r="O6" s="2">
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1.6203703853534535E-4</v>
+      </c>
+      <c r="Q6" s="2">
         <v>4.1666666948003694E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S6" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <f t="shared" si="6"/>
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="U6" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="V6" s="2">
+        <f t="shared" si="8"/>
+        <v>5.787037662230432E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>44359.219039351854</v>
+        <v>44736.524178240739</v>
       </c>
       <c r="C7" s="1">
-        <v>44359.219224537039</v>
+        <v>44736.524340277778</v>
       </c>
       <c r="D7" s="1">
-        <v>44359.219224537039</v>
+        <v>44736.524340277778</v>
       </c>
       <c r="E7" s="1">
-        <v>44359.219270833331</v>
+        <v>44736.524375000001</v>
       </c>
       <c r="F7" s="1">
-        <v>44359.219270833331</v>
+        <v>44736.524375000001</v>
       </c>
       <c r="G7" s="1">
-        <v>44359.219444444447</v>
+        <v>44736.524537037039</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="1"/>
-        <v>1.8518518481869251E-4</v>
+        <v>1.6203703853534535E-4</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="2"/>
-        <v>4.6296292566694319E-5</v>
+        <v>3.4722223062999547E-5</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="3"/>
-        <v>1.7361111531499773E-4</v>
+        <v>1.6203703853534535E-4</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="4"/>
+        <v>3.5879630013369024E-4</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1.8518518481869251E-4</v>
+      </c>
+      <c r="O7" s="2">
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1.7361111531499773E-4</v>
+      </c>
+      <c r="Q7" s="2">
         <v>4.0509259270038456E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S7" s="2">
+        <f t="shared" si="5"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="6"/>
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="V7" s="2">
+        <f t="shared" si="8"/>
+        <v>4.6296292566694319E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>44359.219444444447</v>
+        <v>44737.289641203701</v>
       </c>
       <c r="C8" s="1">
-        <v>44359.247418981482</v>
+        <v>44737.308749999997</v>
       </c>
       <c r="D8" s="1">
-        <v>44359.247418981482</v>
+        <v>44737.308749999997</v>
       </c>
       <c r="E8" s="1">
-        <v>44359.252384259256</v>
+        <v>44737.313634259262</v>
       </c>
       <c r="F8" s="1">
-        <v>44359.252384259256</v>
+        <v>44737.313634259262</v>
       </c>
       <c r="G8" s="1">
-        <v>44359.287094907406</v>
+        <v>44737.330254629633</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
-        <v>2.7974537035333924E-2</v>
+        <v>1.9108796295768116E-2</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>4.9652777743176557E-3</v>
+        <v>4.8842592659639195E-3</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="3"/>
-        <v>3.4710648149484769E-2</v>
+        <v>1.6620370370219462E-2</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="4"/>
+        <v>4.0613425931951497E-2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2.7974537035333924E-2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>4.9652777743176557E-3</v>
+      </c>
+      <c r="P8" s="2">
+        <v>3.4710648149484769E-2</v>
+      </c>
+      <c r="Q8" s="2">
         <v>6.7650462959136348E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S8" s="2">
+        <f t="shared" si="5"/>
+        <v>8.8657407395658083E-3</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="6"/>
+        <v>8.1018508353736252E-5</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="7"/>
+        <v>1.8090277779265307E-2</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="8"/>
+        <v>2.7037037027184851E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>44359.287094907406</v>
+        <v>44737.330254629633</v>
       </c>
       <c r="C9" s="1">
-        <v>44359.287430555552</v>
+        <v>44737.33053240741</v>
       </c>
       <c r="D9" s="1">
-        <v>44359.287430555552</v>
+        <v>44737.33053240741</v>
       </c>
       <c r="E9" s="1">
-        <v>44359.287465277775</v>
+        <v>44737.330590277779</v>
       </c>
       <c r="F9" s="1">
-        <v>44359.287465277775</v>
+        <v>44737.330590277779</v>
       </c>
       <c r="G9" s="1">
-        <v>44359.287789351853</v>
+        <v>44737.330925925926</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>3.3564814657438546E-4</v>
+        <v>2.7777777722803876E-4</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="2"/>
-        <v>3.4722223062999547E-5</v>
+        <v>5.7870369346346706E-5</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="3"/>
-        <v>3.2407407707069069E-4</v>
+        <v>3.3564814657438546E-4</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="4"/>
+        <v>6.7129629314877093E-4</v>
+      </c>
+      <c r="N9" s="2">
+        <v>3.3564814657438546E-4</v>
+      </c>
+      <c r="O9" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="P9" s="2">
+        <v>3.2407407707069069E-4</v>
+      </c>
+      <c r="Q9" s="2">
         <v>6.944444467080757E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S9" s="2">
+        <f t="shared" si="5"/>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="6"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="V9" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3148153559304774E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>44359.287789351853</v>
+        <v>44737.645104166666</v>
       </c>
       <c r="C10" s="1">
-        <v>44359.288171296299</v>
+        <v>44737.646249999998</v>
       </c>
       <c r="D10" s="1">
-        <v>44359.288171296299</v>
+        <v>44737.646249999998</v>
       </c>
       <c r="E10" s="1">
-        <v>44359.288194444445</v>
+        <v>44737.646319444444</v>
       </c>
       <c r="F10" s="1">
-        <v>44359.288194444445</v>
+        <v>44737.646319444444</v>
       </c>
       <c r="G10" s="1">
-        <v>44359.288298611114</v>
+        <v>44737.646493055552</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>3.819444464170374E-4</v>
+        <v>1.1458333319751546E-3</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="2"/>
-        <v>2.314814628334716E-5</v>
+        <v>6.9444446125999093E-5</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="3"/>
-        <v>1.0416666918899864E-4</v>
+        <v>1.7361110803904012E-4</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="4"/>
+        <v>1.3888888861401938E-3</v>
+      </c>
+      <c r="N10" s="2">
+        <v>3.819444464170374E-4</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1.0416666918899864E-4</v>
+      </c>
+      <c r="Q10" s="2">
         <v>5.092592618893832E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S10" s="2">
+        <f t="shared" si="5"/>
+        <v>7.6388888555811718E-4</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="6"/>
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="7"/>
+        <v>6.9444438850041479E-5</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="8"/>
+        <v>8.7962962425081059E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>44359.288298611114</v>
+        <v>44737.330925925926</v>
       </c>
       <c r="C11" s="1">
-        <v>44359.288437499999</v>
+        <v>44737.331076388888</v>
       </c>
       <c r="D11" s="1">
-        <v>44359.288437499999</v>
+        <v>44737.331076388888</v>
       </c>
       <c r="E11" s="1">
-        <v>44359.288449074076</v>
+        <v>44737.331099537034</v>
       </c>
       <c r="F11" s="1">
-        <v>44359.288449074076</v>
+        <v>44737.331099537034</v>
       </c>
       <c r="G11" s="1">
-        <v>44359.288622685184</v>
+        <v>44737.331284722219</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>1.3888888497604057E-4</v>
+        <v>1.5046296175569296E-4</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="2"/>
-        <v>1.1574076779652387E-5</v>
+        <v>2.314814628334716E-5</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="3"/>
-        <v>1.7361110803904012E-4</v>
+        <v>1.8518518481869251E-4</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="4"/>
+        <v>3.5879629285773262E-4</v>
+      </c>
+      <c r="N11" s="2">
+        <v>1.3888888497604057E-4</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1.7361110803904012E-4</v>
+      </c>
+      <c r="Q11" s="2">
         <v>3.2407406979473308E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S11" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="6"/>
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="V11" s="2">
+        <f t="shared" si="8"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>44359.288622685184</v>
+        <v>44737.331284722219</v>
       </c>
       <c r="C12" s="1">
-        <v>44359.2887962963</v>
+        <v>44737.331469907411</v>
       </c>
       <c r="D12" s="1">
-        <v>44359.2887962963</v>
+        <v>44737.331469907411</v>
       </c>
       <c r="E12" s="1">
-        <v>44359.288842592592</v>
+        <v>44737.33152777778</v>
       </c>
       <c r="F12" s="1">
-        <v>44359.288842592592</v>
+        <v>44737.33152777778</v>
       </c>
       <c r="G12" s="1">
-        <v>44359.289236111108</v>
+        <v>44737.331944444442</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
-        <v>1.7361111531499773E-4</v>
+        <v>1.8518519209465012E-4</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="2"/>
-        <v>4.6296292566694319E-5</v>
+        <v>5.7870369346346706E-5</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="3"/>
-        <v>3.9351851592073217E-4</v>
+        <v>4.1666666220407933E-4</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" si="4"/>
-        <v>6.1342592380242422E-4</v>
+        <v>6.5972222364507616E-4</v>
       </c>
       <c r="L12" s="8">
         <f>SUM(K3:K12)</f>
-        <v>7.4675925920018926E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+        <v>4.9710648148902692E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1.7361111531499773E-4</v>
+      </c>
+      <c r="O12" s="2">
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="P12" s="2">
+        <v>3.9351851592073217E-4</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>6.1342592380242422E-4</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="6"/>
+        <v>1.1574076779652387E-5</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="7"/>
+        <v>2.314814628334716E-5</v>
+      </c>
+      <c r="V12" s="2">
+        <f t="shared" si="8"/>
+        <v>4.6296299842651933E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="1">
-        <v>44359.289236111108</v>
+        <v>44737.913865740738</v>
       </c>
       <c r="C13" s="1">
-        <v>44359.303171296298</v>
+        <v>44737.933564814812</v>
       </c>
       <c r="D13" s="1">
-        <v>44359.303171296298</v>
+        <v>44737.933564814812</v>
       </c>
       <c r="E13" s="1">
-        <v>44359.30541666667</v>
+        <v>44737.938761574071</v>
       </c>
       <c r="F13" s="1">
-        <v>44359.30541666667</v>
+        <v>44737.938761574071</v>
       </c>
       <c r="G13" s="1">
-        <v>44359.318518518521</v>
+        <v>44737.95417824074</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
-        <v>1.393518519034842E-2</v>
+        <v>1.9699074073287193E-2</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="2"/>
-        <v>2.2453703713836148E-3</v>
+        <v>5.1967592589790002E-3</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="3"/>
-        <v>1.3101851851388346E-2</v>
+        <v>1.541666666889796E-2</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="4"/>
+        <v>4.0312500001164153E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1.393518519034842E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <v>2.2453703713836148E-3</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1.3101851851388346E-2</v>
+      </c>
+      <c r="Q13" s="2">
         <v>2.9282407413120382E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S13" s="2">
+        <f t="shared" si="5"/>
+        <v>5.7638888829387724E-3</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="6"/>
+        <v>2.9513888875953853E-3</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="7"/>
+        <v>2.3148148175096139E-3</v>
+      </c>
+      <c r="V13" s="2">
+        <f t="shared" si="8"/>
+        <v>1.1030092588043772E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="1">
-        <v>44359.318518518521</v>
+        <v>44737.95417824074</v>
       </c>
       <c r="C14" s="1">
-        <v>44359.318761574075</v>
+        <v>44737.954502314817</v>
       </c>
       <c r="D14" s="1">
-        <v>44359.318761574075</v>
+        <v>44737.954502314817</v>
       </c>
       <c r="E14" s="1">
-        <v>44359.318796296298</v>
+        <v>44737.954571759263</v>
       </c>
       <c r="F14" s="1">
-        <v>44359.318796296298</v>
+        <v>44737.954571759263</v>
       </c>
       <c r="G14" s="1">
-        <v>44359.318981481483</v>
+        <v>44737.954768518517</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>2.4305555416503921E-4</v>
+        <v>3.2407407707069069E-4</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="2"/>
-        <v>3.4722223062999547E-5</v>
+        <v>6.9444446125999093E-5</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="3"/>
-        <v>1.8518518481869251E-4</v>
+        <v>1.9675925432238728E-4</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="4"/>
+        <v>5.9027777751907706E-4</v>
+      </c>
+      <c r="N14" s="2">
+        <v>2.4305555416503921E-4</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1.8518518481869251E-4</v>
+      </c>
+      <c r="Q14" s="2">
         <v>4.6296296204673126E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S14" s="2">
+        <f t="shared" si="5"/>
+        <v>8.101852290565148E-5</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="6"/>
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="7"/>
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="V14" s="2">
+        <f t="shared" si="8"/>
+        <v>1.273148154723458E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="1">
-        <v>44359.318981481483</v>
+        <v>44737.954768518517</v>
       </c>
       <c r="C15" s="1">
-        <v>44359.357499999998</v>
+        <v>44737.991435185184</v>
       </c>
       <c r="D15" s="1">
-        <v>44359.357499999998</v>
+        <v>44737.991435185184</v>
       </c>
       <c r="E15" s="1">
-        <v>44359.362592592595</v>
+        <v>44738.000081018516</v>
       </c>
       <c r="F15" s="1">
-        <v>44359.362592592595</v>
+        <v>44738.000081018516</v>
       </c>
       <c r="G15" s="1">
-        <v>44359.395381944443</v>
+        <v>44738.035856481481</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>3.8518518515047617E-2</v>
+        <v>3.6666666666860692E-2</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="2"/>
-        <v>5.0925925970659591E-3</v>
+        <v>8.6458333316841163E-3</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="3"/>
-        <v>3.2789351847895887E-2</v>
+        <v>3.5775462965830229E-2</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="4"/>
+        <v>8.1087962964375038E-2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>3.8518518515047617E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>5.0925925970659591E-3</v>
+      </c>
+      <c r="P15" s="2">
+        <v>3.2789351847895887E-2</v>
+      </c>
+      <c r="Q15" s="2">
         <v>7.6400462960009463E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S15" s="2">
+        <f t="shared" si="5"/>
+        <v>1.8518518481869251E-3</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="6"/>
+        <v>3.5532407346181571E-3</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9861111179343425E-3</v>
+      </c>
+      <c r="V15" s="2">
+        <f t="shared" si="8"/>
+        <v>4.6875000043655746E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="1">
-        <v>44359.395381944443</v>
+        <v>44738.372511574074</v>
       </c>
       <c r="C16" s="1">
-        <v>44359.803541666668</v>
+        <v>44738.856851851851</v>
       </c>
       <c r="D16" s="1">
-        <v>44359.803541666668</v>
+        <v>44738.856851851851</v>
       </c>
       <c r="E16" s="1">
-        <v>44359.864571759259</v>
+        <v>44738.967442129629</v>
       </c>
       <c r="F16" s="1">
-        <v>44359.864571759259</v>
+        <v>44738.967442129629</v>
       </c>
       <c r="G16" s="1">
-        <v>44360.173819444448</v>
+        <v>44739.352592592593</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
-        <v>0.40815972222480923</v>
+        <v>0.484340277776937</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="2"/>
-        <v>6.1030092590954155E-2</v>
+        <v>0.11059027777810115</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="3"/>
-        <v>0.30924768518889323</v>
+        <v>0.38515046296379296</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="4"/>
+        <v>0.98008101851883112</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.40815972222480923</v>
+      </c>
+      <c r="O16" s="2">
+        <v>6.1030092590954155E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.30924768518889323</v>
+      </c>
+      <c r="Q16" s="2">
         <v>0.77843750000465661</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="S16" s="2">
+        <f t="shared" si="5"/>
+        <v>7.6180555552127771E-2</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="6"/>
+        <v>4.9560185187146999E-2</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" si="7"/>
+        <v>7.5902777774899732E-2</v>
+      </c>
+      <c r="V16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.2016435185141745</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>85</v>
       </c>
       <c r="B17" s="1">
-        <v>44360.173819444448</v>
+        <v>44739.352592592593</v>
       </c>
       <c r="C17" s="1">
-        <v>44360.439166666663</v>
+        <v>44739.659282407411</v>
       </c>
       <c r="D17" s="1">
-        <v>44360.439166666663</v>
+        <v>44739.659282407411</v>
       </c>
       <c r="E17" s="1">
-        <v>44360.48641203704</v>
+        <v>44739.736643518518</v>
       </c>
       <c r="F17" s="1">
-        <v>44360.48641203704</v>
+        <v>44739.736643518518</v>
       </c>
       <c r="G17" s="1">
-        <v>44360.686562499999</v>
+        <v>44739.977835648147</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
-        <v>0.265347222215496</v>
+        <v>0.30668981481721858</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="2"/>
-        <v>4.7245370376913343E-2</v>
+        <v>7.7361111107165925E-2</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="3"/>
-        <v>0.20015046295884531</v>
+        <v>0.24119212962978054</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="4"/>
+        <v>0.62524305555416504</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.265347222215496</v>
+      </c>
+      <c r="O17" s="2">
+        <v>4.7245370376913343E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.20015046295884531</v>
+      </c>
+      <c r="Q17" s="2">
         <v>0.51274305555125466</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="S17" s="2">
+        <f t="shared" si="5"/>
+        <v>4.1342592601722572E-2</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="6"/>
+        <v>3.0115740730252583E-2</v>
+      </c>
+      <c r="U17" s="2">
+        <f t="shared" si="7"/>
+        <v>4.1041666670935228E-2</v>
+      </c>
+      <c r="V17" s="2">
+        <f t="shared" si="8"/>
+        <v>0.11250000000291038</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="1">
-        <v>44360.715127314812</v>
+        <v>44739.977835648147</v>
       </c>
       <c r="C18" s="1">
-        <v>44360.883553240739</v>
+        <v>44740.245138888888</v>
       </c>
       <c r="D18" s="1">
-        <v>44360.686562499999</v>
+        <v>44739.977835648147</v>
       </c>
       <c r="E18" s="1">
-        <v>44360.715127314812</v>
+        <v>44740.031747685185</v>
       </c>
       <c r="F18" s="1">
-        <v>44360.883553240739</v>
+        <v>44740.245416666665</v>
       </c>
       <c r="G18" s="1">
-        <v>44360.996678240743</v>
+        <v>44740.40347222222</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
-        <v>0.16842592592729488</v>
+        <v>0.26730324074014788</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="2"/>
-        <v>2.8564814812853001E-2</v>
+        <v>5.391203703766223E-2</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="3"/>
-        <v>0.11312500000349246</v>
+        <v>0.15805555555562023</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="4"/>
-        <v>0.31011574074364034</v>
+        <v>0.47927083333343035</v>
       </c>
       <c r="L18" s="8">
         <f>SUM(K13:K18)</f>
-        <v>1.7074421296347282</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2.2065856481494848</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.16842592592729488</v>
+      </c>
+      <c r="O18" s="2">
+        <v>2.8564814812853001E-2</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.11312500000349246</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0.31011574074364034</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="5"/>
+        <v>9.8877314812853001E-2</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="6"/>
+        <v>2.5347222224809229E-2</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" si="7"/>
+        <v>4.4930555552127771E-2</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" si="8"/>
+        <v>0.16915509258979</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -3109,8 +3618,36 @@
         <f>K19+K25</f>
         <v>0.34474537037021946</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19" s="2">
+        <v>8.8020833332848269E-2</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1.5578703700157348E-2</v>
+      </c>
+      <c r="P19" s="2">
+        <v>6.0115740743640345E-2</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0.16371527777664596</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -3148,8 +3685,36 @@
         <f t="shared" si="4"/>
         <v>2.3148148466134444E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20" s="2">
+        <v>1.0416666918899864E-4</v>
+      </c>
+      <c r="O20" s="2">
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="P20" s="2">
+        <v>6.9444446125999093E-5</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>2.3148148466134444E-4</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -3187,8 +3752,36 @@
         <f t="shared" si="4"/>
         <v>0.16702546296437504</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N21" s="2">
+        <v>8.8750000002619345E-2</v>
+      </c>
+      <c r="O21" s="2">
+        <v>1.5775462961755693E-2</v>
+      </c>
+      <c r="P21" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0.16702546296437504</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T21" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U21" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V21" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -3226,8 +3819,36 @@
         <f t="shared" si="4"/>
         <v>1.1226851856918074E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22" s="2">
+        <v>4.0509259270038456E-4</v>
+      </c>
+      <c r="O22" s="2">
+        <v>3.4722222335403785E-4</v>
+      </c>
+      <c r="P22" s="2">
+        <v>3.7037036963738501E-4</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1.1226851856918074E-3</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -3265,8 +3886,36 @@
         <f t="shared" si="4"/>
         <v>9.2592592409346253E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23" s="2">
+        <v>4.6296299842651933E-5</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1.1574069503694773E-5</v>
+      </c>
+      <c r="P23" s="2">
+        <v>3.4722223062999547E-5</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -3304,8 +3953,36 @@
         <f t="shared" si="4"/>
         <v>3.2638888878864236E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24" s="2">
+        <v>3.9351852319668978E-4</v>
+      </c>
+      <c r="O24" s="2">
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="P24" s="2">
+        <v>2.7777777722803876E-3</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>3.2638888878864236E-3</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -3343,8 +4020,36 @@
         <f t="shared" si="4"/>
         <v>0.1810300925935735</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25" s="2">
+        <v>9.7256944442051463E-2</v>
+      </c>
+      <c r="O25" s="13">
+        <v>1.5706018522905651E-2</v>
+      </c>
+      <c r="P25" s="2">
+        <v>6.8067129628616385E-2</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.1810300925935735</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -3382,8 +4087,36 @@
         <f t="shared" si="4"/>
         <v>1.2037037013215013E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26" s="2">
+        <v>4.5138888526707888E-4</v>
+      </c>
+      <c r="O26" s="2">
+        <v>3.2407407707069069E-4</v>
+      </c>
+      <c r="P26" s="2">
+        <v>4.2824073898373172E-4</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>1.2037037013215013E-3</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -3425,8 +4158,36 @@
         <f>K23+K27</f>
         <v>9.2592593136942014E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27" s="2">
+        <v>3.9351852319668978E-4</v>
+      </c>
+      <c r="O27" s="2">
+        <v>9.2592592409346253E-5</v>
+      </c>
+      <c r="P27" s="2">
+        <v>3.4722222335403785E-4</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>8.3333333896007389E-4</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -3457,15 +4218,43 @@
         <v>6.6122685180744156E-2</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" ref="J28:J29" si="5">G28-F28</f>
+        <f t="shared" ref="J28:J29" si="9">G28-F28</f>
         <v>0.24398148147884058</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" ref="K28:K29" si="6">SUM(H28:J28)</f>
+        <f t="shared" ref="K28:K29" si="10">SUM(H28:J28)</f>
         <v>0.6664467592490837</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28" s="2">
+        <v>0.35634259258949896</v>
+      </c>
+      <c r="O28" s="2">
+        <v>6.6122685180744156E-2</v>
+      </c>
+      <c r="P28" s="2">
+        <v>0.24398148147884058</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>0.6664467592490837</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U28" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -3496,43 +4285,99 @@
         <v>5.1631944443215616E-2</v>
       </c>
       <c r="J29" s="2">
+        <f t="shared" si="9"/>
+        <v>0.17331018518598285</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="10"/>
+        <v>0.49151620370685123</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0.26657407407765277</v>
+      </c>
+      <c r="O29" s="2">
+        <v>5.1631944443215616E-2</v>
+      </c>
+      <c r="P29" s="2">
+        <v>0.17331018518598285</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>0.49151620370685123</v>
+      </c>
+      <c r="S29" s="2">
         <f t="shared" si="5"/>
-        <v>0.17331018518598285</v>
-      </c>
-      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+      <c r="T29" s="2">
         <f t="shared" si="6"/>
-        <v>0.49151620370685123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="U29" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G30" s="1"/>
       <c r="H30" s="8">
         <f>SUM(H3:H29)</f>
+        <v>2.0386689814986312</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" ref="I30:K30" si="11">SUM(I3:I29)</f>
+        <v>0.42770833332906477</v>
+      </c>
+      <c r="J30" s="8">
+        <f t="shared" si="11"/>
+        <v>1.4664004629521514</v>
+      </c>
+      <c r="K30" s="8">
+        <f t="shared" si="11"/>
+        <v>3.9327777777798474</v>
+      </c>
+      <c r="N30" s="8">
         <v>1.8255902777818847</v>
       </c>
-      <c r="I30" s="8">
-        <f t="shared" ref="I30:K30" si="7">SUM(I3:I29)</f>
+      <c r="O30" s="8">
         <v>0.31582175925723277</v>
       </c>
-      <c r="J30" s="8">
+      <c r="P30" s="8">
+        <v>1.3171874999970896</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>3.458599537036207</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="5"/>
+        <v>0.21307870371674653</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="6"/>
+        <v>0.111886574071832</v>
+      </c>
+      <c r="U30" s="2">
         <f t="shared" si="7"/>
-        <v>1.3171874999970896</v>
-      </c>
-      <c r="K30" s="8">
-        <f t="shared" si="7"/>
-        <v>3.458599537036207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.14921296295506181</v>
+      </c>
+      <c r="V30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.47417824074364034</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="8">
         <f>L12+L18+M19+L27</f>
-        <v>2.127789351856336</v>
+        <v>2.6019675925999763</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -3542,7 +4387,7 @@
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="10">
         <f>Pentaho_CHPC!M47/Performance_CHPC!B33</f>
-        <v>3.2402479696969158</v>
+        <v>2.6497505760269369</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -3560,12 +4405,32 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
   </mergeCells>
+  <conditionalFormatting sqref="S3:S30">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>N3&lt;H3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T30">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>O3&lt;I3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:U30">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>P3&lt;J3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V30">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>SUM(N3-H3,O3-I3,P3-J3)&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3589,18 +4454,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="14"/>
+      <c r="G1" s="16"/>
       <c r="H1" t="s">
         <v>6</v>
       </c>
@@ -4585,8 +5450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373E5D0C-070B-4F8C-A080-FA6C8B658209}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
@@ -4605,18 +5470,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="14"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
@@ -4768,7 +5633,7 @@
         <v>4.6296299842651933E-5</v>
       </c>
       <c r="I5" s="8">
-        <f t="shared" ref="I5:J17" si="3">E5-D5</f>
+        <f t="shared" ref="I5:I17" si="3">E5-D5</f>
         <v>7.638888928340748E-4</v>
       </c>
       <c r="J5" s="8"/>
@@ -5106,7 +5971,7 @@
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8">
-        <f t="shared" ref="K3:K14" si="4">SUM(H14:J14)</f>
+        <f t="shared" ref="K14" si="4">SUM(H14:J14)</f>
         <v>2.0601851865649223E-3</v>
       </c>
       <c r="L14" s="8">
@@ -5438,7 +6303,7 @@
         <v>1.0490972222251003</v>
       </c>
       <c r="K22" s="8">
-        <f t="shared" ref="K18:K47" si="8">SUM(H22:J22)</f>
+        <f t="shared" ref="K22:K47" si="8">SUM(H22:J22)</f>
         <v>2.6697916666744277</v>
       </c>
       <c r="N22" s="10">

</xml_diff>